<commit_message>
Fendt 1050 Vario with correct motor and transmission data
</commit_message>
<xml_diff>
--- a/Documents/MotorNeu.xlsx
+++ b/Documents/MotorNeu.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ls13_mods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d027464\Documents\GitHub\GearboxAddon\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="0" windowWidth="20400" windowHeight="9945"/>
+    <workbookView xWindow="7800" yWindow="0" windowWidth="20400" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate from Values" sheetId="3" r:id="rId1"/>
@@ -219,6 +219,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -244,9 +247,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -477,55 +477,55 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>746.80555555555554</c:v>
+                  <c:v>1333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>849</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>935.47222222222217</c:v>
+                  <c:v>2133.333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1006.2222222222222</c:v>
+                  <c:v>2333.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1061.25</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1100.5555555555554</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1124.1388888888889</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1132</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1125.6188725490197</c:v>
+                  <c:v>2287.6429738562092</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1106.4754901960785</c:v>
+                  <c:v>2175.2859477124184</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1074.5698529411764</c:v>
+                  <c:v>2062.9289215686276</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1029.9019607843136</c:v>
+                  <c:v>1950.5718954248364</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>971.47279964617405</c:v>
+                  <c:v>1791.3415366146457</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>910.86134453781506</c:v>
+                  <c:v>1313.6504601840736</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>848.37935174069639</c:v>
+                  <c:v>517.49866613311974</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>765.48606361149109</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>357.22682968536247</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -608,8 +608,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="368446496"/>
-        <c:axId val="368443752"/>
+        <c:axId val="335014272"/>
+        <c:axId val="335021328"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -791,55 +791,55 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.445956951716113</c:v>
+                  <c:v>132.9144851657941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.723769633507871</c:v>
+                  <c:v>205.06806282722513</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119.89717277486912</c:v>
+                  <c:v>273.42408376963351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>143.29447353112278</c:v>
+                  <c:v>332.28621291448519</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166.24397905759164</c:v>
+                  <c:v>375.95811518324609</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>188.0739965095986</c:v>
+                  <c:v>410.13612565445027</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>208.11283304246652</c:v>
+                  <c:v>444.3141361256545</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>225.68879581151836</c:v>
+                  <c:v>478.49214659685873</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>240.4463350785341</c:v>
+                  <c:v>488.66928446771385</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>252.1142059336824</c:v>
+                  <c:v>495.6463059918558</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>260.14717277486915</c:v>
+                  <c:v>499.42321116928446</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>263.99999999999994</c:v>
+                  <c:v>499.99999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>262.85714285714283</c:v>
+                  <c:v>484.69387755102036</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>259.42857142857144</c:v>
+                  <c:v>374.14965986394554</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>253.71428571428572</c:v>
+                  <c:v>154.76190476190476</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>239.82558139534885</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>117.00581395348837</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -922,11 +922,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="368444928"/>
-        <c:axId val="368442184"/>
+        <c:axId val="335014664"/>
+        <c:axId val="335013880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="368446496"/>
+        <c:axId val="335014272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368443752"/>
+        <c:crossAx val="335021328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +991,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="368443752"/>
+        <c:axId val="335021328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,12 +1048,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368446496"/>
+        <c:crossAx val="335014272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368442184"/>
+        <c:axId val="335013880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,12 +1096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368444928"/>
+        <c:crossAx val="335014664"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="368444928"/>
+        <c:axId val="335014664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="368442184"/>
+        <c:crossAx val="335013880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,58 +1395,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>220</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>220</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>220</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>217.55555555555554</c:v>
+                  <c:v>200.04938271604939</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>215.55555555555554</c:v>
+                  <c:v>197.08641975308643</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>214</c:v>
+                  <c:v>195.11111111111111</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>212.88888888888889</c:v>
+                  <c:v>194.12345679012347</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>212.22222222222223</c:v>
+                  <c:v>194.17355371900825</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>212</c:v>
+                  <c:v>195.56198347107437</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>212.2488888888889</c:v>
+                  <c:v>198.3388429752066</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>212.99555555555557</c:v>
+                  <c:v>202.50413223140495</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>214.24</c:v>
+                  <c:v>208.05785123966942</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>215.98222222222222</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>218.22222222222223</c:v>
+                  <c:v>232.55102040816325</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>220.96</c:v>
+                  <c:v>285.20408163265307</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>224.19555555555556</c:v>
+                  <c:v>372.9591836734694</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>229.53125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>321.34375</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1528,11 +1528,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="368441792"/>
-        <c:axId val="368444144"/>
+        <c:axId val="335015840"/>
+        <c:axId val="335019368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="368441792"/>
+        <c:axId val="335015840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368444144"/>
+        <c:crossAx val="335019368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="368444144"/>
+        <c:axId val="335019368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -1636,7 +1636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368441792"/>
+        <c:crossAx val="335015840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1909,11 +1909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368442968"/>
-        <c:axId val="368445320"/>
+        <c:axId val="335018584"/>
+        <c:axId val="335015448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368442968"/>
+        <c:axId val="335018584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2700"/>
@@ -1972,12 +1972,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368445320"/>
+        <c:crossAx val="335015448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368445320"/>
+        <c:axId val="335015448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368442968"/>
+        <c:crossAx val="335018584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2295,11 +2295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368447280"/>
-        <c:axId val="368444536"/>
+        <c:axId val="297582488"/>
+        <c:axId val="335510816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368447280"/>
+        <c:axId val="297582488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2400"/>
@@ -2358,12 +2358,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368444536"/>
+        <c:crossAx val="335510816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368444536"/>
+        <c:axId val="335510816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368447280"/>
+        <c:crossAx val="297582488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4853,13 +4853,13 @@
     <tableColumn id="4" name="motor" dataDxfId="10">
       <calculatedColumnFormula>Table15[[#This Row],[pto]]/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="9">
-      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</calculatedColumnFormula>
+    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="8">
+    <tableColumn id="5" name="xml" dataDxfId="9">
       <calculatedColumnFormula>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="7">
+    <tableColumn id="8" name="xml2" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4935,17 +4935,17 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$A$22*Table1[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="6">
+    <tableColumn id="6" name="kw_pto" dataDxfId="7">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="5">
+    <tableColumn id="3" name="ps" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor"/>
-    <tableColumn id="5" name="xml" dataDxfId="4">
+    <tableColumn id="5" name="xml" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table1[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table1[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="3">
+    <tableColumn id="8" name="xml2" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table1[[#This Row],[rpm]]/Table3[ratedRpm],3),""" torque=""",ROUND(Table1[[#This Row],[motor]]/MAX(Table1[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4979,16 +4979,16 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$I$2*Table13[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="2">
+    <tableColumn id="6" name="kw_pto" dataDxfId="3">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="1">
+    <tableColumn id="3" name="ps" dataDxfId="2">
       <calculatedColumnFormula>Table13[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor">
       <calculatedColumnFormula>C2/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="0">
+    <tableColumn id="5" name="xml" dataDxfId="1">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table13[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table13[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5262,7 +5262,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I25"/>
+      <selection activeCell="I7" sqref="I7:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5339,22 +5339,22 @@
         <v>1800</v>
       </c>
       <c r="B2">
-        <v>264</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>2150</v>
+        <v>1800</v>
       </c>
       <c r="D2">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="E2">
-        <v>1400</v>
+        <v>1100</v>
       </c>
       <c r="F2">
         <v>1400</v>
       </c>
       <c r="G2">
-        <v>1132</v>
+        <v>2400</v>
       </c>
       <c r="H2">
         <v>800</v>
@@ -5363,10 +5363,10 @@
         <v>0.75</v>
       </c>
       <c r="J2">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0.94</v>
@@ -5376,19 +5376,19 @@
       </c>
       <c r="N2" t="str">
         <f>CONCATENATE("&lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS]," | ",Table36[ratedRpm],": ",Table36[PS]," | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT]," | ",Table36[idleRatio]," | ",Table36[linearDown]," --&gt;")</f>
-        <v>&lt;!-- 1800: 264 | 2150: 250 | 1400..1400: 1132 | 0.75 | 0 --&gt;</v>
+        <v>&lt;!-- 1800: 500 | 1800: 500 | 1100..1400: 2400 | 0.75 | 1 --&gt;</v>
       </c>
       <c r="O2">
-        <v>1400</v>
+        <v>1250</v>
       </c>
       <c r="P2">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="Q2">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="R2">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5417,31 +5417,31 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</f>
-        <v>6.9444444444444448E-7</v>
+        <v>2.7777777777777779E-6</v>
       </c>
       <c r="B4">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>2.2548153537033219E-4</v>
+        <v>4.6815427559912878E-4</v>
       </c>
       <c r="C4">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>5.6370383842583041E-7</v>
+        <v>1.170385688997822E-6</v>
       </c>
       <c r="D4">
         <f>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>1.1428571428571428E-4</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</f>
-        <v>1029.9019607843136</v>
+        <v>1950.5718954248364</v>
       </c>
       <c r="F4">
         <f>Table36[PS]/1.36*9550/Table36[ratedRpm]</f>
-        <v>816.51846785225712</v>
+        <v>1950.5718954248364</v>
       </c>
       <c r="G4" s="3">
         <f>Table36[idleRatio]*Table36[maxT]/Table7[Nm2]</f>
-        <v>1.0397805235602096</v>
+        <v>0.92280628272251319</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -5501,12 +5501,12 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>220</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>204</v>
       </c>
       <c r="I7" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="0" motorTorque="0" fuelUsageRatio="220"/&gt;&lt;!-- 1800: 264 | 2150: 250 | 1400..1400: 1132 | 0.75 | 0 --&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="0" motorTorque="0" fuelUsageRatio="204"/&gt;&lt;!-- 1800: 500 | 1800: 500 | 1100..1400: 2400 | 0.75 | 1 --&gt;</v>
       </c>
       <c r="J7" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
@@ -5519,35 +5519,35 @@
       </c>
       <c r="B8">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>746.80555555555554</v>
+        <v>1333.3333333333335</v>
       </c>
       <c r="D8">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>701.99722222222215</v>
+        <v>1253.3333333333335</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>51.455293775450841</v>
+        <v>91.86736474694591</v>
       </c>
       <c r="F8" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>74.445956951716113</v>
+        <v>132.9144851657941</v>
       </c>
       <c r="G8">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>746.80555555555554</v>
+        <v>1333.3333333333335</v>
       </c>
       <c r="H8">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>220</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>204</v>
       </c>
       <c r="I8" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="747" fuelUsageRatio="220"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="1333" fuelUsageRatio="204"/&gt;</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.292" torque="0.66"/&gt;</v>
+        <v>&lt;torque normRpm="0.292" torque="0.556"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -5556,31 +5556,31 @@
       </c>
       <c r="B9">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>849</v>
+        <v>1800</v>
       </c>
       <c r="D9">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>798.06</v>
+        <v>1692</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>66.853193717277492</v>
+        <v>141.73821989528795</v>
       </c>
       <c r="F9" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>96.723769633507871</v>
+        <v>205.06806282722513</v>
       </c>
       <c r="G9">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>849</v>
+        <v>1800</v>
       </c>
       <c r="H9">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>220</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>204</v>
       </c>
       <c r="I9" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="849" fuelUsageRatio="220"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="1800" fuelUsageRatio="204"/&gt;</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
@@ -5593,35 +5593,35 @@
       </c>
       <c r="B10">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>935.47222222222217</v>
+        <v>2133.333333333333</v>
       </c>
       <c r="D10">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>879.34388888888884</v>
+        <v>2005.333333333333</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>82.870104712041879</v>
+        <v>188.98429319371726</v>
       </c>
       <c r="F10" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>119.89717277486912</v>
+        <v>273.42408376963351</v>
       </c>
       <c r="G10">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>935.47222222222217</v>
+        <v>2133.333333333333</v>
       </c>
       <c r="H10">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>217.55555555555554</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>200.04938271604939</v>
       </c>
       <c r="I10" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="935" fuelUsageRatio="218"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="2133" fuelUsageRatio="200"/&gt;</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.375" torque="0.826"/&gt;</v>
+        <v>&lt;torque normRpm="0.375" torque="0.889"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -5630,35 +5630,35 @@
       </c>
       <c r="B11">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1006.2222222222222</v>
+        <v>2333.3333333333335</v>
       </c>
       <c r="D11">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>945.84888888888884</v>
+        <v>2193.3333333333335</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>99.041768470040722</v>
+        <v>229.66841186736477</v>
       </c>
       <c r="F11">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>143.29447353112278</v>
+        <v>332.28621291448519</v>
       </c>
       <c r="G11">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1006.2222222222222</v>
+        <v>2333.3333333333335</v>
       </c>
       <c r="H11">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>215.55555555555554</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>197.08641975308643</v>
       </c>
       <c r="I11" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1006" fuelUsageRatio="216"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="2333" fuelUsageRatio="197"/&gt;</v>
       </c>
       <c r="J11" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.417" torque="0.889"/&gt;</v>
+        <v>&lt;torque normRpm="0.417" torque="0.972"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -5667,35 +5667,35 @@
       </c>
       <c r="B12">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1061.25</v>
+        <v>2400</v>
       </c>
       <c r="D12">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>997.57499999999993</v>
+        <v>2256</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>114.90392670157068</v>
+        <v>259.85340314136124</v>
       </c>
       <c r="F12">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>166.24397905759164</v>
+        <v>375.95811518324609</v>
       </c>
       <c r="G12">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1061.25</v>
+        <v>2400</v>
       </c>
       <c r="H12">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>214</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>195.11111111111111</v>
       </c>
       <c r="I12" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1061" fuelUsageRatio="214"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="2400" fuelUsageRatio="195"/&gt;</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.458" torque="0.938"/&gt;</v>
+        <v>&lt;torque normRpm="0.458" torque="1"/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -5704,35 +5704,35 @@
       </c>
       <c r="B13">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1100.5555555555554</v>
+        <v>2400</v>
       </c>
       <c r="D13">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1034.5222222222221</v>
+        <v>2256</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>129.99232111692842</v>
+        <v>283.47643979057591</v>
       </c>
       <c r="F13">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>188.0739965095986</v>
+        <v>410.13612565445027</v>
       </c>
       <c r="G13">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1100.5555555555554</v>
+        <v>2400</v>
       </c>
       <c r="H13">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>212.88888888888889</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>194.12345679012347</v>
       </c>
       <c r="I13" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1101" fuelUsageRatio="213"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="2400" fuelUsageRatio="194"/&gt;</v>
       </c>
       <c r="J13" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.5" torque="0.972"/&gt;</v>
+        <v>&lt;torque normRpm="0.5" torque="1"/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -5741,35 +5741,35 @@
       </c>
       <c r="B14">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1124.1388888888889</v>
+        <v>2400</v>
       </c>
       <c r="D14">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1056.6905555555554</v>
+        <v>2256</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>143.84269342641068</v>
+        <v>307.09947643979058</v>
       </c>
       <c r="F14">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>208.11283304246652</v>
+        <v>444.3141361256545</v>
       </c>
       <c r="G14">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1124.1388888888889</v>
+        <v>2400</v>
       </c>
       <c r="H14">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>212.22222222222223</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>194.17355371900825</v>
       </c>
       <c r="I14" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1124" fuelUsageRatio="212"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="2400" fuelUsageRatio="194"/&gt;</v>
       </c>
       <c r="J14" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.542" torque="0.993"/&gt;</v>
+        <v>&lt;torque normRpm="0.542" torque="1"/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -5778,31 +5778,31 @@
       </c>
       <c r="B15">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1132</v>
+        <v>2400</v>
       </c>
       <c r="D15">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1064.08</v>
+        <v>2256</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>155.99078534031415</v>
+        <v>330.72251308900525</v>
       </c>
       <c r="F15">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>225.68879581151836</v>
+        <v>478.49214659685873</v>
       </c>
       <c r="G15">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1132</v>
+        <v>2400</v>
       </c>
       <c r="H15">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>212</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>195.56198347107437</v>
       </c>
       <c r="I15" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1132" fuelUsageRatio="212"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="2400" fuelUsageRatio="196"/&gt;</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
@@ -5815,35 +5815,35 @@
       </c>
       <c r="B16">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1125.6188725490197</v>
+        <v>2287.6429738562092</v>
       </c>
       <c r="D16">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1058.0817401960785</v>
+        <v>2150.3843954248364</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>166.19084924545737</v>
+        <v>337.75671132327273</v>
       </c>
       <c r="F16">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>240.4463350785341</v>
+        <v>488.66928446771385</v>
       </c>
       <c r="G16">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1125.6188725490197</v>
+        <v>2287.6429738562092</v>
       </c>
       <c r="H16">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>212.2488888888889</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>198.3388429752066</v>
       </c>
       <c r="I16" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1126" fuelUsageRatio="212"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="2288" fuelUsageRatio="198"/&gt;</v>
       </c>
       <c r="J16" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.625" torque="0.994"/&gt;</v>
+        <v>&lt;torque normRpm="0.625" torque="0.953"/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5852,35 +5852,35 @@
       </c>
       <c r="B17">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1106.4754901960785</v>
+        <v>2175.2859477124184</v>
       </c>
       <c r="D17">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1040.0869607843138</v>
+        <v>2044.7687908496732</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>174.2554070423981</v>
+        <v>342.57906443554731</v>
       </c>
       <c r="F17">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>252.1142059336824</v>
+        <v>495.6463059918558</v>
       </c>
       <c r="G17">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1106.4754901960785</v>
+        <v>2175.2859477124184</v>
       </c>
       <c r="H17">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>212.99555555555557</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>202.50413223140495</v>
       </c>
       <c r="I17" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1106" fuelUsageRatio="213"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="2175" fuelUsageRatio="203"/&gt;</v>
       </c>
       <c r="J17" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.667" torque="0.977"/&gt;</v>
+        <v>&lt;torque normRpm="0.667" torque="0.906"/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5889,35 +5889,35 @@
       </c>
       <c r="B18">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1074.5698529411764</v>
+        <v>2062.9289215686276</v>
       </c>
       <c r="D18">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1010.0956617647057</v>
+        <v>1939.1531862745098</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>179.80760471204187</v>
+        <v>345.18957242582894</v>
       </c>
       <c r="F18">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>260.14717277486915</v>
+        <v>499.42321116928446</v>
       </c>
       <c r="G18">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1074.5698529411764</v>
+        <v>2062.9289215686276</v>
       </c>
       <c r="H18">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>214.24</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>208.05785123966942</v>
       </c>
       <c r="I18" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1075" fuelUsageRatio="214"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="2063" fuelUsageRatio="208"/&gt;</v>
       </c>
       <c r="J18" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.708" torque="0.949"/&gt;</v>
+        <v>&lt;torque normRpm="0.708" torque="0.86"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -5926,35 +5926,35 @@
       </c>
       <c r="B19">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1029.9019607843136</v>
+        <v>1950.5718954248364</v>
       </c>
       <c r="D19">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>968.10784313725469</v>
+        <v>1833.537581699346</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>182.47058823529406</v>
+        <v>345.58823529411757</v>
       </c>
       <c r="F19">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>263.99999999999994</v>
+        <v>499.99999999999994</v>
       </c>
       <c r="G19">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1029.9019607843136</v>
+        <v>1950.5718954248364</v>
       </c>
       <c r="H19">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>215.98222222222222</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>215</v>
       </c>
       <c r="I19" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="1030" fuelUsageRatio="216"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="1951" fuelUsageRatio="215"/&gt;</v>
       </c>
       <c r="J19" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.75" torque="0.91"/&gt;</v>
+        <v>&lt;torque normRpm="0.75" torque="0.813"/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5963,35 +5963,35 @@
       </c>
       <c r="B20">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>971.47279964617405</v>
+        <v>1791.3415366146457</v>
       </c>
       <c r="D20">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>913.1844316674036</v>
+        <v>1683.8610444177668</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>181.68067226890753</v>
+        <v>335.0090036014405</v>
       </c>
       <c r="F20">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>262.85714285714283</v>
+        <v>484.69387755102036</v>
       </c>
       <c r="G20">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>971.47279964617405</v>
+        <v>1791.3415366146457</v>
       </c>
       <c r="H20">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>218.22222222222223</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>232.55102040816325</v>
       </c>
       <c r="I20" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="971" fuelUsageRatio="218"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="1791" fuelUsageRatio="233"/&gt;</v>
       </c>
       <c r="J20" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.792" torque="0.858"/&gt;</v>
+        <v>&lt;torque normRpm="0.792" torque="0.746"/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -6000,35 +6000,35 @@
       </c>
       <c r="B21">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>910.86134453781506</v>
+        <v>1313.6504601840736</v>
       </c>
       <c r="D21">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>856.20966386554608</v>
+        <v>1234.8314325730291</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>179.31092436974788</v>
+        <v>258.60344137655056</v>
       </c>
       <c r="F21">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>259.42857142857144</v>
+        <v>374.14965986394554</v>
       </c>
       <c r="G21">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>910.86134453781506</v>
+        <v>1313.6504601840736</v>
       </c>
       <c r="H21">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>220.96</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>285.20408163265307</v>
       </c>
       <c r="I21" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="911" fuelUsageRatio="221"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="1314" fuelUsageRatio="285"/&gt;</v>
       </c>
       <c r="J21" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.833" torque="0.805"/&gt;</v>
+        <v>&lt;torque normRpm="0.833" torque="0.547"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6037,35 +6037,35 @@
       </c>
       <c r="B22">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>848.37935174069628</v>
+        <v>517.49866613311974</v>
       </c>
       <c r="D22">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>797.47659063625451</v>
+        <v>486.44874616513255</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>175.36134453781511</v>
+        <v>106.9677871148459</v>
       </c>
       <c r="F22">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>253.71428571428572</v>
+        <v>154.76190476190476</v>
       </c>
       <c r="G22">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>848.37935174069639</v>
+        <v>517.49866613311974</v>
       </c>
       <c r="H22">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>224.19555555555556</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>372.9591836734694</v>
       </c>
       <c r="I22" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="848" fuelUsageRatio="224"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="517" fuelUsageRatio="373"/&gt;</v>
       </c>
       <c r="J22" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.875" torque="0.749"/&gt;</v>
+        <v>&lt;torque normRpm="0.875" torque="0.216"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6074,35 +6074,35 @@
       </c>
       <c r="B23">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>765.48606361149109</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>719.55689979480155</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>165.76179890560874</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>239.82558139534885</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>765.48606361149109</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>229.53125</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>0</v>
       </c>
       <c r="I23" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="765" fuelUsageRatio="230"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
       </c>
       <c r="J23" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.917" torque="0.676"/&gt;</v>
+        <v>&lt;torque normRpm="0.917" torque="0"/&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6111,35 +6111,35 @@
       </c>
       <c r="B24">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>357.22682968536247</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>335.79321990424069</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>80.87166552667577</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>117.00581395348837</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>357.22682968536247</v>
+        <v>0</v>
       </c>
       <c r="H24">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
-        <v>321.34375</v>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
+        <v>0</v>
       </c>
       <c r="I24" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="357" fuelUsageRatio="321"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
       </c>
       <c r="J24" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.958" torque="0.316"/&gt;</v>
+        <v>&lt;torque normRpm="0.958" torque="0"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -6167,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I25" s="5" t="str">
@@ -6204,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I26" s="5" t="str">
@@ -6242,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I27" s="5" t="str">
@@ -6280,7 +6280,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I28" s="5" t="str">
@@ -6318,7 +6318,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I29" s="5" t="str">
@@ -6356,7 +6356,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I30" s="5" t="str">
@@ -6394,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I31" s="5" t="str">
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I32" s="5" t="str">
@@ -6470,7 +6470,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I33" s="5" t="str">
@@ -6508,7 +6508,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I34" s="5" t="str">
@@ -6546,7 +6546,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I35" s="5" t="str">
@@ -6584,7 +6584,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I36" s="5" t="str">
@@ -6622,7 +6622,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I37" s="5" t="str">
@@ -6660,7 +6660,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I38" s="5" t="str">
@@ -6698,7 +6698,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I39" s="5" t="str">
@@ -6736,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I40" s="5" t="str">
@@ -6774,7 +6774,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I41" s="5" t="str">
@@ -6812,7 +6812,7 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I42" s="5" t="str">
@@ -6850,7 +6850,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I43" s="5" t="str">
@@ -6888,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I44" s="5" t="str">
@@ -6926,7 +6926,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I45" s="5" t="str">
@@ -6964,7 +6964,7 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^3,0))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
         <v>0</v>
       </c>
       <c r="I46" s="5" t="str">

</xml_diff>

<commit_message>
Optimal speed with PTO / combine
</commit_message>
<xml_diff>
--- a/Documents/MotorNeu.xlsx
+++ b/Documents/MotorNeu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="0" windowWidth="20400" windowHeight="9945"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="20400" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate from Values" sheetId="3" r:id="rId1"/>
@@ -219,9 +219,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -247,6 +244,9 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -477,58 +477,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1333.3333333333335</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1800</c:v>
+                  <c:v>262.39999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2133.333333333333</c:v>
+                  <c:v>506.34999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2333.3333333333335</c:v>
+                  <c:v>680.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2400</c:v>
+                  <c:v>785.15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2400</c:v>
+                  <c:v>820</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2400</c:v>
+                  <c:v>807.6846209409581</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2400</c:v>
+                  <c:v>793.57791401878262</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2287.6429738562092</c:v>
+                  <c:v>777.67987923347403</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2175.2859477124184</c:v>
+                  <c:v>759.99051658503197</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2062.9289215686276</c:v>
+                  <c:v>740.50982607345645</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1950.5718954248364</c:v>
+                  <c:v>719.23780769874759</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1791.3415366146457</c:v>
+                  <c:v>696.17446146090538</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1313.6504601840736</c:v>
+                  <c:v>671.31978735992982</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>517.49866613311974</c:v>
+                  <c:v>641.74659762895044</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>606.45053475935822</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>539.06714200831834</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>336.91696375519905</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -608,8 +608,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="335014272"/>
-        <c:axId val="335021328"/>
+        <c:axId val="289520224"/>
+        <c:axId val="289522184"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -791,58 +791,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>132.9144851657941</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>205.06806282722513</c:v>
+                  <c:v>29.894366492146588</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>273.42408376963351</c:v>
+                  <c:v>64.897633507853399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>332.28621291448519</c:v>
+                  <c:v>96.923141361256569</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375.95811518324609</c:v>
+                  <c:v>122.99313089005237</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>410.13612565445027</c:v>
+                  <c:v>140.12984293193719</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>444.3141361256545</c:v>
+                  <c:v>149.52737275639936</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>478.49214659685873</c:v>
+                  <c:v>158.21699982112693</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>488.66928446771385</c:v>
+                  <c:v>166.12219409804052</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>495.6463059918558</c:v>
+                  <c:v>173.16642555906068</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>499.42321116928446</c:v>
+                  <c:v>179.273164176108</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>499.99999999999994</c:v>
+                  <c:v>184.36587992110307</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>484.69387755102036</c:v>
+                  <c:v>188.36804276596644</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>374.14965986394554</c:v>
+                  <c:v>191.20312268261878</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>154.76190476190476</c:v>
+                  <c:v>191.91919191919192</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>176.56565656565652</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>115.15151515151516</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -922,11 +922,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="335014664"/>
-        <c:axId val="335013880"/>
+        <c:axId val="289522576"/>
+        <c:axId val="289519048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335014272"/>
+        <c:axId val="289520224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335021328"/>
+        <c:crossAx val="289522184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +991,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335021328"/>
+        <c:axId val="289522184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,12 +1048,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335014272"/>
+        <c:crossAx val="289520224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335013880"/>
+        <c:axId val="289519048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,12 +1096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335014664"/>
+        <c:crossAx val="289522576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="335014664"/>
+        <c:axId val="289522576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1111,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="335013880"/>
+        <c:crossAx val="289519048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1395,64 +1395,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>204</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>204</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>204</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200.04938271604939</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>197.08641975308643</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>195.11111111111111</c:v>
+                  <c:v>243.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>194.12345679012347</c:v>
+                  <c:v>231.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>194.17355371900825</c:v>
+                  <c:v>222.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>195.56198347107437</c:v>
+                  <c:v>216.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>198.3388429752066</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>202.50413223140495</c:v>
+                  <c:v>215.32653061224491</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>208.05785123966942</c:v>
+                  <c:v>216.30612244897958</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>215</c:v>
+                  <c:v>217.9387755102041</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>232.55102040816325</c:v>
+                  <c:v>220.22448979591837</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>285.20408163265307</c:v>
+                  <c:v>223.16326530612244</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>372.9591836734694</c:v>
+                  <c:v>226.75510204081633</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>256.66666666666669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>333.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>462</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1528,11 +1528,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="335015840"/>
-        <c:axId val="335019368"/>
+        <c:axId val="289519440"/>
+        <c:axId val="289524536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="335015840"/>
+        <c:axId val="289519440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335019368"/>
+        <c:crossAx val="289524536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1583,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="335019368"/>
+        <c:axId val="289524536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -1636,7 +1636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335015840"/>
+        <c:crossAx val="289519440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1909,11 +1909,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="335018584"/>
-        <c:axId val="335015448"/>
+        <c:axId val="289519832"/>
+        <c:axId val="289523360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="335018584"/>
+        <c:axId val="289519832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2700"/>
@@ -1972,12 +1972,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335015448"/>
+        <c:crossAx val="289523360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335015448"/>
+        <c:axId val="289523360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,7 +2034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335018584"/>
+        <c:crossAx val="289519832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2295,11 +2295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297582488"/>
-        <c:axId val="335510816"/>
+        <c:axId val="357515944"/>
+        <c:axId val="357521432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297582488"/>
+        <c:axId val="357515944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2400"/>
@@ -2358,12 +2358,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="335510816"/>
+        <c:crossAx val="357521432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="335510816"/>
+        <c:axId val="357521432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297582488"/>
+        <c:crossAx val="357515944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4853,13 +4853,13 @@
     <tableColumn id="4" name="motor" dataDxfId="10">
       <calculatedColumnFormula>Table15[[#This Row],[pto]]/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="0">
+    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="9">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="9">
+    <tableColumn id="5" name="xml" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="8">
+    <tableColumn id="8" name="xml2" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4872,7 +4872,9 @@
   <autoFilter ref="A1:R2"/>
   <tableColumns count="18">
     <tableColumn id="10" name="maxPRpm"/>
-    <tableColumn id="14" name="maxPS"/>
+    <tableColumn id="14" name="maxPS">
+      <calculatedColumnFormula>190*133.5/132</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" name="ratedRpm"/>
     <tableColumn id="3" name="PS"/>
     <tableColumn id="12" name="maxTRpm1"/>
@@ -4935,17 +4937,17 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$A$22*Table1[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="7">
+    <tableColumn id="6" name="kw_pto" dataDxfId="6">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="6">
+    <tableColumn id="3" name="ps" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor"/>
-    <tableColumn id="5" name="xml" dataDxfId="5">
+    <tableColumn id="5" name="xml" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table1[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table1[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="4">
+    <tableColumn id="8" name="xml2" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table1[[#This Row],[rpm]]/Table3[ratedRpm],3),""" torque=""",ROUND(Table1[[#This Row],[motor]]/MAX(Table1[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4979,16 +4981,16 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$I$2*Table13[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="3">
+    <tableColumn id="6" name="kw_pto" dataDxfId="2">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="2">
+    <tableColumn id="3" name="ps" dataDxfId="1">
       <calculatedColumnFormula>Table13[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor">
       <calculatedColumnFormula>C2/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="1">
+    <tableColumn id="5" name="xml" dataDxfId="0">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table13[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table13[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5262,7 +5264,7 @@
   <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I23"/>
+      <selection activeCell="I7" sqref="I7:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5336,37 +5338,38 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1800</v>
+        <v>2050</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <f>190*133.5/132</f>
+        <v>192.15909090909091</v>
       </c>
       <c r="C2">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="D2">
-        <v>500</v>
+        <v>190</v>
       </c>
       <c r="E2">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="F2">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="G2">
-        <v>2400</v>
+        <v>820</v>
       </c>
       <c r="H2">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="I2" s="3">
-        <v>0.75</v>
+        <v>0.83</v>
       </c>
       <c r="J2">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="L2">
         <v>0.94</v>
@@ -5376,19 +5379,19 @@
       </c>
       <c r="N2" t="str">
         <f>CONCATENATE("&lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS]," | ",Table36[ratedRpm],": ",Table36[PS]," | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT]," | ",Table36[idleRatio]," | ",Table36[linearDown]," --&gt;")</f>
-        <v>&lt;!-- 1800: 500 | 1800: 500 | 1100..1400: 2400 | 0.75 | 1 --&gt;</v>
+        <v>&lt;!-- 2050: 192.159090909091 | 2200: 190 | 1200..1200: 820 | 0.83 | 0.6 --&gt;</v>
       </c>
       <c r="O2">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="P2">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="Q2">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="R2">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -5417,31 +5420,31 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</f>
-        <v>2.7777777777777779E-6</v>
+        <v>4.2500000000000008E-6</v>
       </c>
       <c r="B4">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>4.6815427559912878E-4</v>
+        <v>2.321080310462454E-4</v>
       </c>
       <c r="C4">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.170385688997822E-6</v>
+        <v>2.7306827181911222E-7</v>
       </c>
       <c r="D4">
         <f>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>0</v>
+        <v>9.5959595959595848E-5</v>
       </c>
       <c r="E4">
         <f>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</f>
-        <v>1950.5718954248364</v>
+        <v>658.22070236076695</v>
       </c>
       <c r="F4">
         <f>Table36[PS]/1.36*9550/Table36[ratedRpm]</f>
-        <v>1950.5718954248364</v>
+        <v>606.45053475935822</v>
       </c>
       <c r="G4" s="3">
         <f>Table36[idleRatio]*Table36[maxT]/Table7[Nm2]</f>
-        <v>0.92280628272251319</v>
+        <v>1.1222679526040233</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -5502,11 +5505,11 @@
       </c>
       <c r="H7">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="I7" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="0" motorTorque="0" fuelUsageRatio="204"/&gt;&lt;!-- 1800: 500 | 1800: 500 | 1100..1400: 2400 | 0.75 | 1 --&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="0" motorTorque="0" fuelUsageRatio="260"/&gt;&lt;!-- 2050: 192.159090909091 | 2200: 190 | 1200..1200: 820 | 0.83 | 0.6 --&gt;</v>
       </c>
       <c r="J7" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
@@ -5519,35 +5522,35 @@
       </c>
       <c r="B8">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1333.3333333333335</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1253.3333333333335</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>91.86736474694591</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>132.9144851657941</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1333.3333333333335</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="I8" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="1333" fuelUsageRatio="204"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="0" fuelUsageRatio="260"/&gt;</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.292" torque="0.556"/&gt;</v>
+        <v>&lt;torque normRpm="0.292" torque="0"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -5556,35 +5559,35 @@
       </c>
       <c r="B9">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1800</v>
+        <v>262.39999999999986</v>
       </c>
       <c r="D9">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1692</v>
+        <v>246.65599999999986</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>141.73821989528795</v>
+        <v>20.66228272251308</v>
       </c>
       <c r="F9" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>205.06806282722513</v>
+        <v>29.894366492146588</v>
       </c>
       <c r="G9">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1800</v>
+        <v>262.39999999999986</v>
       </c>
       <c r="H9">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="I9" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="1800" fuelUsageRatio="204"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="262" fuelUsageRatio="260"/&gt;</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.333" torque="0.75"/&gt;</v>
+        <v>&lt;torque normRpm="0.333" torque="0.32"/&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -5593,35 +5596,35 @@
       </c>
       <c r="B10">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2133.333333333333</v>
+        <v>506.34999999999997</v>
       </c>
       <c r="D10">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2005.333333333333</v>
+        <v>475.96899999999994</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>188.98429319371726</v>
+        <v>44.855717277486903</v>
       </c>
       <c r="F10" s="1">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>273.42408376963351</v>
+        <v>64.897633507853399</v>
       </c>
       <c r="G10">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2133.333333333333</v>
+        <v>506.34999999999997</v>
       </c>
       <c r="H10">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>200.04938271604939</v>
+        <v>260</v>
       </c>
       <c r="I10" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="2133" fuelUsageRatio="200"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="506" fuelUsageRatio="260"/&gt;</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.375" torque="0.889"/&gt;</v>
+        <v>&lt;torque normRpm="0.375" torque="0.618"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -5630,35 +5633,35 @@
       </c>
       <c r="B11">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2333.3333333333335</v>
+        <v>680.6</v>
       </c>
       <c r="D11">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2193.3333333333335</v>
+        <v>639.76400000000001</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>229.66841186736477</v>
+        <v>66.990994764397911</v>
       </c>
       <c r="F11">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>332.28621291448519</v>
+        <v>96.923141361256569</v>
       </c>
       <c r="G11">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2333.3333333333335</v>
+        <v>680.6</v>
       </c>
       <c r="H11">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>197.08641975308643</v>
+        <v>260</v>
       </c>
       <c r="I11" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="2333" fuelUsageRatio="197"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="681" fuelUsageRatio="260"/&gt;</v>
       </c>
       <c r="J11" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.417" torque="0.972"/&gt;</v>
+        <v>&lt;torque normRpm="0.417" torque="0.83"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -5667,35 +5670,35 @@
       </c>
       <c r="B12">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2400</v>
+        <v>785.15</v>
       </c>
       <c r="D12">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2256</v>
+        <v>738.04099999999994</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>259.85340314136124</v>
+        <v>85.009958115183238</v>
       </c>
       <c r="F12">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>375.95811518324609</v>
+        <v>122.99313089005237</v>
       </c>
       <c r="G12">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2400</v>
+        <v>785.15</v>
       </c>
       <c r="H12">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>195.11111111111111</v>
+        <v>243.8</v>
       </c>
       <c r="I12" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="2400" fuelUsageRatio="195"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="785" fuelUsageRatio="244"/&gt;</v>
       </c>
       <c r="J12" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.458" torque="1"/&gt;</v>
+        <v>&lt;torque normRpm="0.458" torque="0.958"/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -5704,31 +5707,31 @@
       </c>
       <c r="B13">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2400</v>
+        <v>820</v>
       </c>
       <c r="D13">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2256</v>
+        <v>770.8</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>283.47643979057591</v>
+        <v>96.854450261780102</v>
       </c>
       <c r="F13">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>410.13612565445027</v>
+        <v>140.12984293193719</v>
       </c>
       <c r="G13">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2400</v>
+        <v>820</v>
       </c>
       <c r="H13">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>194.12345679012347</v>
+        <v>231.2</v>
       </c>
       <c r="I13" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="2400" fuelUsageRatio="194"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="820" fuelUsageRatio="231"/&gt;</v>
       </c>
       <c r="J13" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
@@ -5741,35 +5744,35 @@
       </c>
       <c r="B14">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2400</v>
+        <v>807.6846209409581</v>
       </c>
       <c r="D14">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2256</v>
+        <v>759.22354368450056</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>307.09947643979058</v>
+        <v>103.34980175809956</v>
       </c>
       <c r="F14">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>444.3141361256545</v>
+        <v>149.52737275639936</v>
       </c>
       <c r="G14">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2400</v>
+        <v>807.6846209409581</v>
       </c>
       <c r="H14">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>194.17355371900825</v>
+        <v>222.2</v>
       </c>
       <c r="I14" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="2400" fuelUsageRatio="194"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="808" fuelUsageRatio="222"/&gt;</v>
       </c>
       <c r="J14" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.542" torque="1"/&gt;</v>
+        <v>&lt;torque normRpm="0.542" torque="0.985"/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -5778,35 +5781,35 @@
       </c>
       <c r="B15">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2400</v>
+        <v>793.57791401878262</v>
       </c>
       <c r="D15">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2256</v>
+        <v>745.96323917765562</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>330.72251308900525</v>
+        <v>109.35586752342596</v>
       </c>
       <c r="F15">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>478.49214659685873</v>
+        <v>158.21699982112693</v>
       </c>
       <c r="G15">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2400</v>
+        <v>793.57791401878262</v>
       </c>
       <c r="H15">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>195.56198347107437</v>
+        <v>216.8</v>
       </c>
       <c r="I15" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="2400" fuelUsageRatio="196"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="794" fuelUsageRatio="217"/&gt;</v>
       </c>
       <c r="J15" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.583" torque="1"/&gt;</v>
+        <v>&lt;torque normRpm="0.583" torque="0.968"/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -5815,35 +5818,35 @@
       </c>
       <c r="B16">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2287.6429738562092</v>
+        <v>777.67987923347403</v>
       </c>
       <c r="D16">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2150.3843954248364</v>
+        <v>731.0190864794655</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>337.75671132327273</v>
+        <v>114.8197518030574</v>
       </c>
       <c r="F16">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>488.66928446771385</v>
+        <v>166.12219409804052</v>
       </c>
       <c r="G16">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2287.6429738562092</v>
+        <v>777.67987923347403</v>
       </c>
       <c r="H16">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>198.3388429752066</v>
+        <v>215</v>
       </c>
       <c r="I16" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="2288" fuelUsageRatio="198"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="778" fuelUsageRatio="215"/&gt;</v>
       </c>
       <c r="J16" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.625" torque="0.953"/&gt;</v>
+        <v>&lt;torque normRpm="0.625" torque="0.948"/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5852,35 +5855,35 @@
       </c>
       <c r="B17">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2175.2859477124184</v>
+        <v>759.99051658503186</v>
       </c>
       <c r="D17">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>2044.7687908496732</v>
+        <v>714.39108558992996</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>342.57906443554731</v>
+        <v>119.68855884229194</v>
       </c>
       <c r="F17">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>495.6463059918558</v>
+        <v>173.16642555906068</v>
       </c>
       <c r="G17">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2175.2859477124184</v>
+        <v>759.99051658503197</v>
       </c>
       <c r="H17">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>202.50413223140495</v>
+        <v>215.32653061224491</v>
       </c>
       <c r="I17" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="2175" fuelUsageRatio="203"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="760" fuelUsageRatio="215"/&gt;</v>
       </c>
       <c r="J17" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.667" torque="0.906"/&gt;</v>
+        <v>&lt;torque normRpm="0.667" torque="0.927"/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5889,35 +5892,35 @@
       </c>
       <c r="B18">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>2062.9289215686276</v>
+        <v>740.50982607345645</v>
       </c>
       <c r="D18">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1939.1531862745098</v>
+        <v>696.079236509049</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>345.18957242582894</v>
+        <v>123.90939288642757</v>
       </c>
       <c r="F18">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>499.42321116928446</v>
+        <v>179.273164176108</v>
       </c>
       <c r="G18">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>2062.9289215686276</v>
+        <v>740.50982607345645</v>
       </c>
       <c r="H18">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>208.05785123966942</v>
+        <v>216.30612244897958</v>
       </c>
       <c r="I18" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="2063" fuelUsageRatio="208"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="741" fuelUsageRatio="216"/&gt;</v>
       </c>
       <c r="J18" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.708" torque="0.86"/&gt;</v>
+        <v>&lt;torque normRpm="0.708" torque="0.903"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -5926,35 +5929,35 @@
       </c>
       <c r="B19">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1950.5718954248364</v>
+        <v>719.23780769874759</v>
       </c>
       <c r="D19">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1833.537581699346</v>
+        <v>676.08353923682273</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>345.58823529411757</v>
+        <v>127.42935818076241</v>
       </c>
       <c r="F19">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>499.99999999999994</v>
+        <v>184.36587992110307</v>
       </c>
       <c r="G19">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1950.5718954248364</v>
+        <v>719.23780769874759</v>
       </c>
       <c r="H19">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>215</v>
+        <v>217.9387755102041</v>
       </c>
       <c r="I19" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="1951" fuelUsageRatio="215"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="719" fuelUsageRatio="218"/&gt;</v>
       </c>
       <c r="J19" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.75" torque="0.813"/&gt;</v>
+        <v>&lt;torque normRpm="0.75" torque="0.877"/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5963,35 +5966,35 @@
       </c>
       <c r="B20">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1791.3415366146457</v>
+        <v>696.17446146090538</v>
       </c>
       <c r="D20">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1683.8610444177668</v>
+        <v>654.40399377325105</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>335.0090036014405</v>
+        <v>130.19555897059445</v>
       </c>
       <c r="F20">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>484.69387755102036</v>
+        <v>188.36804276596644</v>
       </c>
       <c r="G20">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1791.3415366146457</v>
+        <v>696.17446146090538</v>
       </c>
       <c r="H20">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>232.55102040816325</v>
+        <v>220.22448979591837</v>
       </c>
       <c r="I20" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="1791" fuelUsageRatio="233"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="696" fuelUsageRatio="220"/&gt;</v>
       </c>
       <c r="J20" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.792" torque="0.746"/&gt;</v>
+        <v>&lt;torque normRpm="0.792" torque="0.849"/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -6000,35 +6003,35 @@
       </c>
       <c r="B21">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>1313.6504601840736</v>
+        <v>671.31978735992982</v>
       </c>
       <c r="D21">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1234.8314325730291</v>
+        <v>631.04060011833394</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>258.60344137655056</v>
+        <v>132.15509950122177</v>
       </c>
       <c r="F21">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>374.14965986394554</v>
+        <v>191.20312268261878</v>
       </c>
       <c r="G21">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>1313.6504601840736</v>
+        <v>671.31978735992982</v>
       </c>
       <c r="H21">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>285.20408163265307</v>
+        <v>223.16326530612244</v>
       </c>
       <c r="I21" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="1314" fuelUsageRatio="285"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="671" fuelUsageRatio="223"/&gt;</v>
       </c>
       <c r="J21" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.833" torque="0.547"/&gt;</v>
+        <v>&lt;torque normRpm="0.833" torque="0.819"/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6037,35 +6040,35 @@
       </c>
       <c r="B22">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>517.49866613311974</v>
+        <v>641.74659762895055</v>
       </c>
       <c r="D22">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>486.44874616513255</v>
+        <v>603.24180177121343</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>106.9677871148459</v>
+        <v>132.65002970885322</v>
       </c>
       <c r="F22">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>154.76190476190476</v>
+        <v>191.91919191919192</v>
       </c>
       <c r="G22">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>517.49866613311974</v>
+        <v>641.74659762895044</v>
       </c>
       <c r="H22">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>372.9591836734694</v>
+        <v>226.75510204081633</v>
       </c>
       <c r="I22" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="517" fuelUsageRatio="373"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="642" fuelUsageRatio="227"/&gt;</v>
       </c>
       <c r="J22" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.875" torque="0.216"/&gt;</v>
+        <v>&lt;torque normRpm="0.875" torque="0.783"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6074,35 +6077,35 @@
       </c>
       <c r="B23">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>0</v>
+        <v>606.45053475935822</v>
       </c>
       <c r="D23">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>570.06350267379673</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>131.3235294117647</v>
       </c>
       <c r="F23">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="G23">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>0</v>
+        <v>606.45053475935822</v>
       </c>
       <c r="H23">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="I23" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="606" fuelUsageRatio="231"/&gt;</v>
       </c>
       <c r="J23" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.917" torque="0"/&gt;</v>
+        <v>&lt;torque normRpm="0.917" torque="0.74"/&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6111,35 +6114,35 @@
       </c>
       <c r="B24">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>0</v>
+        <v>539.06714200831834</v>
       </c>
       <c r="D24">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>506.72311348781921</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>122.03802733214494</v>
       </c>
       <c r="F24">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>0</v>
+        <v>176.56565656565652</v>
       </c>
       <c r="G24">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>0</v>
+        <v>539.06714200831834</v>
       </c>
       <c r="H24">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>0</v>
+        <v>256.66666666666669</v>
       </c>
       <c r="I24" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="539" fuelUsageRatio="257"/&gt;</v>
       </c>
       <c r="J24" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="0.958" torque="0"/&gt;</v>
+        <v>&lt;torque normRpm="0.958" torque="0.657"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -6148,35 +6151,35 @@
       </c>
       <c r="B25">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;1,0,IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],MAX(0,Table7[Nm2]*(1-(Table15[[#This Row],[rpm]]-Table36[ratedRpm])^2/(Table36[fadeOut]^2))),(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/Table15[[#This Row],[rpm]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT],Table36[maxT])))))</f>
-        <v>0</v>
+        <v>336.91696375519905</v>
       </c>
       <c r="D25">
         <f>$L$2*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>316.70194592988707</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>79.590017825311932</v>
       </c>
       <c r="F25">
         <f>Table15[[#This Row],[kw_pto]]*1.36/0.94</f>
-        <v>0</v>
+        <v>115.15151515151516</v>
       </c>
       <c r="G25">
         <f>Table15[[#This Row],[pto]]/0.94</f>
-        <v>0</v>
+        <v>336.91696375519905</v>
       </c>
       <c r="H25">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>0</v>
+        <v>333.66666666666663</v>
       </c>
       <c r="I25" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="337" fuelUsageRatio="334"/&gt;</v>
       </c>
       <c r="J25" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>
-        <v>&lt;torque normRpm="1" torque="0"/&gt;</v>
+        <v>&lt;torque normRpm="1" torque="0.411"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -6205,11 +6208,11 @@
       </c>
       <c r="H26">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[idleRpm],Table36[fuelIdleRate],IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2,0))))</f>
-        <v>0</v>
+        <v>462</v>
       </c>
       <c r="I26" s="5" t="str">
         <f>CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],0),"""/&gt;",IF(Table15[[#This Row],[rpm]]&lt;1,Table36[xmlComment],IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),"")))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2500" motorTorque="0" fuelUsageRatio="0"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2500" motorTorque="0" fuelUsageRatio="462"/&gt;</v>
       </c>
       <c r="J26" s="4" t="str">
         <f>CONCATENATE("&lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[maxRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")</f>

</xml_diff>

<commit_message>
v1.2.99.94: Even more realistic fuel consumption
</commit_message>
<xml_diff>
--- a/Documents/MotorNeu.xlsx
+++ b/Documents/MotorNeu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="0" windowWidth="20400" windowHeight="9945"/>
+    <workbookView xWindow="23190" yWindow="0" windowWidth="20400" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate from Values" sheetId="3" r:id="rId1"/>
@@ -541,71 +541,6 @@
   <dxfs count="73">
     <dxf>
       <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -617,113 +552,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="6"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1251,6 +1079,96 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1389,6 +1307,62 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1411,6 +1385,32 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1677,61 +1677,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212.26633744855968</c:v>
+                  <c:v>240.37037037037044</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>437.0189300411522</c:v>
+                  <c:v>704.81481481481478</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>906.36374485596684</c:v>
+                  <c:v>912.59259259259272</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1042.4092181069957</c:v>
+                  <c:v>953.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1137.81</c:v>
+                  <c:v>990</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1173</c:v>
+                  <c:v>1023.6111111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1173</c:v>
+                  <c:v>1051.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1173</c:v>
+                  <c:v>1072.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1173</c:v>
+                  <c:v>1087.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1173</c:v>
+                  <c:v>1096.9444444444443</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1173</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1152.2705060971757</c:v>
+                  <c:v>1072.4929856811145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1106.5226574840462</c:v>
+                  <c:v>1032.6557093425604</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1053.3088235294117</c:v>
+                  <c:v>975.28594771241819</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>997.87151702786366</c:v>
+                  <c:v>923.95510835913308</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>948.85569852941171</c:v>
+                  <c:v>796.06627888149092</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>906.17997198879539</c:v>
+                  <c:v>478.62033819495952</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>825.35460243878128</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>534.80409581228059</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1951,61 +1951,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.65302057613169</c:v>
+                  <c:v>228.3518518518519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>415.16798353909468</c:v>
+                  <c:v>669.57407407407413</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>861.04555761316851</c:v>
+                  <c:v>866.96296296296305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>990.28875720164592</c:v>
+                  <c:v>905.66666666666674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1080.9195</c:v>
+                  <c:v>940.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>972.43055555555554</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>998.55555555555566</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>1018.875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>1033.3888888888889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>1042.0972222222222</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1114.3499999999999</c:v>
+                  <c:v>1045</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1088.0201370320856</c:v>
+                  <c:v>987.47702205882354</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1024.0189525007863</c:v>
+                  <c:v>929.39013840830444</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>967.12901069518705</c:v>
+                  <c:v>877.75735294117646</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>916.22748381649308</c:v>
+                  <c:v>831.55959752321974</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>866.89710060160417</c:v>
+                  <c:v>716.45965099334182</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>815.56197478991601</c:v>
+                  <c:v>430.75830437546352</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>742.81914219490329</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>481.32368623105259</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2068,8 +2068,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318334496"/>
-        <c:axId val="318337632"/>
+        <c:axId val="374297712"/>
+        <c:axId val="374295752"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2239,61 +2239,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0228504600004311</c:v>
+                  <c:v>3.4230754314523959</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.894062611768252</c:v>
+                  <c:v>40.148613535000962</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.351652890353989</c:v>
+                  <c:v>90.972580957921295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118.75824390580225</c:v>
+                  <c:v>108.61012216404887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145.83030785340313</c:v>
+                  <c:v>126.88586387434555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>167.04502617801046</c:v>
+                  <c:v>145.77079697498544</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>183.74952879581153</c:v>
+                  <c:v>164.65573007562537</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>200.4540314136126</c:v>
+                  <c:v>183.27958115183247</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>217.15853403141364</c:v>
+                  <c:v>201.38126817917399</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>233.86303664921471</c:v>
+                  <c:v>218.699709133217</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>250.56753926701575</c:v>
+                  <c:v>234.97382198952886</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>262.54875615366012</c:v>
+                  <c:v>244.37117663268117</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>267.88276273331041</c:v>
+                  <c:v>249.99999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>270</c:v>
+                  <c:v>249.99999999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>269.99999999999994</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>270.25</c:v>
+                  <c:v>226.7330134615346</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>270.99999999999994</c:v>
+                  <c:v>143.13504564238789</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>258.58230057558467</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>175.16934153935222</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
                   <c:v>0</c:v>
@@ -2513,61 +2513,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8717079370004095</c:v>
+                  <c:v>3.2519216598797756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.649359481179843</c:v>
+                  <c:v>38.141182858250929</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.834070245836287</c:v>
+                  <c:v>86.423951910025224</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>112.82033171051211</c:v>
+                  <c:v>103.17961605584642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>138.53879246073296</c:v>
+                  <c:v>120.54157068062827</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>158.69277486910991</c:v>
+                  <c:v>138.48225712623619</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>174.56205235602093</c:v>
+                  <c:v>156.42294357184412</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>190.43132984293194</c:v>
+                  <c:v>174.11560209424087</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>206.30060732984293</c:v>
+                  <c:v>191.31220477021526</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>222.16988481675392</c:v>
+                  <c:v>207.76472367655614</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>238.03916230366491</c:v>
+                  <c:v>223.22513089005241</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>247.90909090909093</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>247.90909090909088</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>247.90909090909088</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>247.90909090909088</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>246.90681818181815</c:v>
+                  <c:v>204.05971211538113</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>243.9</c:v>
+                  <c:v>128.8215410781491</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>232.72407051802622</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>157.65240738541704</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
                   <c:v>0</c:v>
@@ -2630,11 +2630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318331752"/>
-        <c:axId val="318332928"/>
+        <c:axId val="374298104"/>
+        <c:axId val="374300064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318334496"/>
+        <c:axId val="374297712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -2738,13 +2738,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318337632"/>
+        <c:crossAx val="374295752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318337632"/>
+        <c:axId val="374295752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,12 +2846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318334496"/>
+        <c:crossAx val="374297712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318332928"/>
+        <c:axId val="374300064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,12 +2894,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318331752"/>
+        <c:crossAx val="374298104"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318331752"/>
+        <c:axId val="374298104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2909,7 +2909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318332928"/>
+        <c:crossAx val="374300064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3197,64 +3197,64 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>311.38559556786686</c:v>
+                  <c:v>304.1749999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>295.71246537396109</c:v>
+                  <c:v>289.7999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>256.33850415512461</c:v>
+                  <c:v>253.57499999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>228.43268698060939</c:v>
+                  <c:v>227.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.67922437673127</c:v>
+                  <c:v>221.37499999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>216.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>211.99501385041552</c:v>
+                  <c:v>212.17499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>209.06426592797783</c:v>
+                  <c:v>209.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>207.40775623268698</c:v>
+                  <c:v>207.57499999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>207.01368233194526</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>207.49256395002973</c:v>
+                  <c:v>207.63888888888889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>208.65556216537775</c:v>
+                  <c:v>209.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>210.5026769779893</c:v>
+                  <c:v>212.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>213.03390838786436</c:v>
+                  <c:v>217.22222222222223</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>216.24925639500299</c:v>
+                  <c:v>222.97222222222223</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>220.14872099940513</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>224.73230220107078</c:v>
+                  <c:v>244.75450687929043</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>230</c:v>
+                  <c:v>313.46409493927865</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>244.75450687929043</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>313.46409493927865</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>460</c:v>
@@ -3317,11 +3317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318332144"/>
-        <c:axId val="318334888"/>
+        <c:axId val="374296144"/>
+        <c:axId val="374300456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318332144"/>
+        <c:axId val="374296144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -3425,13 +3425,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318334888"/>
+        <c:crossAx val="374300456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318334888"/>
+        <c:axId val="374300456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3529,7 +3529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318332144"/>
+        <c:crossAx val="374296144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -3845,11 +3845,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318336064"/>
-        <c:axId val="318335280"/>
+        <c:axId val="374300848"/>
+        <c:axId val="374296928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318336064"/>
+        <c:axId val="374300848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2700"/>
@@ -3908,12 +3908,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318335280"/>
+        <c:crossAx val="374296928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318335280"/>
+        <c:axId val="374296928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318336064"/>
+        <c:crossAx val="374300848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4231,11 +4231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="317180528"/>
-        <c:axId val="317182096"/>
+        <c:axId val="374231496"/>
+        <c:axId val="374237376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="317180528"/>
+        <c:axId val="374231496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2400"/>
@@ -4294,12 +4294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317182096"/>
+        <c:crossAx val="374237376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="317182096"/>
+        <c:axId val="374237376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317180528"/>
+        <c:crossAx val="374231496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6813,46 +6813,46 @@
     <tableColumn id="3" name="ps" dataDxfId="63">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="psEco" dataDxfId="8">
+    <tableColumn id="13" name="psEco" dataDxfId="62">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="3">
+    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="61">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="7">
-      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</calculatedColumnFormula>
+    <tableColumn id="5" name="xml" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="6">
+    <tableColumn id="8" name="xml2" dataDxfId="60">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="t1" dataDxfId="62">
+    <tableColumn id="15" name="t1" dataDxfId="59">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="t2" dataDxfId="61">
+    <tableColumn id="18" name="t2" dataDxfId="58">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="t3" dataDxfId="5">
+    <tableColumn id="19" name="t3" dataDxfId="57">
       <calculatedColumnFormula>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="t4" dataDxfId="60">
+    <tableColumn id="16" name="t4" dataDxfId="56">
       <calculatedColumnFormula>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="t5" dataDxfId="59">
+    <tableColumn id="17" name="t5" dataDxfId="55">
       <calculatedColumnFormula>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="t1E" dataDxfId="58">
+    <tableColumn id="21" name="t1E" dataDxfId="54">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="t2E" dataDxfId="57">
+    <tableColumn id="22" name="t2E" dataDxfId="53">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="t3E" dataDxfId="4">
+    <tableColumn id="23" name="t3E" dataDxfId="52">
       <calculatedColumnFormula>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="t4E" dataDxfId="56">
+    <tableColumn id="24" name="t4E" dataDxfId="51">
       <calculatedColumnFormula>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="t5E" dataDxfId="55">
+    <tableColumn id="25" name="t5E" dataDxfId="50">
       <calculatedColumnFormula>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6861,7 +6861,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="A1:Y2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6886,45 +6886,45 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="25">
-    <tableColumn id="10" name="maxPRpm" dataDxfId="2"/>
-    <tableColumn id="14" name="maxPS" dataDxfId="1"/>
-    <tableColumn id="19" name="maxPSEco" dataDxfId="0">
+    <tableColumn id="10" name="maxPRpm" dataDxfId="48"/>
+    <tableColumn id="14" name="maxPS" dataDxfId="47"/>
+    <tableColumn id="19" name="maxPSEco" dataDxfId="46">
       <calculatedColumnFormula>Table36[maxPsEcoRate]*Table36[maxPS]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="ratedRpm"/>
     <tableColumn id="3" name="PS"/>
-    <tableColumn id="20" name="PSEco" dataDxfId="53">
+    <tableColumn id="20" name="PSEco" dataDxfId="45">
       <calculatedColumnFormula>Table36[PSEcoRate]*Table36[PS]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="maxTRpm1" dataDxfId="52"/>
-    <tableColumn id="4" name="maxTRpm" dataDxfId="51"/>
-    <tableColumn id="5" name="maxT" dataDxfId="50"/>
-    <tableColumn id="21" name="maxTEco" dataDxfId="49">
+    <tableColumn id="12" name="maxTRpm1" dataDxfId="44"/>
+    <tableColumn id="4" name="maxTRpm" dataDxfId="43"/>
+    <tableColumn id="5" name="maxT" dataDxfId="42"/>
+    <tableColumn id="21" name="maxTEco" dataDxfId="41">
       <calculatedColumnFormula>Table36[NmEcoRate]*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="idleRpm"/>
     <tableColumn id="7" name="idleRatio" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="fadeOut" dataDxfId="48"/>
-    <tableColumn id="15" name="linearDown" dataDxfId="47"/>
-    <tableColumn id="25" name="fadeOutExp" dataDxfId="46"/>
-    <tableColumn id="22" name="Efficiency" dataDxfId="45"/>
-    <tableColumn id="16" name="Factor" dataDxfId="44"/>
-    <tableColumn id="13" name="fuelMinRate" dataDxfId="12"/>
-    <tableColumn id="18" name="fuelRatedRate" dataDxfId="9">
+    <tableColumn id="11" name="fadeOut" dataDxfId="40"/>
+    <tableColumn id="15" name="linearDown" dataDxfId="39"/>
+    <tableColumn id="25" name="fadeOutExp" dataDxfId="38"/>
+    <tableColumn id="22" name="Efficiency" dataDxfId="37"/>
+    <tableColumn id="16" name="Factor" dataDxfId="36"/>
+    <tableColumn id="13" name="fuelMinRate" dataDxfId="35"/>
+    <tableColumn id="18" name="fuelRatedRate" dataDxfId="34">
       <calculatedColumnFormula>Table36[fuelMinRate]/0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="fuelMinRpm" dataDxfId="11">
+    <tableColumn id="9" name="fuelMinRpm" dataDxfId="33">
       <calculatedColumnFormula>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="fuelIdleRate" dataDxfId="10">
+    <tableColumn id="17" name="fuelIdleRate" dataDxfId="32">
       <calculatedColumnFormula>0.94*Table36[fuelRatedRate]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="normRpm" dataDxfId="43">
+    <tableColumn id="1" name="normRpm" dataDxfId="31">
       <calculatedColumnFormula>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PSEcoRate" dataDxfId="42"/>
+    <tableColumn id="8" name="PSEcoRate" dataDxfId="30"/>
     <tableColumn id="23" name="NmEcoRate"/>
-    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="41">
+    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="29">
       <calculatedColumnFormula>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6933,7 +6933,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:S4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:S4" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A3:S4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6952,61 +6952,61 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" name="f1" dataDxfId="38">
+    <tableColumn id="1" name="f1" dataDxfId="26">
       <calculatedColumnFormula>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="f2" dataDxfId="37">
+    <tableColumn id="2" name="f2" dataDxfId="25">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="f3" dataDxfId="36">
+    <tableColumn id="5" name="f3" dataDxfId="24">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="f4" dataDxfId="35">
+    <tableColumn id="6" name="f4" dataDxfId="23">
       <calculatedColumnFormula>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Nm" dataDxfId="34">
+    <tableColumn id="3" name="Nm" dataDxfId="22">
       <calculatedColumnFormula>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Nm2" dataDxfId="33">
+    <tableColumn id="4" name="Nm2" dataDxfId="21">
       <calculatedColumnFormula>Table36[PS]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Anfahrmoment" dataDxfId="32" dataCellStyle="Percent">
+    <tableColumn id="7" name="Anfahrmoment" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>Table7[Nm1000]/Table7[Nm2Eco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="AnstiegE" dataDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="17" name="AnstiegE" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxTEco]/Table7[Nm2Eco]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Anstieg" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="14" name="Anstieg" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxT]/Table7[Nm2]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Abfall" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="15" name="Abfall" dataDxfId="17" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table36[maxTRpm]/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Nm1000" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="16" name="Nm1000" dataDxfId="16" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NmEco" dataDxfId="27">
+    <tableColumn id="8" name="NmEco" dataDxfId="15">
       <calculatedColumnFormula>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Nm2Eco" dataDxfId="26">
+    <tableColumn id="9" name="Nm2Eco" dataDxfId="14">
       <calculatedColumnFormula>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="f2Eco" dataDxfId="25">
+    <tableColumn id="12" name="f2Eco" dataDxfId="13">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="f3Eco" dataDxfId="24">
+    <tableColumn id="10" name="f3Eco" dataDxfId="12">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="f4Eco" dataDxfId="23">
+    <tableColumn id="11" name="f4Eco" dataDxfId="11">
       <calculatedColumnFormula>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="idleT" dataDxfId="22">
+    <tableColumn id="13" name="idleT" dataDxfId="10">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="idleTEco" dataDxfId="21">
+    <tableColumn id="19" name="idleTEco" dataDxfId="9">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="xmlComment" dataDxfId="20">
+    <tableColumn id="21" name="xmlComment" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7023,17 +7023,17 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$A$22*Table1[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="19">
+    <tableColumn id="6" name="kw_pto" dataDxfId="7">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="18">
+    <tableColumn id="3" name="ps" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor"/>
-    <tableColumn id="5" name="xml" dataDxfId="17">
+    <tableColumn id="5" name="xml" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table1[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table1[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="16">
+    <tableColumn id="8" name="xml2" dataDxfId="4">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table1[[#This Row],[rpm]]/Table3[ratedRpm],3),""" torque=""",ROUND(Table1[[#This Row],[motor]]/MAX(Table1[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7067,16 +7067,16 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$I$2*Table13[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="15">
+    <tableColumn id="6" name="kw_pto" dataDxfId="3">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="14">
+    <tableColumn id="3" name="ps" dataDxfId="2">
       <calculatedColumnFormula>Table13[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor">
       <calculatedColumnFormula>C2/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="13">
+    <tableColumn id="5" name="xml" dataDxfId="1">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table13[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table13[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7350,7 +7350,7 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7448,49 +7448,49 @@
         <v>1900</v>
       </c>
       <c r="B2" s="14">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="C2" s="18">
         <f>Table36[maxPsEcoRate]*Table36[maxPS]</f>
-        <v>247.90909090909091</v>
+        <v>225</v>
       </c>
       <c r="D2" s="7">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="E2" s="8">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="F2" s="19">
         <f>Table36[PSEcoRate]*Table36[PS]</f>
-        <v>243.9</v>
+        <v>225</v>
       </c>
       <c r="G2" s="13">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H2" s="14">
-        <v>1550</v>
+        <v>1500</v>
       </c>
       <c r="I2" s="14">
-        <v>1173</v>
+        <v>1100</v>
       </c>
       <c r="J2" s="18">
         <f>Table36[NmEcoRate]*Table36[maxT]</f>
-        <v>1114.3499999999999</v>
+        <v>1045</v>
       </c>
       <c r="K2" s="7">
         <v>900</v>
       </c>
       <c r="L2" s="11">
-        <v>0.97</v>
+        <v>0.9</v>
       </c>
       <c r="M2" s="9">
         <v>300</v>
       </c>
       <c r="N2" s="13">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="O2" s="14">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="P2" s="14">
         <v>0.94</v>
@@ -7507,7 +7507,7 @@
       </c>
       <c r="T2" s="17">
         <f>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</f>
-        <v>1280</v>
+        <v>1300</v>
       </c>
       <c r="U2" s="19">
         <f>0.94*Table36[fuelRatedRate]</f>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="V2" s="16">
         <f>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</f>
-        <v>2200</v>
+        <v>2000</v>
       </c>
       <c r="W2" s="7">
         <v>0.9</v>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="Y2" s="29">
         <f>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</f>
-        <v>0.91818181818181821</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -7590,82 +7590,82 @@
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <f>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</f>
-        <v>3.0000000000000026E-6</v>
+        <v>2.7777777777777771E-7</v>
       </c>
       <c r="B4" s="12">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>4.2657041279292737E-4</v>
+        <v>4.0010202645651574E-4</v>
       </c>
       <c r="C4" s="12">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.2187726079797926E-6</v>
+        <v>1.0002550661412894E-6</v>
       </c>
       <c r="D4" s="12">
         <f>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>-2.5000000000000001E-5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="12">
         <f>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</f>
-        <v>997.87151702786366</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="F4" s="12">
         <f>Table36[PS]/1.36*9550/Table36[ratedRpm]</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="G4" s="23">
         <f>Table7[Nm1000]/Table7[Nm2Eco]</f>
-        <v>1.3663584552075885</v>
+        <v>1.1694057268437723</v>
       </c>
       <c r="H4" s="24">
         <f>Table36[maxTEco]/Table7[Nm2Eco]-1</f>
-        <v>0.36635845520758847</v>
+        <v>0.25667481093659106</v>
       </c>
       <c r="I4" s="24">
         <f>Table36[maxT]/Table7[Nm2]-1</f>
-        <v>0.2944448523019263</v>
+        <v>0.19053403141361258</v>
       </c>
       <c r="J4" s="25">
         <f>1-Table36[maxTRpm]/Table36[ratedRpm]</f>
-        <v>0.26190476190476186</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="K4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</f>
-        <v>1114.3499999999999</v>
+        <v>972.43055555555554</v>
       </c>
       <c r="L4" s="12">
         <f>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</f>
-        <v>916.22748381649308</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="M4" s="12">
         <f>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="N4" s="12">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>5.0797714537880974E-4</v>
+        <v>5.1062297243248866E-4</v>
       </c>
       <c r="O4" s="12">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.4513632725108851E-6</v>
+        <v>1.2765574310812216E-6</v>
       </c>
       <c r="P4" s="12">
         <f>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>1.0022727272727252E-4</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</f>
-        <v>1137.81</v>
+        <v>990</v>
       </c>
       <c r="R4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</f>
-        <v>1080.9195</v>
+        <v>940.5</v>
       </c>
       <c r="S4" s="12" t="str">
         <f>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 270(248) | 2100: 271(244) | 1000..1550: 1173(1114) | 97 | 0.8 | 300 | 2.2 | 2200 | 1280: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="62.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" s="4" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -7765,15 +7765,15 @@
       </c>
       <c r="J7" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>311.38559556786686</v>
+        <v>304.1749999999999</v>
       </c>
       <c r="K7" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 270(248) | 2100: 271(244) | 1000..1550: 1173(1114) | 97 | 0.8 | 300 | 2.2 | 2200 | 1280: 207 --&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
       </c>
       <c r="L7" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 270(248) | 2100: 271(244) | 1000..1550: 1173(1114) | 97 | 0.8 | 300 | 2.2 | 2200 | 1280: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
       </c>
       <c r="M7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="N7" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>412.50000000000011</v>
       </c>
       <c r="O7" s="3" t="e">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
@@ -7789,11 +7789,11 @@
       </c>
       <c r="P7" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2529696.6911764704</v>
+        <v>1755514.7058823528</v>
       </c>
       <c r="Q7" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="S7" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>391.87500000000011</v>
       </c>
       <c r="T7" s="3" t="e">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
@@ -7809,11 +7809,11 @@
       </c>
       <c r="U7" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>1579963.2352941176</v>
       </c>
       <c r="V7" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -7822,81 +7822,81 @@
       </c>
       <c r="B8" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>212.26633744855968</v>
+        <v>240.37037037037044</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>201.65302057613169</v>
+        <v>228.3518518518519</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>212.26633744855968</v>
+        <v>240.37037037037044</v>
       </c>
       <c r="G8" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>201.65302057613169</v>
+        <v>228.3518518518519</v>
       </c>
       <c r="H8" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>3.0228504600004311</v>
+        <v>3.4230754314523959</v>
       </c>
       <c r="I8" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>2.8717079370004095</v>
+        <v>3.2519216598797756</v>
       </c>
       <c r="J8" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>295.71246537396109</v>
+        <v>289.7999999999999</v>
       </c>
       <c r="K8" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="212" motorTorqueEco="202" fuelUsageRatio="295.7"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="240" motorTorqueEco="228" fuelUsageRatio="289.8"/&gt;</v>
       </c>
       <c r="L8" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.045" torque="0.181"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.05" torque="0.219"/&gt;</v>
       </c>
       <c r="M8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>238.79962962962966</v>
+        <v>207.77777777777783</v>
       </c>
       <c r="N8" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>501.11111111111131</v>
       </c>
       <c r="O8" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1152.2705060971757</v>
+        <v>329.80359907120709</v>
       </c>
       <c r="P8" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>24647.426470588231</v>
+        <v>17555.147058823528</v>
       </c>
       <c r="Q8" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>226.85964814814818</v>
+        <v>197.38888888888894</v>
       </c>
       <c r="S8" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>476.05555555555571</v>
       </c>
       <c r="T8" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1090.8987633905238</v>
+        <v>111.19823916408642</v>
       </c>
       <c r="U8" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>15799.632352941177</v>
       </c>
       <c r="V8" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -7905,81 +7905,81 @@
       </c>
       <c r="B9" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>437.0189300411522</v>
+        <v>704.81481481481478</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>415.16798353909468</v>
+        <v>669.57407407407413</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>437.0189300411522</v>
+        <v>704.81481481481478</v>
       </c>
       <c r="G9" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>415.16798353909468</v>
+        <v>669.57407407407413</v>
       </c>
       <c r="H9" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>24.894062611768252</v>
+        <v>40.148613535000962</v>
       </c>
       <c r="I9" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>23.649359481179843</v>
+        <v>38.141182858250929</v>
       </c>
       <c r="J9" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>256.33850415512461</v>
+        <v>253.57499999999993</v>
       </c>
       <c r="K9" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="437" motorTorqueEco="415" fuelUsageRatio="256.3"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="705" motorTorqueEco="670" fuelUsageRatio="253.6"/&gt;</v>
       </c>
       <c r="L9" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.182" torque="0.373"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.2" torque="0.641"/&gt;</v>
       </c>
       <c r="M9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>786.63407407407396</v>
+        <v>684.44444444444446</v>
       </c>
       <c r="N9" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>730.27777777777783</v>
       </c>
       <c r="O9" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1255.203165476717</v>
+        <v>676.39197948916387</v>
       </c>
       <c r="P9" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>5727.3667279411757</v>
+        <v>4388.786764705882</v>
       </c>
       <c r="Q9" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>747.30237037037034</v>
+        <v>650.22222222222217</v>
       </c>
       <c r="S9" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>693.76388888888903</v>
       </c>
       <c r="T9" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1207.346283106544</v>
+        <v>531.4090315402475</v>
       </c>
       <c r="U9" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>393.19539605615779</v>
+        <v>3949.9080882352941</v>
       </c>
       <c r="V9" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -7988,81 +7988,81 @@
       </c>
       <c r="B10" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>906.36374485596684</v>
+        <v>912.59259259259272</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>861.04555761316851</v>
+        <v>866.96296296296305</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>906.36374485596684</v>
+        <v>912.59259259259272</v>
       </c>
       <c r="G10" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>861.04555761316851</v>
+        <v>866.96296296296305</v>
       </c>
       <c r="H10" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>90.351652890353989</v>
+        <v>90.972580957921295</v>
       </c>
       <c r="I10" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>85.834070245836287</v>
+        <v>86.423951910025224</v>
       </c>
       <c r="J10" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>228.43268698060939</v>
+        <v>227.7</v>
       </c>
       <c r="K10" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="906" motorTorqueEco="861" fuelUsageRatio="228.4"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="913" motorTorqueEco="867" fuelUsageRatio="227.7"/&gt;</v>
       </c>
       <c r="L10" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.318" torque="0.773"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.35" torque="0.83"/&gt;</v>
       </c>
       <c r="M10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1081.6218518518517</v>
+        <v>941.11111111111109</v>
       </c>
       <c r="N10" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>856.28999999999974</v>
+        <v>904.44444444444457</v>
       </c>
       <c r="O10" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1306.6694951664876</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="P10" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>3069.6428571428564</v>
+        <v>2507.8781512605042</v>
       </c>
       <c r="Q10" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>1027.5407592592592</v>
+        <v>894.05555555555554</v>
       </c>
       <c r="S10" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>813.47549999999967</v>
+        <v>859.22222222222229</v>
       </c>
       <c r="T10" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1265.5700429645542</v>
+        <v>831.55959752321985</v>
       </c>
       <c r="U10" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1039.0823147440824</v>
+        <v>2257.0903361344535</v>
       </c>
       <c r="V10" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -8071,81 +8071,81 @@
       </c>
       <c r="B11" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1042.4092181069957</v>
+        <v>953.33333333333337</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>990.28875720164592</v>
+        <v>905.66666666666674</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1042.4092181069957</v>
+        <v>953.33333333333337</v>
       </c>
       <c r="G11" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>990.28875720164592</v>
+        <v>905.66666666666674</v>
       </c>
       <c r="H11" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>118.75824390580225</v>
+        <v>108.61012216404887</v>
       </c>
       <c r="I11" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>112.82033171051211</v>
+        <v>103.17961605584642</v>
       </c>
       <c r="J11" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>221.67922437673127</v>
+        <v>221.37499999999997</v>
       </c>
       <c r="K11" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="1042" motorTorqueEco="990" fuelUsageRatio="221.7"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="953" motorTorqueEco="906" fuelUsageRatio="221.4"/&gt;</v>
       </c>
       <c r="L11" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.364" torque="0.889"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.4" torque="0.867"/&gt;</v>
       </c>
       <c r="M11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1123.7629629629628</v>
+        <v>977.77777777777771</v>
       </c>
       <c r="N11" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1032.2399999999998</v>
+        <v>950.27777777777783</v>
       </c>
       <c r="O11" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1312.3879762431288</v>
+        <v>984.47053986068101</v>
       </c>
       <c r="P11" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2635.466452205882</v>
+        <v>2194.393382352941</v>
       </c>
       <c r="Q11" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>1067.5748148148148</v>
+        <v>928.8888888888888</v>
       </c>
       <c r="S11" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>980.62799999999982</v>
+        <v>902.76388888888891</v>
       </c>
       <c r="T11" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1272.0393496154443</v>
+        <v>904.9297358746129</v>
       </c>
       <c r="U11" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1111.5400442847615</v>
+        <v>1974.9540441176471</v>
       </c>
       <c r="V11" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -8154,81 +8154,81 @@
       </c>
       <c r="B12" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1137.81</v>
+        <v>990</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1080.9195</v>
+        <v>940.5</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1137.81</v>
+        <v>990</v>
       </c>
       <c r="G12" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1080.9195</v>
+        <v>940.5</v>
       </c>
       <c r="H12" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>145.83030785340313</v>
+        <v>126.88586387434555</v>
       </c>
       <c r="I12" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>138.53879246073296</v>
+        <v>120.54157068062827</v>
       </c>
       <c r="J12" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
         <v>216.2</v>
       </c>
       <c r="K12" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="1138" motorTorqueEco="1081" fuelUsageRatio="216.2"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="990" motorTorqueEco="941" fuelUsageRatio="216.2"/&gt;</v>
       </c>
       <c r="L12" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.409" torque="0.97"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.45" torque="0.9"/&gt;</v>
       </c>
       <c r="M12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1137.81</v>
+        <v>990</v>
       </c>
       <c r="N12" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1137.81</v>
+        <v>990</v>
       </c>
       <c r="O12" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1312.3879762431288</v>
+        <v>1033.9831656346751</v>
       </c>
       <c r="P12" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2301.6748366013071</v>
+        <v>1950.5718954248364</v>
       </c>
       <c r="Q12" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>1080.9195</v>
+        <v>940.5</v>
       </c>
       <c r="S12" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1080.9195</v>
+        <v>940.5</v>
       </c>
       <c r="T12" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1272.0393496154441</v>
+        <v>964.95984907120737</v>
       </c>
       <c r="U12" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1152.2560160427822</v>
+        <v>1755.5147058823529</v>
       </c>
       <c r="V12" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -8237,81 +8237,81 @@
       </c>
       <c r="B13" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>972.43055555555554</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="G13" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>972.43055555555554</v>
       </c>
       <c r="H13" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>167.04502617801046</v>
+        <v>145.77079697498544</v>
       </c>
       <c r="I13" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>158.69277486910991</v>
+        <v>138.48225712623619</v>
       </c>
       <c r="J13" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>211.99501385041552</v>
+        <v>212.17499999999998</v>
       </c>
       <c r="K13" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="212"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1024" motorTorqueEco="972" fuelUsageRatio="212.2"/&gt;</v>
       </c>
       <c r="L13" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.455" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="0.931"/&gt;</v>
       </c>
       <c r="M13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1123.7629629629628</v>
+        <v>977.77777777777771</v>
       </c>
       <c r="N13" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1173</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="O13" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1306.6694951664876</v>
+        <v>1072.4929856811145</v>
       </c>
       <c r="P13" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2038.1525735294115</v>
+        <v>1755.5147058823527</v>
       </c>
       <c r="Q13" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>1067.5748148148148</v>
+        <v>928.8888888888888</v>
       </c>
       <c r="S13" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1114.3499999999999</v>
+        <v>972.43055555555554</v>
       </c>
       <c r="T13" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1265.5700429645542</v>
+        <v>1011.6499371130031</v>
       </c>
       <c r="U13" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1170.7527573529424</v>
+        <v>1579.9632352941176</v>
       </c>
       <c r="V13" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -8320,81 +8320,81 @@
       </c>
       <c r="B14" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>998.55555555555566</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="G14" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>998.55555555555566</v>
       </c>
       <c r="H14" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>183.74952879581153</v>
+        <v>164.65573007562537</v>
       </c>
       <c r="I14" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>174.56205235602093</v>
+        <v>156.42294357184412</v>
       </c>
       <c r="J14" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>209.06426592797783</v>
+        <v>209.3</v>
       </c>
       <c r="K14" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="209.1"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1051" motorTorqueEco="999" fuelUsageRatio="209.3"/&gt;</v>
       </c>
       <c r="L14" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.55" torque="0.956"/&gt;</v>
       </c>
       <c r="M14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1081.6218518518517</v>
+        <v>941.11111111111109</v>
       </c>
       <c r="N14" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1137.81</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="O14" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1295.2325330132053</v>
+        <v>1100</v>
       </c>
       <c r="P14" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1825.7352941176468</v>
+        <v>1595.922459893048</v>
       </c>
       <c r="Q14" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>1027.5407592592592</v>
+        <v>894.05555555555554</v>
       </c>
       <c r="S14" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1080.9195</v>
+        <v>998.55555555555566</v>
       </c>
       <c r="T14" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1252.6314296627743</v>
+        <v>1045</v>
       </c>
       <c r="U14" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1173.0900583373852</v>
+        <v>1436.3302139037432</v>
       </c>
       <c r="V14" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -8403,81 +8403,81 @@
       </c>
       <c r="B15" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1072.5</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>1018.875</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1072.5</v>
       </c>
       <c r="G15" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>1018.875</v>
       </c>
       <c r="H15" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>200.4540314136126</v>
+        <v>183.27958115183247</v>
       </c>
       <c r="I15" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>190.43132984293194</v>
+        <v>174.11560209424087</v>
       </c>
       <c r="J15" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.40775623268698</v>
+        <v>207.57499999999999</v>
       </c>
       <c r="K15" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="207.4"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1073" motorTorqueEco="1019" fuelUsageRatio="207.6"/&gt;</v>
       </c>
       <c r="L15" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.545" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.6" torque="0.975"/&gt;</v>
       </c>
       <c r="M15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>1011.3866666666667</v>
+        <v>880.00000000000011</v>
       </c>
       <c r="N15" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1032.2399999999998</v>
+        <v>1072.5</v>
       </c>
       <c r="O15" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1278.0770897832817</v>
+        <v>1116.5042085913312</v>
       </c>
       <c r="P15" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1651.6467524509803</v>
+        <v>1462.9289215686274</v>
       </c>
       <c r="Q15" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>960.81733333333341</v>
+        <v>836.00000000000011</v>
       </c>
       <c r="S15" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>980.62799999999982</v>
+        <v>1018.875</v>
       </c>
       <c r="T15" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1233.2235097101041</v>
+        <v>1065.010037732198</v>
       </c>
       <c r="U15" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1163.3077790775405</v>
+        <v>1316.6360294117646</v>
       </c>
       <c r="V15" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -8486,81 +8486,81 @@
       </c>
       <c r="B16" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>1033.3888888888889</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="G16" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>1033.3888888888889</v>
       </c>
       <c r="H16" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>217.15853403141364</v>
+        <v>201.38126817917399</v>
       </c>
       <c r="I16" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>206.30060732984293</v>
+        <v>191.31220477021526</v>
       </c>
       <c r="J16" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.01368233194526</v>
+        <v>207</v>
       </c>
       <c r="K16" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="207"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1088" motorTorqueEco="1033" fuelUsageRatio="207"/&gt;</v>
       </c>
       <c r="L16" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.591" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.65" torque="0.989"/&gt;</v>
       </c>
       <c r="M16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>913.05740740740737</v>
+        <v>794.44444444444446</v>
       </c>
       <c r="N16" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>856.28999999999974</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="O16" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1255.203165476717</v>
+        <v>1122.0056114551082</v>
       </c>
       <c r="P16" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1507.0418552036199</v>
+        <v>1350.3959276018097</v>
       </c>
       <c r="Q16" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>867.40453703703702</v>
+        <v>754.72222222222229</v>
       </c>
       <c r="S16" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>813.47549999999967</v>
+        <v>1033.3888888888889</v>
       </c>
       <c r="T16" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1207.3462831065438</v>
+        <v>1071.6800503095974</v>
       </c>
       <c r="U16" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1144.2027457836284</v>
+        <v>1215.356334841629</v>
       </c>
       <c r="V16" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -8569,81 +8569,81 @@
       </c>
       <c r="B17" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>1042.0972222222222</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="G17" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>1042.0972222222222</v>
       </c>
       <c r="H17" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>233.86303664921471</v>
+        <v>218.699709133217</v>
       </c>
       <c r="I17" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>222.16988481675392</v>
+        <v>207.76472367655614</v>
       </c>
       <c r="J17" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.49256395002973</v>
+        <v>207.63888888888889</v>
       </c>
       <c r="K17" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="207.5"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1097" motorTorqueEco="1042" fuelUsageRatio="207.6"/&gt;</v>
       </c>
       <c r="L17" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.636" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.7" torque="0.997"/&gt;</v>
       </c>
       <c r="M17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>786.63407407407396</v>
+        <v>684.44444444444446</v>
       </c>
       <c r="N17" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>609.95999999999947</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="O17" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1226.6107600935113</v>
+        <v>1116.5042085913312</v>
       </c>
       <c r="P17" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1385.6026785714284</v>
+        <v>1253.9390756302521</v>
       </c>
       <c r="Q17" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>747.30237037037034</v>
+        <v>650.22222222222217</v>
       </c>
       <c r="S17" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>579.46199999999953</v>
+        <v>1042.0972222222222</v>
       </c>
       <c r="T17" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1174.9997498520936</v>
+        <v>1065.010037732198</v>
       </c>
       <c r="U17" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1117.7726914629488</v>
+        <v>1128.5451680672268</v>
       </c>
       <c r="V17" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -8652,81 +8652,81 @@
       </c>
       <c r="B18" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1173</v>
+        <v>1100</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1114.3499999999999</v>
+        <v>1045</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1173</v>
+        <v>1100</v>
       </c>
       <c r="G18" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1114.3499999999999</v>
+        <v>1045</v>
       </c>
       <c r="H18" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>250.56753926701575</v>
+        <v>234.97382198952886</v>
       </c>
       <c r="I18" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>238.03916230366491</v>
+        <v>223.22513089005241</v>
       </c>
       <c r="J18" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>208.65556216537775</v>
+        <v>209.55555555555554</v>
       </c>
       <c r="K18" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1173" motorTorqueEco="1114" fuelUsageRatio="208.7"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1100" motorTorqueEco="1045" fuelUsageRatio="209.6"/&gt;</v>
       </c>
       <c r="L18" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.682" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.75" torque="1"/&gt;</v>
       </c>
       <c r="M18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>632.11666666666656</v>
+        <v>549.99999999999989</v>
       </c>
       <c r="N18" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>293.2499999999992</v>
+        <v>1100</v>
       </c>
       <c r="O18" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1192.2998736336638</v>
+        <v>1100</v>
       </c>
       <c r="P18" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1282.6960784313726</v>
+        <v>1170.3431372549019</v>
       </c>
       <c r="Q18" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>600.51083333333327</v>
+        <v>522.49999999999989</v>
       </c>
       <c r="S18" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>278.58749999999924</v>
+        <v>1045</v>
       </c>
       <c r="T18" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1136.1839099467538</v>
+        <v>1045</v>
       </c>
       <c r="U18" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1085.4826203208556</v>
+        <v>1053.3088235294117</v>
       </c>
       <c r="V18" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -8735,81 +8735,81 @@
       </c>
       <c r="B19" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1152.2705060971757</v>
+        <v>1072.4929856811145</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1088.0201370320856</v>
+        <v>987.47702205882354</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1152.2705060971757</v>
+        <v>1072.4929856811145</v>
       </c>
       <c r="G19" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1088.0201370320856</v>
+        <v>987.47702205882354</v>
       </c>
       <c r="H19" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>262.54875615366012</v>
+        <v>244.37117663268117</v>
       </c>
       <c r="I19" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>247.90909090909093</v>
+        <v>225</v>
       </c>
       <c r="J19" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>210.5026769779893</v>
+        <v>212.75</v>
       </c>
       <c r="K19" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1152" motorTorqueEco="1088" fuelUsageRatio="210.5"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1072" motorTorqueEco="987" fuelUsageRatio="212.8"/&gt;</v>
       </c>
       <c r="L19" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.727" torque="0.982"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.8" torque="0.975"/&gt;</v>
       </c>
       <c r="M19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>449.50518518518538</v>
+        <v>391.11111111111131</v>
       </c>
       <c r="N19" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="O19" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1152.2705060971757</v>
+        <v>1072.4929856811145</v>
       </c>
       <c r="P19" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1194.8471966911764</v>
+        <v>1097.1966911764705</v>
       </c>
       <c r="Q19" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>427.02992592592614</v>
+        <v>371.55555555555577</v>
       </c>
       <c r="S19" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>1042.0972222222222</v>
       </c>
       <c r="T19" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1088.0201370320856</v>
+        <v>987.47702205882354</v>
       </c>
       <c r="U19" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1048.4312855113637</v>
+        <v>987.47702205882354</v>
       </c>
       <c r="V19" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -8818,81 +8818,81 @@
       </c>
       <c r="B20" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1106.5226574840462</v>
+        <v>1032.6557093425604</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1024.0189525007863</v>
+        <v>929.39013840830444</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1106.5226574840462</v>
+        <v>1032.6557093425604</v>
       </c>
       <c r="G20" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1024.0189525007863</v>
+        <v>929.39013840830444</v>
       </c>
       <c r="H20" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>267.88276273331041</v>
+        <v>249.99999999999994</v>
       </c>
       <c r="I20" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>247.90909090909088</v>
+        <v>225</v>
       </c>
       <c r="J20" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>213.03390838786436</v>
+        <v>217.22222222222223</v>
       </c>
       <c r="K20" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1107" motorTorqueEco="1024" fuelUsageRatio="213"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1033" motorTorqueEco="929" fuelUsageRatio="217.2"/&gt;</v>
       </c>
       <c r="L20" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.773" torque="0.943"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.85" torque="0.939"/&gt;</v>
       </c>
       <c r="M20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>238.79962962962966</v>
+        <v>207.77777777777783</v>
       </c>
       <c r="N20" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="O20" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1106.5226574840462</v>
+        <v>1032.6557093425604</v>
       </c>
       <c r="P20" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1119.3987889273355</v>
+        <v>1032.6557093425604</v>
       </c>
       <c r="Q20" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>226.85964814814818</v>
+        <v>197.38888888888894</v>
       </c>
       <c r="S20" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>1033.3888888888889</v>
       </c>
       <c r="T20" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1024.0189525007863</v>
+        <v>929.39013840830444</v>
       </c>
       <c r="U20" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1007.4589100346021</v>
+        <v>929.39013840830444</v>
       </c>
       <c r="V20" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -8901,41 +8901,41 @@
       </c>
       <c r="B21" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>1053.3088235294117</v>
+        <v>975.28594771241819</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>967.12901069518705</v>
+        <v>877.75735294117646</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1053.3088235294117</v>
+        <v>975.28594771241819</v>
       </c>
       <c r="G21" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>967.12901069518705</v>
+        <v>877.75735294117646</v>
       </c>
       <c r="H21" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>270</v>
+        <v>249.99999999999994</v>
       </c>
       <c r="I21" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>247.90909090909088</v>
+        <v>225</v>
       </c>
       <c r="J21" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>216.24925639500299</v>
+        <v>222.97222222222223</v>
       </c>
       <c r="K21" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="1053" motorTorqueEco="967" fuelUsageRatio="216.2"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="975" motorTorqueEco="878" fuelUsageRatio="223"/&gt;</v>
       </c>
       <c r="L21" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.818" torque="0.898"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.9" torque="0.887"/&gt;</v>
       </c>
       <c r="M21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8943,19 +8943,19 @@
       </c>
       <c r="N21" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>1072.5</v>
       </c>
       <c r="O21" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1053.3088235294117</v>
+        <v>975.28594771241819</v>
       </c>
       <c r="P21" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1054.284109477124</v>
+        <v>975.28594771241819</v>
       </c>
       <c r="Q21" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -8963,19 +8963,19 @@
       </c>
       <c r="S21" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>1018.875</v>
       </c>
       <c r="T21" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>967.12901069518705</v>
+        <v>877.75735294117646</v>
       </c>
       <c r="U21" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>963.2190006684491</v>
+        <v>877.75735294117646</v>
       </c>
       <c r="V21" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -8984,81 +8984,81 @@
       </c>
       <c r="B22" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>997.87151702786366</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>916.22748381649308</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>997.87151702786366</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="G22" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>916.22748381649308</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="H22" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>269.99999999999994</v>
+        <v>250</v>
       </c>
       <c r="I22" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>247.90909090909088</v>
+        <v>225</v>
       </c>
       <c r="J22" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>220.14872099940513</v>
+        <v>230</v>
       </c>
       <c r="K22" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="998" motorTorqueEco="916" fuelUsageRatio="220.1"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="924" motorTorqueEco="832" fuelUsageRatio="230"/&gt;</v>
       </c>
       <c r="L22" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.864" torque="0.851"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.95" torque="0.84"/&gt;</v>
       </c>
       <c r="M22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-266.89370370370386</v>
+        <v>-232.22222222222237</v>
       </c>
       <c r="N22" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="O22" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>997.87151702786366</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="P22" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>997.87151702786366</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="Q22" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="R22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-253.54901851851866</v>
+        <v>-220.61111111111126</v>
       </c>
       <c r="S22" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>998.55555555555566</v>
       </c>
       <c r="T22" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>916.22748381649308</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="U22" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>916.22748381649308</v>
+        <v>831.55959752321974</v>
       </c>
       <c r="V22" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>831.55959752321974</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -9067,81 +9067,81 @@
       </c>
       <c r="B23" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>948.85569852941171</v>
+        <v>796.06627888149092</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>866.89710060160417</v>
+        <v>716.45965099334182</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>948.85569852941171</v>
+        <v>796.06627888149092</v>
       </c>
       <c r="G23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>866.89710060160417</v>
+        <v>716.45965099334182</v>
       </c>
       <c r="H23" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>270.25</v>
+        <v>226.7330134615346</v>
       </c>
       <c r="I23" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>246.90681818181815</v>
+        <v>204.05971211538113</v>
       </c>
       <c r="J23" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>224.73230220107078</v>
+        <v>244.75450687929043</v>
       </c>
       <c r="K23" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="949" motorTorqueEco="867" fuelUsageRatio="224.7"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="796" motorTorqueEco="716" fuelUsageRatio="244.8"/&gt;</v>
       </c>
       <c r="L23" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.909" torque="0.809"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.724"/&gt;</v>
       </c>
       <c r="M23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-561.88148148148173</v>
+        <v>-488.88888888888908</v>
       </c>
       <c r="N23" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="O23" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>934.96822518481054</v>
+        <v>852.4368711300308</v>
       </c>
       <c r="P23" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>948.85569852941171</v>
+        <v>877.75735294117635</v>
       </c>
       <c r="Q23" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>796.06627888149092</v>
       </c>
       <c r="R23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-533.78740740740761</v>
+        <v>-464.44444444444463</v>
       </c>
       <c r="S23" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>972.43055555555554</v>
       </c>
       <c r="T23" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>845.06511065670281</v>
+        <v>744.84943401702776</v>
       </c>
       <c r="U23" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>866.89710060160417</v>
+        <v>789.98161764705878</v>
       </c>
       <c r="V23" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>716.45965099334182</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -9150,81 +9150,81 @@
       </c>
       <c r="B24" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>906.17997198879539</v>
+        <v>478.62033819495952</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>815.56197478991601</v>
+        <v>430.75830437546352</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>906.17997198879539</v>
+        <v>478.62033819495952</v>
       </c>
       <c r="G24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>815.56197478991601</v>
+        <v>430.75830437546352</v>
       </c>
       <c r="H24" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>270.99999999999994</v>
+        <v>143.13504564238789</v>
       </c>
       <c r="I24" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>243.9</v>
+        <v>128.8215410781491</v>
       </c>
       <c r="J24" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>230</v>
+        <v>313.46409493927865</v>
       </c>
       <c r="K24" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="906" motorTorqueEco="816" fuelUsageRatio="230"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="479" motorTorqueEco="431" fuelUsageRatio="313.5"/&gt;</v>
       </c>
       <c r="L24" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.955" torque="0.773"/&gt;</v>
+        <v/>
       </c>
       <c r="M24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-884.96333333333371</v>
+        <v>-770.00000000000034</v>
       </c>
       <c r="N24" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>990</v>
       </c>
       <c r="O24" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>866.34645226511634</v>
+        <v>769.91582817337451</v>
       </c>
       <c r="P24" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>906.17997198879539</v>
+        <v>835.95938375350136</v>
       </c>
       <c r="Q24" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>906.17997198879539</v>
+        <v>478.62033819495952</v>
       </c>
       <c r="R24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-840.71516666666707</v>
+        <v>-731.50000000000034</v>
       </c>
       <c r="S24" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>940.5</v>
       </c>
       <c r="T24" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>767.43343084602259</v>
+        <v>644.79924535603709</v>
       </c>
       <c r="U24" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>815.56197478991601</v>
+        <v>752.36344537815125</v>
       </c>
       <c r="V24" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>815.56197478991601</v>
+        <v>430.75830437546352</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -9233,81 +9233,81 @@
       </c>
       <c r="B25" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>825.35460243878128</v>
+        <v>0</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>742.81914219490329</v>
+        <v>0</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>825.35460243878128</v>
+        <v>0</v>
       </c>
       <c r="G25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>742.81914219490329</v>
+        <v>0</v>
       </c>
       <c r="H25" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>258.58230057558467</v>
+        <v>0</v>
       </c>
       <c r="I25" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>232.72407051802622</v>
+        <v>0</v>
       </c>
       <c r="J25" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>244.75450687929043</v>
+        <v>460</v>
       </c>
       <c r="K25" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="825" motorTorqueEco="743" fuelUsageRatio="244.8"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="0" motorTorqueEco="0" fuelUsageRatio="460"/&gt;</v>
       </c>
       <c r="L25" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.704"/&gt;</v>
+        <v/>
       </c>
       <c r="M25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-1236.1392592592597</v>
+        <v>-1075.5555555555559</v>
       </c>
       <c r="N25" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>950.27777777777783</v>
       </c>
       <c r="O25" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>792.00619826878096</v>
+        <v>676.39197948916399</v>
       </c>
       <c r="P25" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>868.97977941176464</v>
+        <v>797.96122994652399</v>
       </c>
       <c r="Q25" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>825.35460243878128</v>
+        <v>0</v>
       </c>
       <c r="R25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1174.3322962962966</v>
+        <v>-1021.7777777777782</v>
       </c>
       <c r="S25" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>902.76388888888891</v>
       </c>
       <c r="T25" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>683.33244438445251</v>
+        <v>531.40903154024738</v>
       </c>
       <c r="U25" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>762.49548037190084</v>
+        <v>718.16510695187162</v>
       </c>
       <c r="V25" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>742.81914219490329</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -9316,37 +9316,37 @@
       </c>
       <c r="B26" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>534.80409581228059</v>
+        <v>0</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="3">
         <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>481.32368623105259</v>
+        <v>0</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>534.80409581228059</v>
+        <v>0</v>
       </c>
       <c r="G26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>481.32368623105259</v>
+        <v>0</v>
       </c>
       <c r="H26" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>175.16934153935222</v>
+        <v>0</v>
       </c>
       <c r="I26" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>157.65240738541704</v>
+        <v>0</v>
       </c>
       <c r="J26" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>313.46409493927865</v>
+        <v>460</v>
       </c>
       <c r="K26" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="535" motorTorqueEco="481" fuelUsageRatio="313.5"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v/>
       </c>
       <c r="L26" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
@@ -9354,43 +9354,43 @@
       </c>
       <c r="M26" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-1615.4092592592583</v>
+        <v>-1405.5555555555547</v>
       </c>
       <c r="N26" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>904.44444444444457</v>
       </c>
       <c r="O26" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>711.94746319580429</v>
+        <v>571.86532507739912</v>
       </c>
       <c r="P26" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>836.54092071611251</v>
+        <v>763.26726342710992</v>
       </c>
       <c r="Q26" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>534.80409581228059</v>
+        <v>0</v>
       </c>
       <c r="R26" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1534.6387962962954</v>
+        <v>-1335.2777777777769</v>
       </c>
       <c r="S26" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>859.22222222222229</v>
       </c>
       <c r="T26" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>592.76215127199214</v>
+        <v>404.67879256965921</v>
       </c>
       <c r="U26" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>707.92344803534058</v>
+        <v>686.9405370843989</v>
       </c>
       <c r="V26" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>481.32368623105259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -9428,8 +9428,8 @@
         <v>460</v>
       </c>
       <c r="K27" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="0" motorTorqueEco="0" fuelUsageRatio="460"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v/>
       </c>
       <c r="L27" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
@@ -9437,19 +9437,19 @@
       </c>
       <c r="M27" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-2022.7733333333326</v>
+        <v>-1759.9999999999995</v>
       </c>
       <c r="N27" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>852.5</v>
       </c>
       <c r="O27" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>626.17024704618655</v>
+        <v>456.33586493808031</v>
       </c>
       <c r="P27" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>808.26822916666652</v>
+        <v>731.4644607843137</v>
       </c>
       <c r="Q27" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9457,19 +9457,19 @@
       </c>
       <c r="R27" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1921.6346666666661</v>
+        <v>-1671.9999999999995</v>
       </c>
       <c r="S27" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>809.875</v>
       </c>
       <c r="T27" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>495.72255150864191</v>
+        <v>264.60852844427217</v>
       </c>
       <c r="U27" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>652.03407002005349</v>
+        <v>658.31801470588232</v>
       </c>
       <c r="V27" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9511,7 +9511,7 @@
         <v>460</v>
       </c>
       <c r="K28" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L28" s="10" t="str">
@@ -9520,19 +9520,19 @@
       </c>
       <c r="M28" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-2458.2314814814813</v>
+        <v>-2138.8888888888887</v>
       </c>
       <c r="N28" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>794.44444444444457</v>
       </c>
       <c r="O28" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>534.67454981992751</v>
+        <v>329.80359907120709</v>
       </c>
       <c r="P28" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>783.66176470588232</v>
+        <v>702.2058823529411</v>
       </c>
       <c r="Q28" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9540,19 +9540,19 @@
       </c>
       <c r="R28" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-2335.3199074074073</v>
+        <v>-2031.9444444444443</v>
       </c>
       <c r="S28" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>754.72222222222229</v>
       </c>
       <c r="T28" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>392.21364509440167</v>
+        <v>111.19823916408642</v>
       </c>
       <c r="U28" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>594.98542780748676</v>
+        <v>631.98529411764707</v>
       </c>
       <c r="V28" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9594,7 +9594,7 @@
         <v>460</v>
       </c>
       <c r="K29" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L29" s="10" t="str">
@@ -9603,19 +9603,19 @@
       </c>
       <c r="M29" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-3669.7884259259245</v>
+        <v>-3193.0555555555547</v>
       </c>
       <c r="N29" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>622.56944444444457</v>
       </c>
       <c r="O29" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>280.91695204397502</v>
+        <v>0</v>
       </c>
       <c r="P29" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>735.56066176470586</v>
+        <v>638.36898395721914</v>
       </c>
       <c r="Q29" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9623,19 +9623,19 @@
       </c>
       <c r="R29" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-3486.2990046296286</v>
+        <v>-3033.4027777777769</v>
       </c>
       <c r="S29" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>591.44097222222229</v>
       </c>
       <c r="T29" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>105.13816246115711</v>
+        <v>0</v>
       </c>
       <c r="U29" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>448.12196919056908</v>
+        <v>574.5320855614973</v>
       </c>
       <c r="V29" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9677,7 +9677,7 @@
         <v>460</v>
       </c>
       <c r="K30" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L30" s="10" t="str">
@@ -9686,11 +9686,11 @@
       </c>
       <c r="M30" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-5056.9333333333343</v>
+        <v>-4400.0000000000009</v>
       </c>
       <c r="N30" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>412.50000000000011</v>
       </c>
       <c r="O30" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="P30" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>702.7910539215685</v>
+        <v>585.17156862745094</v>
       </c>
       <c r="Q30" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9706,11 +9706,11 @@
       </c>
       <c r="R30" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-4804.086666666668</v>
+        <v>-4180.0000000000009</v>
       </c>
       <c r="S30" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>391.87500000000011</v>
       </c>
       <c r="T30" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
@@ -9718,7 +9718,7 @@
       </c>
       <c r="U30" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>296.41067847593644</v>
+        <v>526.65441176470586</v>
       </c>
       <c r="V30" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9760,7 +9760,7 @@
         <v>460</v>
       </c>
       <c r="K31" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L31" s="10" t="str">
@@ -9769,11 +9769,11 @@
       </c>
       <c r="M31" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-6619.6662037037031</v>
+        <v>-5759.7222222222217</v>
       </c>
       <c r="N31" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>0</v>
+        <v>164.23611111111137</v>
       </c>
       <c r="O31" s="3">
         <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
@@ -9781,7 +9781,7 @@
       </c>
       <c r="P31" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>681.8149038461537</v>
+        <v>540.15837104072398</v>
       </c>
       <c r="Q31" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9789,11 +9789,11 @@
       </c>
       <c r="R31" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-6288.6828935185185</v>
+        <v>-5471.7361111111113</v>
       </c>
       <c r="S31" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>156.02430555555583</v>
       </c>
       <c r="T31" s="3">
         <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
@@ -9801,7 +9801,7 @@
       </c>
       <c r="U31" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>140.97028614767666</v>
+        <v>486.14253393665155</v>
       </c>
       <c r="V31" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9843,7 +9843,7 @@
         <v>460</v>
       </c>
       <c r="K32" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L32" s="10" t="str">
@@ -9852,7 +9852,7 @@
       </c>
       <c r="M32" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-8357.9870370370372</v>
+        <v>-7272.2222222222217</v>
       </c>
       <c r="N32" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -9864,7 +9864,7 @@
       </c>
       <c r="P32" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>670.10504201680658</v>
+        <v>501.57563025210078</v>
       </c>
       <c r="Q32" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9872,7 +9872,7 @@
       </c>
       <c r="R32" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-7940.0876851851845</v>
+        <v>-6908.6111111111113</v>
       </c>
       <c r="S32" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -9884,7 +9884,7 @@
       </c>
       <c r="U32" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>451.41806722689074</v>
       </c>
       <c r="V32" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9926,7 +9926,7 @@
         <v>460</v>
       </c>
       <c r="K33" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L33" s="10" t="str">
@@ -9935,7 +9935,7 @@
       </c>
       <c r="M33" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-10271.895833333336</v>
+        <v>-8937.5000000000018</v>
       </c>
       <c r="N33" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -9947,7 +9947,7 @@
       </c>
       <c r="P33" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>665.80821078431359</v>
+        <v>468.13725490196072</v>
       </c>
       <c r="Q33" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9955,7 +9955,7 @@
       </c>
       <c r="R33" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-9758.3010416666693</v>
+        <v>-8490.6250000000018</v>
       </c>
       <c r="S33" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="U33" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>421.3235294117647</v>
       </c>
       <c r="V33" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10009,7 +10009,7 @@
         <v>460</v>
       </c>
       <c r="K34" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L34" s="10" t="str">
@@ -10018,7 +10018,7 @@
       </c>
       <c r="M34" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-12361.392592592594</v>
+        <v>-10755.555555555558</v>
       </c>
       <c r="N34" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10030,7 +10030,7 @@
       </c>
       <c r="P34" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>667.53446691176464</v>
+        <v>438.87867647058818</v>
       </c>
       <c r="Q34" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10038,7 +10038,7 @@
       </c>
       <c r="R34" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-11743.322962962964</v>
+        <v>-10217.777777777779</v>
       </c>
       <c r="S34" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10050,7 +10050,7 @@
       </c>
       <c r="U34" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>394.99080882352939</v>
       </c>
       <c r="V34" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10092,7 +10092,7 @@
         <v>460</v>
       </c>
       <c r="K35" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L35" s="10" t="str">
@@ -10101,7 +10101,7 @@
       </c>
       <c r="M35" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-14626.477314814814</v>
+        <v>-12726.388888888889</v>
       </c>
       <c r="N35" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10113,7 +10113,7 @@
       </c>
       <c r="P35" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>674.22091262975778</v>
+        <v>413.06228373702419</v>
       </c>
       <c r="Q35" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10121,7 +10121,7 @@
       </c>
       <c r="R35" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-13895.153449074074</v>
+        <v>-12090.069444444445</v>
       </c>
       <c r="S35" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10133,7 +10133,7 @@
       </c>
       <c r="U35" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>371.75605536332176</v>
       </c>
       <c r="V35" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10175,7 +10175,7 @@
         <v>460</v>
       </c>
       <c r="K36" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L36" s="10" t="str">
@@ -10184,7 +10184,7 @@
       </c>
       <c r="M36" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-17067.149999999998</v>
+        <v>-14850</v>
       </c>
       <c r="N36" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10196,7 +10196,7 @@
       </c>
       <c r="P36" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>685.04084967320262</v>
+        <v>390.11437908496731</v>
       </c>
       <c r="Q36" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10204,7 +10204,7 @@
       </c>
       <c r="R36" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-16213.7925</v>
+        <v>-14107.5</v>
       </c>
       <c r="S36" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10216,7 +10216,7 @@
       </c>
       <c r="U36" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>351.10294117647055</v>
       </c>
       <c r="V36" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10258,7 +10258,7 @@
         <v>460</v>
       </c>
       <c r="K37" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L37" s="10" t="str">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="M37" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-19683.410648148147</v>
+        <v>-17126.388888888891</v>
       </c>
       <c r="N37" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="P37" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>699.34162151702787</v>
+        <v>369.5820433436532</v>
       </c>
       <c r="Q37" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10287,7 +10287,7 @@
       </c>
       <c r="R37" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-18699.24011574074</v>
+        <v>-16270.069444444445</v>
       </c>
       <c r="S37" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="U37" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>332.62383900928791</v>
       </c>
       <c r="V37" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10341,7 +10341,7 @@
         <v>460</v>
       </c>
       <c r="K38" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L38" s="10" t="str">
@@ -10350,7 +10350,7 @@
       </c>
       <c r="M38" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-22475.259259259255</v>
+        <v>-19555.555555555555</v>
       </c>
       <c r="N38" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10362,7 +10362,7 @@
       </c>
       <c r="P38" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>716.60110294117635</v>
+        <v>351.10294117647055</v>
       </c>
       <c r="Q38" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="R38" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-21351.496296296296</v>
+        <v>-18577.777777777777</v>
       </c>
       <c r="S38" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10382,7 +10382,7 @@
       </c>
       <c r="U38" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>315.99264705882354</v>
       </c>
       <c r="V38" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10424,7 +10424,7 @@
         <v>460</v>
       </c>
       <c r="K39" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L39" s="10" t="str">
@@ -10433,7 +10433,7 @@
       </c>
       <c r="M39" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-25442.695833333328</v>
+        <v>-22137.499999999996</v>
       </c>
       <c r="N39" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10445,7 +10445,7 @@
       </c>
       <c r="P39" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>736.3966211484593</v>
+        <v>334.38375350140052</v>
       </c>
       <c r="Q39" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10453,7 +10453,7 @@
       </c>
       <c r="R39" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-24170.56104166666</v>
+        <v>-21030.624999999996</v>
       </c>
       <c r="S39" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10465,7 +10465,7 @@
       </c>
       <c r="U39" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>300.94537815126051</v>
       </c>
       <c r="V39" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10507,7 +10507,7 @@
         <v>460</v>
       </c>
       <c r="K40" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L40" s="10" t="str">
@@ -10516,7 +10516,7 @@
       </c>
       <c r="M40" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-28585.720370370364</v>
+        <v>-24872.222222222219</v>
       </c>
       <c r="N40" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10528,7 +10528,7 @@
       </c>
       <c r="P40" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>758.38235294117646</v>
+        <v>319.18449197860957</v>
       </c>
       <c r="Q40" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10536,7 +10536,7 @@
       </c>
       <c r="R40" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-27156.434351851847</v>
+        <v>-23628.611111111106</v>
       </c>
       <c r="S40" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="U40" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>287.26604278074865</v>
       </c>
       <c r="V40" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10590,7 +10590,7 @@
         <v>460</v>
       </c>
       <c r="K41" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L41" s="10" t="str">
@@ -10599,7 +10599,7 @@
       </c>
       <c r="M41" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-31904.332870370374</v>
+        <v>-27759.722222222226</v>
       </c>
       <c r="N41" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10611,7 +10611,7 @@
       </c>
       <c r="P41" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>782.27261828644498</v>
+        <v>305.30690537084394</v>
       </c>
       <c r="Q41" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10619,7 +10619,7 @@
       </c>
       <c r="R41" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-30309.116226851856</v>
+        <v>-26371.736111111113</v>
       </c>
       <c r="S41" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10631,7 +10631,7 @@
       </c>
       <c r="U41" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>274.77621483375958</v>
       </c>
       <c r="V41" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10673,7 +10673,7 @@
         <v>460</v>
       </c>
       <c r="K42" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L42" s="10" t="str">
@@ -10682,7 +10682,7 @@
       </c>
       <c r="M42" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-35398.533333333333</v>
+        <v>-30800.000000000004</v>
       </c>
       <c r="N42" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="P42" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>807.82935049019602</v>
+        <v>292.58578431372547</v>
       </c>
       <c r="Q42" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="R42" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-33628.606666666667</v>
+        <v>-29260.000000000004</v>
       </c>
       <c r="S42" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10714,7 +10714,7 @@
       </c>
       <c r="U42" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>263.32720588235293</v>
       </c>
       <c r="V42" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>

</xml_diff>

<commit_message>
#12 fixed plus Fendt 611 LSA
</commit_message>
<xml_diff>
--- a/Documents/MotorNeu.xlsx
+++ b/Documents/MotorNeu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23190" yWindow="0" windowWidth="20400" windowHeight="9945"/>
+    <workbookView xWindow="24645" yWindow="0" windowWidth="20400" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate from Values" sheetId="3" r:id="rId1"/>
@@ -551,6 +551,39 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -1369,33 +1402,6 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1441,9 +1447,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1456,9 +1459,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1722,16 +1722,16 @@
                   <c:v>923.95510835913308</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>796.06627888149092</c:v>
+                  <c:v>868.97977941176464</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>478.62033819495952</c:v>
+                  <c:v>802.52100840336129</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>636.71088270018754</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>139.28050559066608</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1951,61 +1951,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>228.3518518518519</c:v>
+                  <c:v>240.37037037037044</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>669.57407407407413</c:v>
+                  <c:v>704.81481481481478</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>866.96296296296305</c:v>
+                  <c:v>912.59259259259272</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>905.66666666666674</c:v>
+                  <c:v>953.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>940.5</c:v>
+                  <c:v>990</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>972.43055555555554</c:v>
+                  <c:v>1023.6111111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>998.55555555555566</c:v>
+                  <c:v>1051.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1018.875</c:v>
+                  <c:v>1072.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1033.3888888888889</c:v>
+                  <c:v>1087.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1042.0972222222222</c:v>
+                  <c:v>1096.9444444444443</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1045</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>987.47702205882354</c:v>
+                  <c:v>1072.4929856811145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>929.39013840830444</c:v>
+                  <c:v>1032.6557093425604</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>877.75735294117646</c:v>
+                  <c:v>975.28594771241819</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>831.55959752321974</c:v>
+                  <c:v>923.95510835913308</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>716.45965099334182</c:v>
+                  <c:v>868.97977941176464</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>430.75830437546352</c:v>
+                  <c:v>802.52100840336129</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>636.71088270018754</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>139.28050559066608</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2068,8 +2068,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374297712"/>
-        <c:axId val="374295752"/>
+        <c:axId val="324524728"/>
+        <c:axId val="357168752"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2284,16 +2284,16 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>226.7330134615346</c:v>
+                  <c:v>247.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>143.13504564238789</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>199.48051948051949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>45.619834710743824</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
                   <c:v>0</c:v>
@@ -2513,61 +2513,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2519216598797756</c:v>
+                  <c:v>3.4230754314523959</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.141182858250929</c:v>
+                  <c:v>40.148613535000962</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.423951910025224</c:v>
+                  <c:v>90.972580957921295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.17961605584642</c:v>
+                  <c:v>108.61012216404887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120.54157068062827</c:v>
+                  <c:v>126.88586387434555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>138.48225712623619</c:v>
+                  <c:v>145.77079697498544</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>156.42294357184412</c:v>
+                  <c:v>164.65573007562537</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>174.11560209424087</c:v>
+                  <c:v>183.27958115183247</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>191.31220477021526</c:v>
+                  <c:v>201.38126817917399</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>207.76472367655614</c:v>
+                  <c:v>218.699709133217</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>223.22513089005241</c:v>
+                  <c:v>234.97382198952886</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>225</c:v>
+                  <c:v>244.37117663268117</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>225</c:v>
+                  <c:v>249.99999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>225</c:v>
+                  <c:v>249.99999999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>225</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>204.05971211538113</c:v>
+                  <c:v>247.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>128.8215410781491</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>199.48051948051949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>45.619834710743824</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
                   <c:v>0</c:v>
@@ -2630,11 +2630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374298104"/>
-        <c:axId val="374300064"/>
+        <c:axId val="276489232"/>
+        <c:axId val="357169136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374297712"/>
+        <c:axId val="324524728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -2738,13 +2738,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374295752"/>
+        <c:crossAx val="357168752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374295752"/>
+        <c:axId val="357168752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,12 +2846,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374297712"/>
+        <c:crossAx val="324524728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374300064"/>
+        <c:axId val="357169136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,12 +2894,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374298104"/>
+        <c:crossAx val="276489232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374298104"/>
+        <c:axId val="276489232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2909,7 +2909,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="374300064"/>
+        <c:crossAx val="357169136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3197,64 +3197,64 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>304.1749999999999</c:v>
+                  <c:v>283.04374999999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>289.7999999999999</c:v>
+                  <c:v>272.4222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>253.57499999999993</c:v>
+                  <c:v>245.3493055555555</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>227.7</c:v>
+                  <c:v>225.46388888888887</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.37499999999997</c:v>
+                  <c:v>220.43263888888887</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>216.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>212.17499999999998</c:v>
+                  <c:v>212.76597222222222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>209.3</c:v>
+                  <c:v>210.13055555555556</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>207.57499999999999</c:v>
+                  <c:v>208.29374999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>207</c:v>
+                  <c:v>207.25555555555556</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>207.01774691358025</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>207.63888888888889</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>209.55555555555554</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>212.75</c:v>
+                  <c:v>209.14737654320987</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>217.22222222222223</c:v>
+                  <c:v>211.54320987654322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>222.97222222222223</c:v>
+                  <c:v>214.82638888888889</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>218.99691358024691</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>224.05478395061729</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>244.75450687929043</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>313.46409493927865</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>460</c:v>
+                  <c:v>262.03842321622847</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>460</c:v>
+                  <c:v>411.23669051775721</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>460</c:v>
@@ -3317,11 +3317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374296144"/>
-        <c:axId val="374300456"/>
+        <c:axId val="276490800"/>
+        <c:axId val="276490016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374296144"/>
+        <c:axId val="276490800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -3425,13 +3425,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374300456"/>
+        <c:crossAx val="276490016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374300456"/>
+        <c:axId val="276490016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3529,7 +3529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374296144"/>
+        <c:crossAx val="276490800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -3845,11 +3845,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374300848"/>
-        <c:axId val="374296928"/>
+        <c:axId val="276490408"/>
+        <c:axId val="276491192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374300848"/>
+        <c:axId val="276490408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2700"/>
@@ -3908,12 +3908,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374296928"/>
+        <c:crossAx val="276491192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374296928"/>
+        <c:axId val="276491192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +3970,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374300848"/>
+        <c:crossAx val="276490408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4231,11 +4231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374231496"/>
-        <c:axId val="374237376"/>
+        <c:axId val="324870288"/>
+        <c:axId val="324875384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374231496"/>
+        <c:axId val="324870288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2400"/>
@@ -4294,12 +4294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374237376"/>
+        <c:crossAx val="324875384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374237376"/>
+        <c:axId val="324875384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374231496"/>
+        <c:crossAx val="324870288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6770,89 +6770,65 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A6:V42" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
-  <autoFilter ref="A6:V42">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
-    <filterColumn colId="15" hiddenButton="1"/>
-    <filterColumn colId="16" hiddenButton="1"/>
-    <filterColumn colId="17" hiddenButton="1"/>
-    <filterColumn colId="18" hiddenButton="1"/>
-    <filterColumn colId="19" hiddenButton="1"/>
-    <filterColumn colId="20" hiddenButton="1"/>
-    <filterColumn colId="21" hiddenButton="1"/>
-  </autoFilter>
   <tableColumns count="22">
     <tableColumn id="1" name="rpm" dataDxfId="70"/>
-    <tableColumn id="7" name="rawData" dataDxfId="69">
-      <calculatedColumnFormula>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</calculatedColumnFormula>
+    <tableColumn id="7" name="rawData" dataDxfId="2">
+      <calculatedColumnFormula>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="manualData" dataDxfId="68"/>
-    <tableColumn id="12" name="rawDataEco" dataDxfId="67">
-      <calculatedColumnFormula>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</calculatedColumnFormula>
+    <tableColumn id="9" name="manualData" dataDxfId="69"/>
+    <tableColumn id="12" name="rawDataEco" dataDxfId="1">
+      <calculatedColumnFormula>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="manDataEco" dataDxfId="66"/>
-    <tableColumn id="4" name="motor" dataDxfId="65">
+    <tableColumn id="11" name="manDataEco" dataDxfId="68"/>
+    <tableColumn id="4" name="motor" dataDxfId="67">
       <calculatedColumnFormula>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="motorEco" dataDxfId="64">
+    <tableColumn id="14" name="motorEco" dataDxfId="66">
       <calculatedColumnFormula>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="63">
+    <tableColumn id="3" name="ps" dataDxfId="65">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="psEco" dataDxfId="62">
+    <tableColumn id="13" name="psEco" dataDxfId="64">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="61">
+    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="63">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="xml" dataDxfId="0">
-      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="60">
+    <tableColumn id="8" name="xml2" dataDxfId="62">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="t1" dataDxfId="59">
+    <tableColumn id="15" name="t1" dataDxfId="11">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="t2" dataDxfId="58">
+    <tableColumn id="18" name="t2" dataDxfId="9">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="t3" dataDxfId="57">
-      <calculatedColumnFormula>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</calculatedColumnFormula>
+    <tableColumn id="19" name="t3" dataDxfId="8">
+      <calculatedColumnFormula>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="t4" dataDxfId="56">
+    <tableColumn id="16" name="t4" dataDxfId="7">
       <calculatedColumnFormula>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="t5" dataDxfId="55">
+    <tableColumn id="17" name="t5" dataDxfId="6">
       <calculatedColumnFormula>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="t1E" dataDxfId="54">
+    <tableColumn id="21" name="t1E" dataDxfId="5">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="t2E" dataDxfId="53">
+    <tableColumn id="22" name="t2E" dataDxfId="4">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="t3E" dataDxfId="52">
-      <calculatedColumnFormula>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</calculatedColumnFormula>
+    <tableColumn id="23" name="t3E" dataDxfId="3">
+      <calculatedColumnFormula>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="t4E" dataDxfId="51">
+    <tableColumn id="24" name="t4E" dataDxfId="10">
       <calculatedColumnFormula>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="t5E" dataDxfId="50">
+    <tableColumn id="25" name="t5E" dataDxfId="61">
       <calculatedColumnFormula>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6861,7 +6837,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="60">
   <autoFilter ref="A1:Y2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6886,45 +6862,45 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="25">
-    <tableColumn id="10" name="maxPRpm" dataDxfId="48"/>
-    <tableColumn id="14" name="maxPS" dataDxfId="47"/>
-    <tableColumn id="19" name="maxPSEco" dataDxfId="46">
+    <tableColumn id="10" name="maxPRpm" dataDxfId="59"/>
+    <tableColumn id="14" name="maxPS" dataDxfId="58"/>
+    <tableColumn id="19" name="maxPSEco" dataDxfId="57">
       <calculatedColumnFormula>Table36[maxPsEcoRate]*Table36[maxPS]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="ratedRpm"/>
     <tableColumn id="3" name="PS"/>
-    <tableColumn id="20" name="PSEco" dataDxfId="45">
-      <calculatedColumnFormula>Table36[PSEcoRate]*Table36[PS]</calculatedColumnFormula>
+    <tableColumn id="20" name="PSEco" dataDxfId="56">
+      <calculatedColumnFormula>Table36[PS]*Table36[PSEcoRate]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="maxTRpm1" dataDxfId="44"/>
-    <tableColumn id="4" name="maxTRpm" dataDxfId="43"/>
-    <tableColumn id="5" name="maxT" dataDxfId="42"/>
-    <tableColumn id="21" name="maxTEco" dataDxfId="41">
+    <tableColumn id="12" name="maxTRpm1" dataDxfId="55"/>
+    <tableColumn id="4" name="maxTRpm" dataDxfId="54"/>
+    <tableColumn id="5" name="maxT" dataDxfId="53"/>
+    <tableColumn id="21" name="maxTEco" dataDxfId="52">
       <calculatedColumnFormula>Table36[NmEcoRate]*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="idleRpm"/>
     <tableColumn id="7" name="idleRatio" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="fadeOut" dataDxfId="40"/>
-    <tableColumn id="15" name="linearDown" dataDxfId="39"/>
-    <tableColumn id="25" name="fadeOutExp" dataDxfId="38"/>
-    <tableColumn id="22" name="Efficiency" dataDxfId="37"/>
-    <tableColumn id="16" name="Factor" dataDxfId="36"/>
-    <tableColumn id="13" name="fuelMinRate" dataDxfId="35"/>
-    <tableColumn id="18" name="fuelRatedRate" dataDxfId="34">
+    <tableColumn id="11" name="fadeOut" dataDxfId="51"/>
+    <tableColumn id="15" name="linearDown" dataDxfId="50"/>
+    <tableColumn id="25" name="fadeOutExp" dataDxfId="49"/>
+    <tableColumn id="22" name="Efficiency" dataDxfId="48"/>
+    <tableColumn id="16" name="Factor" dataDxfId="47"/>
+    <tableColumn id="13" name="fuelMinRate" dataDxfId="46"/>
+    <tableColumn id="18" name="fuelRatedRate" dataDxfId="45">
       <calculatedColumnFormula>Table36[fuelMinRate]/0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="fuelMinRpm" dataDxfId="33">
+    <tableColumn id="9" name="fuelMinRpm" dataDxfId="44">
       <calculatedColumnFormula>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="fuelIdleRate" dataDxfId="32">
+    <tableColumn id="17" name="fuelIdleRate" dataDxfId="43">
       <calculatedColumnFormula>0.94*Table36[fuelRatedRate]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="normRpm" dataDxfId="31">
+    <tableColumn id="1" name="normRpm" dataDxfId="42">
       <calculatedColumnFormula>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PSEcoRate" dataDxfId="30"/>
+    <tableColumn id="8" name="PSEcoRate" dataDxfId="41"/>
     <tableColumn id="23" name="NmEcoRate"/>
-    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="29">
+    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="40">
       <calculatedColumnFormula>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6933,7 +6909,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:S4" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:S4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A3:S4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6952,61 +6928,61 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" name="f1" dataDxfId="26">
+    <tableColumn id="1" name="f1" dataDxfId="37">
       <calculatedColumnFormula>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="f2" dataDxfId="25">
+    <tableColumn id="2" name="f2" dataDxfId="36">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="f3" dataDxfId="24">
+    <tableColumn id="5" name="f3" dataDxfId="35">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="f4" dataDxfId="23">
+    <tableColumn id="6" name="f4" dataDxfId="34">
       <calculatedColumnFormula>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Nm" dataDxfId="22">
+    <tableColumn id="3" name="Nm" dataDxfId="33">
       <calculatedColumnFormula>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Nm2" dataDxfId="21">
+    <tableColumn id="4" name="Nm2" dataDxfId="32">
       <calculatedColumnFormula>Table36[PS]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Anfahrmoment" dataDxfId="20" dataCellStyle="Percent">
+    <tableColumn id="7" name="Anfahrmoment" dataDxfId="31" dataCellStyle="Percent">
       <calculatedColumnFormula>Table7[Nm1000]/Table7[Nm2Eco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="AnstiegE" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="17" name="AnstiegE" dataDxfId="30" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxTEco]/Table7[Nm2Eco]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Anstieg" dataDxfId="18" dataCellStyle="Percent">
+    <tableColumn id="14" name="Anstieg" dataDxfId="29" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxT]/Table7[Nm2]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Abfall" dataDxfId="17" dataCellStyle="Percent">
+    <tableColumn id="15" name="Abfall" dataDxfId="28" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table36[maxTRpm]/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Nm1000" dataDxfId="16" dataCellStyle="Percent">
+    <tableColumn id="16" name="Nm1000" dataDxfId="27" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NmEco" dataDxfId="15">
+    <tableColumn id="8" name="NmEco" dataDxfId="26">
       <calculatedColumnFormula>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Nm2Eco" dataDxfId="14">
+    <tableColumn id="9" name="Nm2Eco" dataDxfId="25">
       <calculatedColumnFormula>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="f2Eco" dataDxfId="13">
+    <tableColumn id="12" name="f2Eco" dataDxfId="24">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="f3Eco" dataDxfId="12">
+    <tableColumn id="10" name="f3Eco" dataDxfId="23">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="f4Eco" dataDxfId="11">
+    <tableColumn id="11" name="f4Eco" dataDxfId="22">
       <calculatedColumnFormula>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="idleT" dataDxfId="10">
+    <tableColumn id="13" name="idleT" dataDxfId="21">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="idleTEco" dataDxfId="9">
+    <tableColumn id="19" name="idleTEco" dataDxfId="20">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="xmlComment" dataDxfId="8">
+    <tableColumn id="21" name="xmlComment" dataDxfId="19">
       <calculatedColumnFormula>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7023,17 +6999,17 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$A$22*Table1[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="7">
+    <tableColumn id="6" name="kw_pto" dataDxfId="18">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="6">
+    <tableColumn id="3" name="ps" dataDxfId="17">
       <calculatedColumnFormula>Table1[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor"/>
-    <tableColumn id="5" name="xml" dataDxfId="5">
+    <tableColumn id="5" name="xml" dataDxfId="16">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table1[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table1[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="4">
+    <tableColumn id="8" name="xml2" dataDxfId="15">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table1[[#This Row],[rpm]]/Table3[ratedRpm],3),""" torque=""",ROUND(Table1[[#This Row],[motor]]/MAX(Table1[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7067,16 +7043,16 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$I$2*Table13[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="3">
+    <tableColumn id="6" name="kw_pto" dataDxfId="14">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="2">
+    <tableColumn id="3" name="ps" dataDxfId="13">
       <calculatedColumnFormula>Table13[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor">
       <calculatedColumnFormula>C2/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="1">
+    <tableColumn id="5" name="xml" dataDxfId="12">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table13[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table13[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7350,17 +7326,17 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -7452,17 +7428,17 @@
       </c>
       <c r="C2" s="18">
         <f>Table36[maxPsEcoRate]*Table36[maxPS]</f>
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="D2" s="7">
-        <v>1900</v>
+        <v>2100</v>
       </c>
       <c r="E2" s="8">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F2" s="19">
-        <f>Table36[PSEcoRate]*Table36[PS]</f>
-        <v>225</v>
+        <f>Table36[PS]*Table36[PSEcoRate]</f>
+        <v>240</v>
       </c>
       <c r="G2" s="13">
         <v>1500</v>
@@ -7475,7 +7451,7 @@
       </c>
       <c r="J2" s="18">
         <f>Table36[NmEcoRate]*Table36[maxT]</f>
-        <v>1045</v>
+        <v>1100</v>
       </c>
       <c r="K2" s="7">
         <v>900</v>
@@ -7484,13 +7460,13 @@
         <v>0.9</v>
       </c>
       <c r="M2" s="9">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="N2" s="13">
         <v>0.5</v>
       </c>
       <c r="O2" s="14">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="P2" s="14">
         <v>0.94</v>
@@ -7507,7 +7483,7 @@
       </c>
       <c r="T2" s="17">
         <f>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</f>
-        <v>1300</v>
+        <v>1380</v>
       </c>
       <c r="U2" s="19">
         <f>0.94*Table36[fuelRatedRate]</f>
@@ -7515,17 +7491,17 @@
       </c>
       <c r="V2" s="16">
         <f>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</f>
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="W2" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="X2" s="9">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="29">
         <f>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -7602,7 +7578,7 @@
       </c>
       <c r="D4" s="12">
         <f>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>0</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="E4" s="12">
         <f>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</f>
@@ -7610,47 +7586,47 @@
       </c>
       <c r="F4" s="12">
         <f>Table36[PS]/1.36*9550/Table36[ratedRpm]</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="G4" s="23">
         <f>Table7[Nm1000]/Table7[Nm2Eco]</f>
-        <v>1.1694057268437723</v>
+        <v>1.2754944735311229</v>
       </c>
       <c r="H4" s="24">
         <f>Table36[maxTEco]/Table7[Nm2Eco]-1</f>
-        <v>0.25667481093659106</v>
+        <v>0.37068062827225146</v>
       </c>
       <c r="I4" s="24">
         <f>Table36[maxT]/Table7[Nm2]-1</f>
-        <v>0.19053403141361258</v>
+        <v>0.37068062827225146</v>
       </c>
       <c r="J4" s="25">
         <f>1-Table36[maxTRpm]/Table36[ratedRpm]</f>
-        <v>0.21052631578947367</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="K4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</f>
-        <v>972.43055555555554</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="L4" s="12">
         <f>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</f>
-        <v>831.55959752321974</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="M4" s="12">
         <f>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="N4" s="12">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>5.1062297243248866E-4</v>
+        <v>4.0010202645651574E-4</v>
       </c>
       <c r="O4" s="12">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.2765574310812216E-6</v>
+        <v>1.0002550661412894E-6</v>
       </c>
       <c r="P4" s="12">
         <f>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>0</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</f>
@@ -7658,14 +7634,14 @@
       </c>
       <c r="R4" s="12">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</f>
-        <v>940.5</v>
+        <v>990</v>
       </c>
       <c r="S4" s="12" t="str">
         <f>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" s="4" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -7738,12 +7714,12 @@
         <v>0</v>
       </c>
       <c r="B7" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E7" s="20"/>
@@ -7765,15 +7741,15 @@
       </c>
       <c r="J7" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>304.1749999999999</v>
+        <v>283.04374999999993</v>
       </c>
       <c r="K7" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
       </c>
       <c r="L7" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(225) | 1900: 250(225) | 1500..1500: 1100(1045) | 90 | 0.5 | 300 | 1.8 | 2000 | 1300: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
       </c>
       <c r="M7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -7783,17 +7759,17 @@
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
         <v>412.50000000000011</v>
       </c>
-      <c r="O7" s="3" t="e">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>#DIV/0!</v>
+      <c r="O7" s="3">
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
+        <v>192.26852747677987</v>
       </c>
       <c r="P7" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1755514.7058823528</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -7801,19 +7777,19 @@
       </c>
       <c r="S7" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>391.87500000000011</v>
-      </c>
-      <c r="T7" s="3" t="e">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>#DIV/0!</v>
+        <v>412.50000000000011</v>
+      </c>
+      <c r="T7" s="3">
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>192.26852747677987</v>
       </c>
       <c r="U7" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1579963.2352941176</v>
+        <v>0</v>
       </c>
       <c r="V7" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -7821,13 +7797,13 @@
         <v>100</v>
       </c>
       <c r="B8" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>240.37037037037044</v>
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>228.3518518518519</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>240.37037037037044</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="3">
@@ -7836,7 +7812,7 @@
       </c>
       <c r="G8" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>228.3518518518519</v>
+        <v>240.37037037037044</v>
       </c>
       <c r="H8" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -7844,19 +7820,19 @@
       </c>
       <c r="I8" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>3.2519216598797756</v>
+        <v>3.4230754314523959</v>
       </c>
       <c r="J8" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>289.7999999999999</v>
+        <v>272.4222222222221</v>
       </c>
       <c r="K8" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="240" motorTorqueEco="228" fuelUsageRatio="289.8"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="240" fuelUsageRatio="272.4"/&gt;</v>
       </c>
       <c r="L8" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.05" torque="0.219"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.045" torque="0.219"/&gt;</v>
       </c>
       <c r="M8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -7867,36 +7843,36 @@
         <v>501.11111111111131</v>
       </c>
       <c r="O8" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>329.80359907120709</v>
       </c>
       <c r="P8" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>17555.147058823528</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>197.38888888888894</v>
+        <v>207.77777777777783</v>
       </c>
       <c r="S8" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>476.05555555555571</v>
+        <v>501.11111111111131</v>
       </c>
       <c r="T8" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>111.19823916408642</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>329.80359907120709</v>
       </c>
       <c r="U8" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>15799.632352941177</v>
+        <v>0</v>
       </c>
       <c r="V8" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -7904,13 +7880,13 @@
         <v>400</v>
       </c>
       <c r="B9" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>704.81481481481478</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>669.57407407407413</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>704.81481481481478</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="3">
@@ -7919,7 +7895,7 @@
       </c>
       <c r="G9" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>669.57407407407413</v>
+        <v>704.81481481481478</v>
       </c>
       <c r="H9" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -7927,19 +7903,19 @@
       </c>
       <c r="I9" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>38.141182858250929</v>
+        <v>40.148613535000962</v>
       </c>
       <c r="J9" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>253.57499999999993</v>
+        <v>245.3493055555555</v>
       </c>
       <c r="K9" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="705" motorTorqueEco="670" fuelUsageRatio="253.6"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="705" fuelUsageRatio="245.3"/&gt;</v>
       </c>
       <c r="L9" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.2" torque="0.641"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.182" torque="0.641"/&gt;</v>
       </c>
       <c r="M9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -7950,36 +7926,36 @@
         <v>730.27777777777783</v>
       </c>
       <c r="O9" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>676.39197948916387</v>
       </c>
       <c r="P9" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>4388.786764705882</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>650.22222222222217</v>
+        <v>684.44444444444446</v>
       </c>
       <c r="S9" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>693.76388888888903</v>
+        <v>730.27777777777783</v>
       </c>
       <c r="T9" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>531.4090315402475</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>676.39197948916387</v>
       </c>
       <c r="U9" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>3949.9080882352941</v>
+        <v>0</v>
       </c>
       <c r="V9" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -7987,13 +7963,13 @@
         <v>700</v>
       </c>
       <c r="B10" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>912.59259259259272</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>866.96296296296305</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>912.59259259259272</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="3">
@@ -8002,7 +7978,7 @@
       </c>
       <c r="G10" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>866.96296296296305</v>
+        <v>912.59259259259272</v>
       </c>
       <c r="H10" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8010,19 +7986,19 @@
       </c>
       <c r="I10" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>86.423951910025224</v>
+        <v>90.972580957921295</v>
       </c>
       <c r="J10" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>227.7</v>
+        <v>225.46388888888887</v>
       </c>
       <c r="K10" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="913" motorTorqueEco="867" fuelUsageRatio="227.7"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="913" fuelUsageRatio="225.5"/&gt;</v>
       </c>
       <c r="L10" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.35" torque="0.83"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.318" torque="0.83"/&gt;</v>
       </c>
       <c r="M10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8033,36 +8009,36 @@
         <v>904.44444444444457</v>
       </c>
       <c r="O10" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>923.95510835913308</v>
       </c>
       <c r="P10" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2507.8781512605042</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>894.05555555555554</v>
+        <v>941.11111111111109</v>
       </c>
       <c r="S10" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>859.22222222222229</v>
+        <v>904.44444444444457</v>
       </c>
       <c r="T10" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>831.55959752321985</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>923.95510835913308</v>
       </c>
       <c r="U10" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2257.0903361344535</v>
+        <v>0</v>
       </c>
       <c r="V10" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -8070,13 +8046,13 @@
         <v>800</v>
       </c>
       <c r="B11" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>953.33333333333337</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>905.66666666666674</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>953.33333333333337</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="3">
@@ -8085,7 +8061,7 @@
       </c>
       <c r="G11" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>905.66666666666674</v>
+        <v>953.33333333333337</v>
       </c>
       <c r="H11" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8093,19 +8069,19 @@
       </c>
       <c r="I11" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>103.17961605584642</v>
+        <v>108.61012216404887</v>
       </c>
       <c r="J11" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>221.37499999999997</v>
+        <v>220.43263888888887</v>
       </c>
       <c r="K11" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="953" motorTorqueEco="906" fuelUsageRatio="221.4"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="953" fuelUsageRatio="220.4"/&gt;</v>
       </c>
       <c r="L11" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.4" torque="0.867"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.364" torque="0.867"/&gt;</v>
       </c>
       <c r="M11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8116,36 +8092,36 @@
         <v>950.27777777777783</v>
       </c>
       <c r="O11" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>984.47053986068101</v>
       </c>
       <c r="P11" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>2194.393382352941</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>928.8888888888888</v>
+        <v>977.77777777777771</v>
       </c>
       <c r="S11" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>902.76388888888891</v>
+        <v>950.27777777777783</v>
       </c>
       <c r="T11" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>904.9297358746129</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>984.47053986068101</v>
       </c>
       <c r="U11" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1974.9540441176471</v>
+        <v>0</v>
       </c>
       <c r="V11" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -8153,13 +8129,13 @@
         <v>900</v>
       </c>
       <c r="B12" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>990</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>940.5</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>990</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="3">
@@ -8168,7 +8144,7 @@
       </c>
       <c r="G12" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>940.5</v>
+        <v>990</v>
       </c>
       <c r="H12" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8176,19 +8152,19 @@
       </c>
       <c r="I12" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>120.54157068062827</v>
+        <v>126.88586387434555</v>
       </c>
       <c r="J12" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
         <v>216.2</v>
       </c>
       <c r="K12" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="990" motorTorqueEco="941" fuelUsageRatio="216.2"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="990" fuelUsageRatio="216.2"/&gt;</v>
       </c>
       <c r="L12" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.45" torque="0.9"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.409" torque="0.9"/&gt;</v>
       </c>
       <c r="M12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8199,36 +8175,36 @@
         <v>990</v>
       </c>
       <c r="O12" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1033.9831656346751</v>
       </c>
       <c r="P12" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1950.5718954248364</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>940.5</v>
+        <v>990</v>
       </c>
       <c r="S12" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>940.5</v>
+        <v>990</v>
       </c>
       <c r="T12" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>964.95984907120737</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1033.9831656346751</v>
       </c>
       <c r="U12" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1755.5147058823529</v>
+        <v>0</v>
       </c>
       <c r="V12" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -8236,13 +8212,13 @@
         <v>1000</v>
       </c>
       <c r="B13" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1023.6111111111111</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>972.43055555555554</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1023.6111111111111</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="3">
@@ -8251,7 +8227,7 @@
       </c>
       <c r="G13" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>972.43055555555554</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="H13" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8259,19 +8235,19 @@
       </c>
       <c r="I13" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>138.48225712623619</v>
+        <v>145.77079697498544</v>
       </c>
       <c r="J13" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>212.17499999999998</v>
+        <v>212.76597222222222</v>
       </c>
       <c r="K13" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1024" motorTorqueEco="972" fuelUsageRatio="212.2"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1024" fuelUsageRatio="212.8"/&gt;</v>
       </c>
       <c r="L13" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="0.931"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.455" torque="0.931"/&gt;</v>
       </c>
       <c r="M13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8282,36 +8258,36 @@
         <v>1023.6111111111111</v>
       </c>
       <c r="O13" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1072.4929856811145</v>
       </c>
       <c r="P13" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1755.5147058823527</v>
+        <v>333.54779411764702</v>
       </c>
       <c r="Q13" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>928.8888888888888</v>
+        <v>977.77777777777771</v>
       </c>
       <c r="S13" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>972.43055555555554</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="T13" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1011.6499371130031</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1072.4929856811145</v>
       </c>
       <c r="U13" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1579.9632352941176</v>
+        <v>333.54779411764702</v>
       </c>
       <c r="V13" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -8319,13 +8295,13 @@
         <v>1100</v>
       </c>
       <c r="B14" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1051.1111111111111</v>
       </c>
       <c r="C14" s="21"/>
       <c r="D14" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>998.55555555555566</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1051.1111111111111</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="3">
@@ -8334,7 +8310,7 @@
       </c>
       <c r="G14" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>998.55555555555566</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="H14" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8342,19 +8318,19 @@
       </c>
       <c r="I14" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>156.42294357184412</v>
+        <v>164.65573007562537</v>
       </c>
       <c r="J14" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>209.3</v>
+        <v>210.13055555555556</v>
       </c>
       <c r="K14" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1051" motorTorqueEco="999" fuelUsageRatio="209.3"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1051" fuelUsageRatio="210.1"/&gt;</v>
       </c>
       <c r="L14" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.55" torque="0.956"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="0.956"/&gt;</v>
       </c>
       <c r="M14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8365,36 +8341,36 @@
         <v>1051.1111111111111</v>
       </c>
       <c r="O14" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1100</v>
       </c>
       <c r="P14" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1595.922459893048</v>
+        <v>574.5320855614973</v>
       </c>
       <c r="Q14" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>894.05555555555554</v>
+        <v>941.11111111111109</v>
       </c>
       <c r="S14" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>998.55555555555566</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="T14" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1045</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1100</v>
       </c>
       <c r="U14" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1436.3302139037432</v>
+        <v>574.5320855614973</v>
       </c>
       <c r="V14" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -8402,13 +8378,13 @@
         <v>1200</v>
       </c>
       <c r="B15" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1072.5</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1018.875</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1072.5</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="3">
@@ -8417,7 +8393,7 @@
       </c>
       <c r="G15" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1018.875</v>
+        <v>1072.5</v>
       </c>
       <c r="H15" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8425,19 +8401,19 @@
       </c>
       <c r="I15" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>174.11560209424087</v>
+        <v>183.27958115183247</v>
       </c>
       <c r="J15" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.57499999999999</v>
+        <v>208.29374999999999</v>
       </c>
       <c r="K15" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1073" motorTorqueEco="1019" fuelUsageRatio="207.6"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1073" fuelUsageRatio="208.3"/&gt;</v>
       </c>
       <c r="L15" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.6" torque="0.975"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.545" torque="0.975"/&gt;</v>
       </c>
       <c r="M15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8448,36 +8424,36 @@
         <v>1072.5</v>
       </c>
       <c r="O15" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1116.5042085913312</v>
       </c>
       <c r="P15" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1462.9289215686274</v>
+        <v>746.09375</v>
       </c>
       <c r="Q15" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>836.00000000000011</v>
+        <v>880.00000000000011</v>
       </c>
       <c r="S15" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1018.875</v>
+        <v>1072.5</v>
       </c>
       <c r="T15" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1065.010037732198</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1116.5042085913312</v>
       </c>
       <c r="U15" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1316.6360294117646</v>
+        <v>746.09375</v>
       </c>
       <c r="V15" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -8485,13 +8461,13 @@
         <v>1300</v>
       </c>
       <c r="B16" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1087.7777777777778</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1033.3888888888889</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1087.7777777777778</v>
       </c>
       <c r="E16" s="21"/>
       <c r="F16" s="3">
@@ -8500,7 +8476,7 @@
       </c>
       <c r="G16" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1033.3888888888889</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="H16" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8508,19 +8484,19 @@
       </c>
       <c r="I16" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>191.31220477021526</v>
+        <v>201.38126817917399</v>
       </c>
       <c r="J16" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207</v>
+        <v>207.25555555555556</v>
       </c>
       <c r="K16" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1088" motorTorqueEco="1033" fuelUsageRatio="207"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1088" fuelUsageRatio="207.3"/&gt;</v>
       </c>
       <c r="L16" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.65" torque="0.989"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.591" torque="0.989"/&gt;</v>
       </c>
       <c r="M16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8531,36 +8507,36 @@
         <v>1087.7777777777778</v>
       </c>
       <c r="O16" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1122.0056114551082</v>
       </c>
       <c r="P16" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1350.3959276018097</v>
+        <v>864.25339366515834</v>
       </c>
       <c r="Q16" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>754.72222222222229</v>
+        <v>794.44444444444446</v>
       </c>
       <c r="S16" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1033.3888888888889</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="T16" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1071.6800503095974</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1122.0056114551082</v>
       </c>
       <c r="U16" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1215.356334841629</v>
+        <v>864.25339366515834</v>
       </c>
       <c r="V16" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -8568,13 +8544,13 @@
         <v>1400</v>
       </c>
       <c r="B17" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1096.9444444444443</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1042.0972222222222</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1096.9444444444443</v>
       </c>
       <c r="E17" s="21"/>
       <c r="F17" s="3">
@@ -8583,7 +8559,7 @@
       </c>
       <c r="G17" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1042.0972222222222</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="H17" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8591,19 +8567,19 @@
       </c>
       <c r="I17" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>207.76472367655614</v>
+        <v>218.699709133217</v>
       </c>
       <c r="J17" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.63888888888889</v>
+        <v>207.01774691358025</v>
       </c>
       <c r="K17" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1097" motorTorqueEco="1042" fuelUsageRatio="207.6"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1097" fuelUsageRatio="207"/&gt;</v>
       </c>
       <c r="L17" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.7" torque="0.997"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.636" torque="0.997"/&gt;</v>
       </c>
       <c r="M17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8614,36 +8590,36 @@
         <v>1096.9444444444443</v>
       </c>
       <c r="O17" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1116.5042085913312</v>
       </c>
       <c r="P17" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1253.9390756302521</v>
+        <v>940.45430672268901</v>
       </c>
       <c r="Q17" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>650.22222222222217</v>
+        <v>684.44444444444446</v>
       </c>
       <c r="S17" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1042.0972222222222</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="T17" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1065.010037732198</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1116.5042085913312</v>
       </c>
       <c r="U17" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1128.5451680672268</v>
+        <v>940.45430672268901</v>
       </c>
       <c r="V17" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -8651,13 +8627,13 @@
         <v>1500</v>
       </c>
       <c r="B18" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1100</v>
       </c>
       <c r="C18" s="21"/>
       <c r="D18" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>1045</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1100</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="3">
@@ -8666,7 +8642,7 @@
       </c>
       <c r="G18" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1045</v>
+        <v>1100</v>
       </c>
       <c r="H18" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8674,19 +8650,19 @@
       </c>
       <c r="I18" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>223.22513089005241</v>
+        <v>234.97382198952886</v>
       </c>
       <c r="J18" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>209.55555555555554</v>
+        <v>207.63888888888889</v>
       </c>
       <c r="K18" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1100" motorTorqueEco="1045" fuelUsageRatio="209.6"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1100" fuelUsageRatio="207.6"/&gt;</v>
       </c>
       <c r="L18" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.75" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.682" torque="1"/&gt;</v>
       </c>
       <c r="M18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8697,36 +8673,36 @@
         <v>1100</v>
       </c>
       <c r="O18" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1100</v>
       </c>
       <c r="P18" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1170.3431372549019</v>
+        <v>983.08823529411757</v>
       </c>
       <c r="Q18" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>522.49999999999989</v>
+        <v>549.99999999999989</v>
       </c>
       <c r="S18" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1045</v>
+        <v>1100</v>
       </c>
       <c r="T18" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>1045</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1100</v>
       </c>
       <c r="U18" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1053.3088235294117</v>
+        <v>983.08823529411757</v>
       </c>
       <c r="V18" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -8734,13 +8710,13 @@
         <v>1600</v>
       </c>
       <c r="B19" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1072.4929856811145</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>987.47702205882354</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1072.4929856811145</v>
       </c>
       <c r="E19" s="21"/>
       <c r="F19" s="3">
@@ -8749,7 +8725,7 @@
       </c>
       <c r="G19" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>987.47702205882354</v>
+        <v>1072.4929856811145</v>
       </c>
       <c r="H19" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8757,19 +8733,19 @@
       </c>
       <c r="I19" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>225</v>
+        <v>244.37117663268117</v>
       </c>
       <c r="J19" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>212.75</v>
+        <v>209.14737654320987</v>
       </c>
       <c r="K19" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1072" motorTorqueEco="987" fuelUsageRatio="212.8"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1072" fuelUsageRatio="209.1"/&gt;</v>
       </c>
       <c r="L19" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.8" torque="0.975"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.727" torque="0.975"/&gt;</v>
       </c>
       <c r="M19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8780,36 +8756,36 @@
         <v>1096.9444444444443</v>
       </c>
       <c r="O19" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>1072.4929856811145</v>
       </c>
       <c r="P19" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1097.1966911764705</v>
+        <v>998.44898897058829</v>
       </c>
       <c r="Q19" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>371.55555555555577</v>
+        <v>391.11111111111131</v>
       </c>
       <c r="S19" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1042.0972222222222</v>
+        <v>1096.9444444444443</v>
       </c>
       <c r="T19" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>987.47702205882354</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1072.4929856811145</v>
       </c>
       <c r="U19" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>987.47702205882354</v>
+        <v>998.44898897058829</v>
       </c>
       <c r="V19" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -8817,13 +8793,13 @@
         <v>1700</v>
       </c>
       <c r="B20" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>1032.6557093425604</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>929.39013840830444</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>1032.6557093425604</v>
       </c>
       <c r="E20" s="21"/>
       <c r="F20" s="3">
@@ -8832,7 +8808,7 @@
       </c>
       <c r="G20" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>929.39013840830444</v>
+        <v>1032.6557093425604</v>
       </c>
       <c r="H20" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8840,19 +8816,19 @@
       </c>
       <c r="I20" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>225</v>
+        <v>249.99999999999994</v>
       </c>
       <c r="J20" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>217.22222222222223</v>
+        <v>211.54320987654322</v>
       </c>
       <c r="K20" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1033" motorTorqueEco="929" fuelUsageRatio="217.2"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1033" fuelUsageRatio="211.5"/&gt;</v>
       </c>
       <c r="L20" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.85" torque="0.939"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.773" torque="0.939"/&gt;</v>
       </c>
       <c r="M20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8863,36 +8839,36 @@
         <v>1087.7777777777778</v>
       </c>
       <c r="O20" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>1032.6557093425604</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
+        <v>1033.9831656346748</v>
       </c>
       <c r="P20" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>1032.6557093425604</v>
+        <v>991.34948096885807</v>
       </c>
       <c r="Q20" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>197.38888888888894</v>
+        <v>207.77777777777783</v>
       </c>
       <c r="S20" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1033.3888888888889</v>
+        <v>1087.7777777777778</v>
       </c>
       <c r="T20" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>929.39013840830444</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>1033.9831656346748</v>
       </c>
       <c r="U20" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>929.39013840830444</v>
+        <v>991.34948096885807</v>
       </c>
       <c r="V20" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -8900,13 +8876,13 @@
         <v>1800</v>
       </c>
       <c r="B21" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>975.28594771241819</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>877.75735294117646</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>975.28594771241819</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="3">
@@ -8915,7 +8891,7 @@
       </c>
       <c r="G21" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>877.75735294117646</v>
+        <v>975.28594771241819</v>
       </c>
       <c r="H21" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -8923,19 +8899,19 @@
       </c>
       <c r="I21" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>225</v>
+        <v>249.99999999999994</v>
       </c>
       <c r="J21" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>222.97222222222223</v>
+        <v>214.82638888888889</v>
       </c>
       <c r="K21" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="975" motorTorqueEco="878" fuelUsageRatio="223"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="975" fuelUsageRatio="214.8"/&gt;</v>
       </c>
       <c r="L21" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.9" torque="0.887"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.818" torque="0.887"/&gt;</v>
       </c>
       <c r="M21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8946,16 +8922,16 @@
         <v>1072.5</v>
       </c>
       <c r="O21" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
-        <v>975.28594771241819</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
+        <v>984.47053986068101</v>
       </c>
       <c r="P21" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>975.28594771241819</v>
+        <v>965.53308823529403</v>
       </c>
       <c r="Q21" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -8963,19 +8939,19 @@
       </c>
       <c r="S21" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1018.875</v>
+        <v>1072.5</v>
       </c>
       <c r="T21" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>877.75735294117646</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>984.47053986068101</v>
       </c>
       <c r="U21" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>877.75735294117646</v>
+        <v>965.53308823529403</v>
       </c>
       <c r="V21" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -8983,13 +8959,13 @@
         <v>1900</v>
       </c>
       <c r="B22" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>923.95510835913308</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>831.55959752321974</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>923.95510835913308</v>
       </c>
       <c r="E22" s="21"/>
       <c r="F22" s="3">
@@ -8998,7 +8974,7 @@
       </c>
       <c r="G22" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>831.55959752321974</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="H22" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
@@ -9006,19 +8982,19 @@
       </c>
       <c r="I22" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="J22" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>230</v>
+        <v>218.99691358024691</v>
       </c>
       <c r="K22" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="924" motorTorqueEco="832" fuelUsageRatio="230"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="924" fuelUsageRatio="219"/&gt;</v>
       </c>
       <c r="L22" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.95" torque="0.84"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.864" torque="0.84"/&gt;</v>
       </c>
       <c r="M22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -9029,7 +9005,7 @@
         <v>1051.1111111111111</v>
       </c>
       <c r="O22" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>923.95510835913308</v>
       </c>
       <c r="P22" s="3">
@@ -9038,27 +9014,27 @@
       </c>
       <c r="Q22" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>923.95510835913308</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-220.61111111111126</v>
+        <v>-232.22222222222237</v>
       </c>
       <c r="S22" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>998.55555555555566</v>
+        <v>1051.1111111111111</v>
       </c>
       <c r="T22" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>831.55959752321974</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>923.95510835913308</v>
       </c>
       <c r="U22" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>831.55959752321974</v>
+        <v>923.95510835913308</v>
       </c>
       <c r="V22" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>831.55959752321974</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -9066,42 +9042,42 @@
         <v>2000</v>
       </c>
       <c r="B23" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>796.06627888149092</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
+        <v>868.97977941176464</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>716.45965099334182</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>868.97977941176464</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>796.06627888149092</v>
+        <v>868.97977941176464</v>
       </c>
       <c r="G23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>716.45965099334182</v>
+        <v>868.97977941176464</v>
       </c>
       <c r="H23" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>226.7330134615346</v>
+        <v>247.5</v>
       </c>
       <c r="I23" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>204.05971211538113</v>
+        <v>247.5</v>
       </c>
       <c r="J23" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>244.75450687929043</v>
+        <v>224.05478395061729</v>
       </c>
       <c r="K23" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="796" motorTorqueEco="716" fuelUsageRatio="244.8"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="869" fuelUsageRatio="224.1"/&gt;</v>
       </c>
       <c r="L23" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.724"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.909" torque="0.79"/&gt;</v>
       </c>
       <c r="M23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -9112,36 +9088,36 @@
         <v>1023.6111111111111</v>
       </c>
       <c r="O23" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>852.4368711300308</v>
       </c>
       <c r="P23" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>877.75735294117635</v>
+        <v>868.97977941176464</v>
       </c>
       <c r="Q23" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>796.06627888149092</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-464.44444444444463</v>
+        <v>-488.88888888888908</v>
       </c>
       <c r="S23" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>972.43055555555554</v>
+        <v>1023.6111111111111</v>
       </c>
       <c r="T23" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>744.84943401702776</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>852.4368711300308</v>
       </c>
       <c r="U23" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>789.98161764705878</v>
+        <v>868.97977941176464</v>
       </c>
       <c r="V23" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>716.45965099334182</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -9149,42 +9125,42 @@
         <v>2100</v>
       </c>
       <c r="B24" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>478.62033819495952</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
+        <v>802.52100840336129</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>430.75830437546352</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>802.52100840336129</v>
       </c>
       <c r="E24" s="21"/>
       <c r="F24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>478.62033819495952</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="G24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>430.75830437546352</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="H24" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>143.13504564238789</v>
+        <v>240</v>
       </c>
       <c r="I24" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>128.8215410781491</v>
+        <v>240</v>
       </c>
       <c r="J24" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>313.46409493927865</v>
+        <v>230</v>
       </c>
       <c r="K24" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="479" motorTorqueEco="431" fuelUsageRatio="313.5"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="803" fuelUsageRatio="230"/&gt;</v>
       </c>
       <c r="L24" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v/>
+        <v xml:space="preserve">        &lt;torque normRpm="0.955" torque="0.73"/&gt;</v>
       </c>
       <c r="M24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -9195,36 +9171,36 @@
         <v>990</v>
       </c>
       <c r="O24" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>769.91582817337451</v>
       </c>
       <c r="P24" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>835.95938375350136</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="Q24" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>478.62033819495952</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="R24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-731.50000000000034</v>
+        <v>-770.00000000000034</v>
       </c>
       <c r="S24" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>940.5</v>
+        <v>990</v>
       </c>
       <c r="T24" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>644.79924535603709</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>769.91582817337451</v>
       </c>
       <c r="U24" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>752.36344537815125</v>
+        <v>802.52100840336129</v>
       </c>
       <c r="V24" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>430.75830437546352</v>
+        <v>802.52100840336129</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -9232,42 +9208,42 @@
         <v>2200</v>
       </c>
       <c r="B25" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>0</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
+        <v>636.71088270018754</v>
       </c>
       <c r="C25" s="21"/>
       <c r="D25" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>0</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>636.71088270018754</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>636.71088270018754</v>
       </c>
       <c r="G25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>0</v>
+        <v>636.71088270018754</v>
       </c>
       <c r="H25" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>0</v>
+        <v>199.48051948051949</v>
       </c>
       <c r="I25" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>0</v>
+        <v>199.48051948051949</v>
       </c>
       <c r="J25" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>262.03842321622847</v>
       </c>
       <c r="K25" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="0" motorTorqueEco="0" fuelUsageRatio="460"/&gt;</v>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="637" fuelUsageRatio="262"/&gt;</v>
       </c>
       <c r="L25" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v/>
+        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.579"/&gt;</v>
       </c>
       <c r="M25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -9278,36 +9254,36 @@
         <v>950.27777777777783</v>
       </c>
       <c r="O25" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>676.39197948916399</v>
       </c>
       <c r="P25" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>797.96122994652399</v>
+        <v>726.14471925133694</v>
       </c>
       <c r="Q25" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>636.71088270018754</v>
       </c>
       <c r="R25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1021.7777777777782</v>
+        <v>-1075.5555555555559</v>
       </c>
       <c r="S25" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>902.76388888888891</v>
+        <v>950.27777777777783</v>
       </c>
       <c r="T25" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>531.40903154024738</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>676.39197948916399</v>
       </c>
       <c r="U25" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>718.16510695187162</v>
+        <v>726.14471925133694</v>
       </c>
       <c r="V25" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>636.71088270018754</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -9315,38 +9291,38 @@
         <v>2300</v>
       </c>
       <c r="B26" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
-        <v>0</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
+        <v>139.28050559066608</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
-        <v>0</v>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
+        <v>139.28050559066608</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>139.28050559066608</v>
       </c>
       <c r="G26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>0</v>
+        <v>139.28050559066608</v>
       </c>
       <c r="H26" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>0</v>
+        <v>45.619834710743824</v>
       </c>
       <c r="I26" s="30">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>0</v>
+        <v>45.619834710743824</v>
       </c>
       <c r="J26" s="30">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>411.23669051775721</v>
       </c>
       <c r="K26" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v/>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="139" fuelUsageRatio="411.2"/&gt;</v>
       </c>
       <c r="L26" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
@@ -9361,36 +9337,36 @@
         <v>904.44444444444457</v>
       </c>
       <c r="O26" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>571.86532507739912</v>
       </c>
       <c r="P26" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>763.26726342710992</v>
+        <v>641.1445012787724</v>
       </c>
       <c r="Q26" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>139.28050559066608</v>
       </c>
       <c r="R26" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1335.2777777777769</v>
+        <v>-1405.5555555555547</v>
       </c>
       <c r="S26" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>859.22222222222229</v>
+        <v>904.44444444444457</v>
       </c>
       <c r="T26" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>404.67879256965921</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>571.86532507739912</v>
       </c>
       <c r="U26" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>686.9405370843989</v>
+        <v>641.1445012787724</v>
       </c>
       <c r="V26" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>139.28050559066608</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -9398,12 +9374,12 @@
         <v>2400</v>
       </c>
       <c r="B27" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E27" s="21"/>
@@ -9428,8 +9404,8 @@
         <v>460</v>
       </c>
       <c r="K27" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v/>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="0" fuelUsageRatio="460"/&gt;</v>
       </c>
       <c r="L27" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
@@ -9444,12 +9420,12 @@
         <v>852.5</v>
       </c>
       <c r="O27" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>456.33586493808031</v>
       </c>
       <c r="P27" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>731.4644607843137</v>
+        <v>548.59834558823525</v>
       </c>
       <c r="Q27" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9457,19 +9433,19 @@
       </c>
       <c r="R27" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1671.9999999999995</v>
+        <v>-1759.9999999999995</v>
       </c>
       <c r="S27" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>809.875</v>
+        <v>852.5</v>
       </c>
       <c r="T27" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>264.60852844427217</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>456.33586493808031</v>
       </c>
       <c r="U27" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>658.31801470588232</v>
+        <v>548.59834558823525</v>
       </c>
       <c r="V27" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9481,12 +9457,12 @@
         <v>2500</v>
       </c>
       <c r="B28" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E28" s="21"/>
@@ -9511,7 +9487,7 @@
         <v>460</v>
       </c>
       <c r="K28" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L28" s="10" t="str">
@@ -9527,12 +9503,12 @@
         <v>794.44444444444457</v>
       </c>
       <c r="O28" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>329.80359907120709</v>
       </c>
       <c r="P28" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>702.2058823529411</v>
+        <v>449.41176470588232</v>
       </c>
       <c r="Q28" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9540,19 +9516,19 @@
       </c>
       <c r="R28" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-2031.9444444444443</v>
+        <v>-2138.8888888888887</v>
       </c>
       <c r="S28" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>754.72222222222229</v>
+        <v>794.44444444444457</v>
       </c>
       <c r="T28" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
-        <v>111.19823916408642</v>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
+        <v>329.80359907120709</v>
       </c>
       <c r="U28" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>631.98529411764707</v>
+        <v>449.41176470588232</v>
       </c>
       <c r="V28" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9564,12 +9540,12 @@
         <v>2750</v>
       </c>
       <c r="B29" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E29" s="21"/>
@@ -9594,7 +9570,7 @@
         <v>460</v>
       </c>
       <c r="K29" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L29" s="10" t="str">
@@ -9610,12 +9586,12 @@
         <v>622.56944444444457</v>
       </c>
       <c r="O29" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P29" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>638.36898395721914</v>
+        <v>177.14739304812832</v>
       </c>
       <c r="Q29" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9623,19 +9599,19 @@
       </c>
       <c r="R29" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-3033.4027777777769</v>
+        <v>-3193.0555555555547</v>
       </c>
       <c r="S29" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>591.44097222222229</v>
+        <v>622.56944444444457</v>
       </c>
       <c r="T29" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U29" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>574.5320855614973</v>
+        <v>177.14739304812832</v>
       </c>
       <c r="V29" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9647,12 +9623,12 @@
         <v>3000</v>
       </c>
       <c r="B30" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E30" s="21"/>
@@ -9677,7 +9653,7 @@
         <v>460</v>
       </c>
       <c r="K30" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L30" s="10" t="str">
@@ -9693,12 +9669,12 @@
         <v>412.50000000000011</v>
       </c>
       <c r="O30" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P30" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>585.17156862745094</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9706,19 +9682,19 @@
       </c>
       <c r="R30" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-4180.0000000000009</v>
+        <v>-4400.0000000000009</v>
       </c>
       <c r="S30" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>391.87500000000011</v>
+        <v>412.50000000000011</v>
       </c>
       <c r="T30" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U30" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>526.65441176470586</v>
+        <v>0</v>
       </c>
       <c r="V30" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9730,12 +9706,12 @@
         <v>3250</v>
       </c>
       <c r="B31" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E31" s="21"/>
@@ -9760,7 +9736,7 @@
         <v>460</v>
       </c>
       <c r="K31" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L31" s="10" t="str">
@@ -9776,12 +9752,12 @@
         <v>164.23611111111137</v>
       </c>
       <c r="O31" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P31" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>540.15837104072398</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9789,19 +9765,19 @@
       </c>
       <c r="R31" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-5471.7361111111113</v>
+        <v>-5759.7222222222217</v>
       </c>
       <c r="S31" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>156.02430555555583</v>
+        <v>164.23611111111137</v>
       </c>
       <c r="T31" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U31" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>486.14253393665155</v>
+        <v>0</v>
       </c>
       <c r="V31" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9813,12 +9789,12 @@
         <v>3500</v>
       </c>
       <c r="B32" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E32" s="21"/>
@@ -9843,7 +9819,7 @@
         <v>460</v>
       </c>
       <c r="K32" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L32" s="10" t="str">
@@ -9859,12 +9835,12 @@
         <v>0</v>
       </c>
       <c r="O32" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P32" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>501.57563025210078</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9872,19 +9848,19 @@
       </c>
       <c r="R32" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-6908.6111111111113</v>
+        <v>-7272.2222222222217</v>
       </c>
       <c r="S32" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T32" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U32" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>451.41806722689074</v>
+        <v>0</v>
       </c>
       <c r="V32" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9896,12 +9872,12 @@
         <v>3750</v>
       </c>
       <c r="B33" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E33" s="21"/>
@@ -9926,7 +9902,7 @@
         <v>460</v>
       </c>
       <c r="K33" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L33" s="10" t="str">
@@ -9942,12 +9918,12 @@
         <v>0</v>
       </c>
       <c r="O33" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P33" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>468.13725490196072</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9955,19 +9931,19 @@
       </c>
       <c r="R33" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-8490.6250000000018</v>
+        <v>-8937.5000000000018</v>
       </c>
       <c r="S33" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T33" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U33" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>421.3235294117647</v>
+        <v>0</v>
       </c>
       <c r="V33" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9979,12 +9955,12 @@
         <v>4000</v>
       </c>
       <c r="B34" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E34" s="21"/>
@@ -10009,7 +9985,7 @@
         <v>460</v>
       </c>
       <c r="K34" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L34" s="10" t="str">
@@ -10025,12 +10001,12 @@
         <v>0</v>
       </c>
       <c r="O34" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P34" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>438.87867647058818</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10038,19 +10014,19 @@
       </c>
       <c r="R34" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-10217.777777777779</v>
+        <v>-10755.555555555558</v>
       </c>
       <c r="S34" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T34" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U34" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>394.99080882352939</v>
+        <v>0</v>
       </c>
       <c r="V34" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10062,12 +10038,12 @@
         <v>4250</v>
       </c>
       <c r="B35" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E35" s="21"/>
@@ -10092,7 +10068,7 @@
         <v>460</v>
       </c>
       <c r="K35" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L35" s="10" t="str">
@@ -10108,12 +10084,12 @@
         <v>0</v>
       </c>
       <c r="O35" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P35" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>413.06228373702419</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10121,19 +10097,19 @@
       </c>
       <c r="R35" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-12090.069444444445</v>
+        <v>-12726.388888888889</v>
       </c>
       <c r="S35" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T35" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U35" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>371.75605536332176</v>
+        <v>0</v>
       </c>
       <c r="V35" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10145,12 +10121,12 @@
         <v>4500</v>
       </c>
       <c r="B36" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E36" s="21"/>
@@ -10175,7 +10151,7 @@
         <v>460</v>
       </c>
       <c r="K36" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L36" s="10" t="str">
@@ -10191,12 +10167,12 @@
         <v>0</v>
       </c>
       <c r="O36" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P36" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>390.11437908496731</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10204,19 +10180,19 @@
       </c>
       <c r="R36" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-14107.5</v>
+        <v>-14850</v>
       </c>
       <c r="S36" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T36" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U36" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>351.10294117647055</v>
+        <v>0</v>
       </c>
       <c r="V36" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10228,12 +10204,12 @@
         <v>4750</v>
       </c>
       <c r="B37" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E37" s="21"/>
@@ -10258,7 +10234,7 @@
         <v>460</v>
       </c>
       <c r="K37" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L37" s="10" t="str">
@@ -10274,12 +10250,12 @@
         <v>0</v>
       </c>
       <c r="O37" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P37" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>369.5820433436532</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10287,19 +10263,19 @@
       </c>
       <c r="R37" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-16270.069444444445</v>
+        <v>-17126.388888888891</v>
       </c>
       <c r="S37" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T37" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U37" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>332.62383900928791</v>
+        <v>0</v>
       </c>
       <c r="V37" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10311,12 +10287,12 @@
         <v>5000</v>
       </c>
       <c r="B38" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E38" s="21"/>
@@ -10341,7 +10317,7 @@
         <v>460</v>
       </c>
       <c r="K38" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L38" s="10" t="str">
@@ -10357,12 +10333,12 @@
         <v>0</v>
       </c>
       <c r="O38" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P38" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>351.10294117647055</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10370,19 +10346,19 @@
       </c>
       <c r="R38" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-18577.777777777777</v>
+        <v>-19555.555555555555</v>
       </c>
       <c r="S38" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T38" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U38" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>315.99264705882354</v>
+        <v>0</v>
       </c>
       <c r="V38" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10394,12 +10370,12 @@
         <v>5250</v>
       </c>
       <c r="B39" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E39" s="21"/>
@@ -10424,7 +10400,7 @@
         <v>460</v>
       </c>
       <c r="K39" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L39" s="10" t="str">
@@ -10440,12 +10416,12 @@
         <v>0</v>
       </c>
       <c r="O39" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P39" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>334.38375350140052</v>
+        <v>0</v>
       </c>
       <c r="Q39" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10453,19 +10429,19 @@
       </c>
       <c r="R39" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-21030.624999999996</v>
+        <v>-22137.499999999996</v>
       </c>
       <c r="S39" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T39" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U39" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>300.94537815126051</v>
+        <v>0</v>
       </c>
       <c r="V39" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10477,12 +10453,12 @@
         <v>5500</v>
       </c>
       <c r="B40" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E40" s="21"/>
@@ -10507,7 +10483,7 @@
         <v>460</v>
       </c>
       <c r="K40" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L40" s="10" t="str">
@@ -10523,12 +10499,12 @@
         <v>0</v>
       </c>
       <c r="O40" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P40" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>319.18449197860957</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10536,19 +10512,19 @@
       </c>
       <c r="R40" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-23628.611111111106</v>
+        <v>-24872.222222222219</v>
       </c>
       <c r="S40" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T40" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U40" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>287.26604278074865</v>
+        <v>0</v>
       </c>
       <c r="V40" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10560,12 +10536,12 @@
         <v>5750</v>
       </c>
       <c r="B41" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E41" s="21"/>
@@ -10590,7 +10566,7 @@
         <v>460</v>
       </c>
       <c r="K41" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L41" s="10" t="str">
@@ -10606,12 +10582,12 @@
         <v>0</v>
       </c>
       <c r="O41" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P41" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>305.30690537084394</v>
+        <v>0</v>
       </c>
       <c r="Q41" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10619,19 +10595,19 @@
       </c>
       <c r="R41" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-26371.736111111113</v>
+        <v>-27759.722222222226</v>
       </c>
       <c r="S41" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T41" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U41" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>274.77621483375958</v>
+        <v>0</v>
       </c>
       <c r="V41" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10643,12 +10619,12 @@
         <v>6000</v>
       </c>
       <c r="B42" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="3">
-        <f>MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco])))))</f>
+        <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
       <c r="E42" s="22"/>
@@ -10673,7 +10649,7 @@
         <v>460</v>
       </c>
       <c r="K42" s="10" t="str">
-        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),""" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""" fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
+        <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
         <v/>
       </c>
       <c r="L42" s="10" t="str">
@@ -10689,12 +10665,12 @@
         <v>0</v>
       </c>
       <c r="O42" s="3">
-        <f>MIN(Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
         <v>0</v>
       </c>
       <c r="P42" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>292.58578431372547</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -10702,19 +10678,19 @@
       </c>
       <c r="R42" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-29260.000000000004</v>
+        <v>-30800.000000000004</v>
       </c>
       <c r="S42" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="T42" s="3">
-        <f>MIN(Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco]))</f>
+        <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
         <v>0</v>
       </c>
       <c r="U42" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>263.32720588235293</v>
+        <v>0</v>
       </c>
       <c r="V42" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>

</xml_diff>

<commit_message>
JD 8400i forage harvester
</commit_message>
<xml_diff>
--- a/Documents/MotorNeu.xlsx
+++ b/Documents/MotorNeu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24645" yWindow="0" windowWidth="20400" windowHeight="9945"/>
+    <workbookView xWindow="26100" yWindow="0" windowWidth="20400" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="Calculate from Values" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>rpm</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>fadeOutExp</t>
+  </si>
+  <si>
+    <t>g/kWh</t>
+  </si>
+  <si>
+    <t>max kW</t>
+  </si>
+  <si>
+    <t>rated kW</t>
   </si>
 </sst>
 </file>
@@ -494,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -512,7 +521,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -526,65 +534,115 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="76">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="6"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1402,6 +1460,47 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1447,6 +1546,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
@@ -1459,6 +1561,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1677,67 +1782,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>240.37037037037044</c:v>
+                  <c:v>65.594032081968592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>704.81481481481478</c:v>
+                  <c:v>198.07791719156796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>912.59259259259272</c:v>
+                  <c:v>268.84252792475007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>953.33333333333337</c:v>
+                  <c:v>286.43267993617201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>990</c:v>
+                  <c:v>303.77999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1023.6111111111111</c:v>
+                  <c:v>320.2873469387755</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1051.1111111111111</c:v>
+                  <c:v>334.25510204081633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1072.5</c:v>
+                  <c:v>345.68326530612245</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1087.7777777777778</c:v>
+                  <c:v>354.57183673469387</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1096.9444444444443</c:v>
+                  <c:v>360.9208163265306</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1100</c:v>
+                  <c:v>364.73020408163262</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1072.4929856811145</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1032.6557093425604</c:v>
+                  <c:v>361.40352941176468</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>975.28594771241819</c:v>
+                  <c:v>355.27490196078435</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>923.95510835913308</c:v>
+                  <c:v>347.61411764705883</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>868.97977941176464</c:v>
+                  <c:v>338.42117647058825</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>802.52100840336129</c:v>
+                  <c:v>327.69607843137254</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>636.71088270018754</c:v>
+                  <c:v>310.4069184491978</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>139.28050559066608</c:v>
+                  <c:v>290.04156010230173</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>242.73862745517255</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>57.094595048925981</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -1951,67 +2056,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>240.37037037037044</c:v>
+                  <c:v>65.594032081968592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>704.81481481481478</c:v>
+                  <c:v>198.07791719156796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>912.59259259259272</c:v>
+                  <c:v>268.84252792475007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>953.33333333333337</c:v>
+                  <c:v>286.43267993617201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>990</c:v>
+                  <c:v>303.77999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1023.6111111111111</c:v>
+                  <c:v>320.2873469387755</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1051.1111111111111</c:v>
+                  <c:v>334.25510204081633</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1072.5</c:v>
+                  <c:v>345.68326530612245</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1087.7777777777778</c:v>
+                  <c:v>354.57183673469387</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1096.9444444444443</c:v>
+                  <c:v>360.9208163265306</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1100</c:v>
+                  <c:v>364.73020408163262</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1072.4929856811145</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1032.6557093425604</c:v>
+                  <c:v>361.40352941176468</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>975.28594771241819</c:v>
+                  <c:v>355.27490196078435</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>923.95510835913308</c:v>
+                  <c:v>347.61411764705883</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>868.97977941176464</c:v>
+                  <c:v>338.42117647058825</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>802.52100840336129</c:v>
+                  <c:v>327.69607843137254</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>636.71088270018754</c:v>
+                  <c:v>310.4069184491978</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>139.28050559066608</c:v>
+                  <c:v>290.04156010230173</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>242.73862745517255</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>57.094595048925981</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -2068,8 +2173,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324524728"/>
-        <c:axId val="357168752"/>
+        <c:axId val="376552432"/>
+        <c:axId val="376552040"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2239,67 +2344,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4230754314523959</c:v>
+                  <c:v>0.93411396472751085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.148613535000962</c:v>
+                  <c:v>11.283181879812876</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.972580957921295</c:v>
+                  <c:v>26.799799642341583</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.61012216404887</c:v>
+                  <c:v>32.632330447178546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>126.88586387434555</c:v>
+                  <c:v>38.934735078534025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>145.77079697498544</c:v>
+                  <c:v>45.61160123944866</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>164.65573007562537</c:v>
+                  <c:v>52.360799230687043</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>183.27958115183247</c:v>
+                  <c:v>59.073831306763559</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>201.38126817917399</c:v>
+                  <c:v>65.642199722192544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>218.699709133217</c:v>
+                  <c:v>71.957406731488419</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>234.97382198952886</c:v>
+                  <c:v>77.910954589165499</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>244.37117663268117</c:v>
+                  <c:v>83.394345549738219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>249.99999999999994</c:v>
+                  <c:v>87.493713089005226</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>249.99999999999994</c:v>
+                  <c:v>91.069419895287965</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>250</c:v>
+                  <c:v>94.056008376963348</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>247.5</c:v>
+                  <c:v>96.388020942408389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>240</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>199.48051948051949</c:v>
+                  <c:v>97.249999999999986</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45.619834710743824</c:v>
+                  <c:v>94.999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>0</c:v>
+                  <c:v>82.963233509286212</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>0</c:v>
+                  <c:v>20.326871535743283</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
                   <c:v>0</c:v>
@@ -2513,67 +2618,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4230754314523959</c:v>
+                  <c:v>0.93411396472751085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.148613535000962</c:v>
+                  <c:v>11.283181879812876</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.972580957921295</c:v>
+                  <c:v>26.799799642341583</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.61012216404887</c:v>
+                  <c:v>32.632330447178546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>126.88586387434555</c:v>
+                  <c:v>38.934735078534025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>145.77079697498544</c:v>
+                  <c:v>45.61160123944866</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>164.65573007562537</c:v>
+                  <c:v>52.360799230687043</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>183.27958115183247</c:v>
+                  <c:v>59.073831306763559</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>201.38126817917399</c:v>
+                  <c:v>65.642199722192544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>218.699709133217</c:v>
+                  <c:v>71.957406731488419</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>234.97382198952886</c:v>
+                  <c:v>77.910954589165499</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>244.37117663268117</c:v>
+                  <c:v>83.394345549738219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>249.99999999999994</c:v>
+                  <c:v>87.493713089005226</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>249.99999999999994</c:v>
+                  <c:v>91.069419895287965</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>250</c:v>
+                  <c:v>94.056008376963348</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>247.5</c:v>
+                  <c:v>96.388020942408389</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>240</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>199.48051948051949</c:v>
+                  <c:v>97.249999999999986</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45.619834710743824</c:v>
+                  <c:v>94.999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>0</c:v>
+                  <c:v>82.963233509286212</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>0</c:v>
+                  <c:v>20.326871535743283</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
                   <c:v>0</c:v>
@@ -2630,11 +2735,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276489232"/>
-        <c:axId val="357169136"/>
+        <c:axId val="376553216"/>
+        <c:axId val="376548904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324524728"/>
+        <c:axId val="376552432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -2738,13 +2843,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357168752"/>
+        <c:crossAx val="376552040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="357168752"/>
+        <c:axId val="376552040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,12 +2951,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324524728"/>
+        <c:crossAx val="376552432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="357169136"/>
+        <c:axId val="376548904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,12 +2999,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276489232"/>
+        <c:crossAx val="376553216"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276489232"/>
+        <c:axId val="376553216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2909,7 +3014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="357169136"/>
+        <c:crossAx val="376548904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3197,112 +3302,112 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>283.04374999999993</c:v>
+                  <c:v>279.95096371882079</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>272.4222222222221</c:v>
+                  <c:v>271.35827664399085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>245.3493055555555</c:v>
+                  <c:v>249.23667800453509</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>225.46388888888887</c:v>
+                  <c:v>232.59977324263036</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>220.43263888888887</c:v>
+                  <c:v>228.27295918367346</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>216.2</c:v>
+                  <c:v>224.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>212.76597222222222</c:v>
+                  <c:v>221.44756235827663</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>210.13055555555556</c:v>
+                  <c:v>218.94897959183672</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>208.29374999999999</c:v>
+                  <c:v>217.05980725623581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>207.25555555555556</c:v>
+                  <c:v>215.78004535147392</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>207.01774691358025</c:v>
+                  <c:v>215.10969387755102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>207.63888888888889</c:v>
+                  <c:v>215.05416981607459</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>209.14737654320987</c:v>
+                  <c:v>215.66358024691357</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>211.54320987654322</c:v>
+                  <c:v>216.95011337868482</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>214.82638888888889</c:v>
+                  <c:v>218.91376921138826</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>218.99691358024691</c:v>
+                  <c:v>221.55454774502394</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>224.05478395061729</c:v>
+                  <c:v>224.87244897959184</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>230</c:v>
+                  <c:v>228.86747291509195</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>262.03842321622847</c:v>
+                  <c:v>233.53961955152431</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>411.23669051775721</c:v>
+                  <c:v>238.88888888888889</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>460</c:v>
+                  <c:v>272.16551203617928</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>460</c:v>
+                  <c:v>427.12989594839519</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>460</c:v>
+                  <c:v>477.77777777777777</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3317,11 +3422,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276490800"/>
-        <c:axId val="276490016"/>
+        <c:axId val="376548512"/>
+        <c:axId val="376555176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276490800"/>
+        <c:axId val="376548512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6000"/>
@@ -3425,13 +3530,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276490016"/>
+        <c:crossAx val="376555176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276490016"/>
+        <c:axId val="376555176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -3529,7 +3634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276490800"/>
+        <c:crossAx val="376548512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -3845,11 +3950,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="276490408"/>
-        <c:axId val="276491192"/>
+        <c:axId val="376555960"/>
+        <c:axId val="375547304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="276490408"/>
+        <c:axId val="376555960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2700"/>
@@ -3908,12 +4013,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276491192"/>
+        <c:crossAx val="375547304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="276491192"/>
+        <c:axId val="375547304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +4075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="276490408"/>
+        <c:crossAx val="376555960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4231,11 +4336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324870288"/>
-        <c:axId val="324875384"/>
+        <c:axId val="375541816"/>
+        <c:axId val="375542992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324870288"/>
+        <c:axId val="375541816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2400"/>
@@ -4294,12 +4399,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324875384"/>
+        <c:crossAx val="375542992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324875384"/>
+        <c:axId val="375542992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324870288"/>
+        <c:crossAx val="375541816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6769,66 +6874,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A6:V42" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A6:V42" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <tableColumns count="22">
-    <tableColumn id="1" name="rpm" dataDxfId="70"/>
-    <tableColumn id="7" name="rawData" dataDxfId="2">
+    <tableColumn id="1" name="rpm" dataDxfId="73"/>
+    <tableColumn id="7" name="rawData" dataDxfId="72">
       <calculatedColumnFormula>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="manualData" dataDxfId="69"/>
-    <tableColumn id="12" name="rawDataEco" dataDxfId="1">
+    <tableColumn id="9" name="manualData" dataDxfId="71"/>
+    <tableColumn id="12" name="rawDataEco" dataDxfId="70">
       <calculatedColumnFormula>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="manDataEco" dataDxfId="68"/>
-    <tableColumn id="4" name="motor" dataDxfId="67">
+    <tableColumn id="11" name="manDataEco" dataDxfId="69"/>
+    <tableColumn id="4" name="motor" dataDxfId="68">
       <calculatedColumnFormula>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="motorEco" dataDxfId="66">
+    <tableColumn id="14" name="motorEco" dataDxfId="67">
       <calculatedColumnFormula>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="65">
+    <tableColumn id="3" name="ps" dataDxfId="66">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="psEco" dataDxfId="64">
+    <tableColumn id="13" name="psEco" dataDxfId="65">
       <calculatedColumnFormula>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="63">
+    <tableColumn id="10" name="fuelUsageRatio" dataDxfId="64">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="0">
+    <tableColumn id="5" name="xml" dataDxfId="63">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="xml2" dataDxfId="62">
       <calculatedColumnFormula>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="t1" dataDxfId="11">
+    <tableColumn id="15" name="t1" dataDxfId="61">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="t2" dataDxfId="9">
+    <tableColumn id="18" name="t2" dataDxfId="60">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="t3" dataDxfId="8">
+    <tableColumn id="19" name="t3" dataDxfId="59">
       <calculatedColumnFormula>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="t4" dataDxfId="7">
+    <tableColumn id="16" name="t4" dataDxfId="58">
       <calculatedColumnFormula>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="t5" dataDxfId="6">
+    <tableColumn id="17" name="t5" dataDxfId="57">
       <calculatedColumnFormula>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="t1E" dataDxfId="5">
+    <tableColumn id="21" name="t1E" dataDxfId="56">
       <calculatedColumnFormula>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="t2E" dataDxfId="4">
+    <tableColumn id="22" name="t2E" dataDxfId="55">
       <calculatedColumnFormula>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="t3E" dataDxfId="3">
+    <tableColumn id="23" name="t3E" dataDxfId="54">
       <calculatedColumnFormula>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="t4E" dataDxfId="10">
+    <tableColumn id="24" name="t4E" dataDxfId="53">
       <calculatedColumnFormula>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="t5E" dataDxfId="61">
+    <tableColumn id="25" name="t5E" dataDxfId="52">
       <calculatedColumnFormula>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6837,7 +6942,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table36" displayName="Table36" ref="A1:Y2" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="A1:Y2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -6862,45 +6967,45 @@
     <filterColumn colId="21" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="25">
-    <tableColumn id="10" name="maxPRpm" dataDxfId="59"/>
-    <tableColumn id="14" name="maxPS" dataDxfId="58"/>
-    <tableColumn id="19" name="maxPSEco" dataDxfId="57">
+    <tableColumn id="10" name="maxPRpm" dataDxfId="50"/>
+    <tableColumn id="14" name="maxPS" dataDxfId="49"/>
+    <tableColumn id="19" name="maxPSEco" dataDxfId="48">
       <calculatedColumnFormula>Table36[maxPsEcoRate]*Table36[maxPS]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="ratedRpm"/>
     <tableColumn id="3" name="PS"/>
-    <tableColumn id="20" name="PSEco" dataDxfId="56">
+    <tableColumn id="20" name="PSEco" dataDxfId="47">
       <calculatedColumnFormula>Table36[PS]*Table36[PSEcoRate]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="maxTRpm1" dataDxfId="55"/>
-    <tableColumn id="4" name="maxTRpm" dataDxfId="54"/>
-    <tableColumn id="5" name="maxT" dataDxfId="53"/>
-    <tableColumn id="21" name="maxTEco" dataDxfId="52">
+    <tableColumn id="12" name="maxTRpm1" dataDxfId="46"/>
+    <tableColumn id="4" name="maxTRpm" dataDxfId="45"/>
+    <tableColumn id="5" name="maxT" dataDxfId="44"/>
+    <tableColumn id="21" name="maxTEco" dataDxfId="43">
       <calculatedColumnFormula>Table36[NmEcoRate]*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="idleRpm"/>
     <tableColumn id="7" name="idleRatio" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="fadeOut" dataDxfId="51"/>
-    <tableColumn id="15" name="linearDown" dataDxfId="50"/>
-    <tableColumn id="25" name="fadeOutExp" dataDxfId="49"/>
-    <tableColumn id="22" name="Efficiency" dataDxfId="48"/>
-    <tableColumn id="16" name="Factor" dataDxfId="47"/>
-    <tableColumn id="13" name="fuelMinRate" dataDxfId="46"/>
-    <tableColumn id="18" name="fuelRatedRate" dataDxfId="45">
+    <tableColumn id="11" name="fadeOut" dataDxfId="42"/>
+    <tableColumn id="15" name="linearDown" dataDxfId="41"/>
+    <tableColumn id="25" name="fadeOutExp" dataDxfId="40"/>
+    <tableColumn id="22" name="Efficiency" dataDxfId="39"/>
+    <tableColumn id="16" name="Factor" dataDxfId="38"/>
+    <tableColumn id="13" name="fuelMinRate" dataDxfId="37"/>
+    <tableColumn id="18" name="fuelRatedRate" dataDxfId="36">
       <calculatedColumnFormula>Table36[fuelMinRate]/0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="fuelMinRpm" dataDxfId="44">
+    <tableColumn id="9" name="fuelMinRpm" dataDxfId="35">
       <calculatedColumnFormula>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="fuelIdleRate" dataDxfId="43">
+    <tableColumn id="17" name="fuelIdleRate" dataDxfId="34">
       <calculatedColumnFormula>0.94*Table36[fuelRatedRate]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="normRpm" dataDxfId="42">
+    <tableColumn id="1" name="normRpm" dataDxfId="33">
       <calculatedColumnFormula>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="PSEcoRate" dataDxfId="41"/>
+    <tableColumn id="8" name="PSEcoRate" dataDxfId="32"/>
     <tableColumn id="23" name="NmEcoRate"/>
-    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="40">
+    <tableColumn id="24" name="maxPsEcoRate" dataDxfId="31">
       <calculatedColumnFormula>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6909,80 +7014,72 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:S4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A3:S4">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
-    <filterColumn colId="15" hiddenButton="1"/>
-    <filterColumn colId="16" hiddenButton="1"/>
-    <filterColumn colId="17" hiddenButton="1"/>
-    <filterColumn colId="18" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="19">
-    <tableColumn id="1" name="f1" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:V4" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <tableColumns count="22">
+    <tableColumn id="1" name="f1" dataDxfId="28">
       <calculatedColumnFormula>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="f2" dataDxfId="36">
+    <tableColumn id="2" name="f2" dataDxfId="27">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="f3" dataDxfId="35">
+    <tableColumn id="5" name="f3" dataDxfId="26">
       <calculatedColumnFormula>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="f4" dataDxfId="34">
+    <tableColumn id="6" name="f4" dataDxfId="25">
       <calculatedColumnFormula>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Nm" dataDxfId="33">
+    <tableColumn id="3" name="Nm" dataDxfId="24">
       <calculatedColumnFormula>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Nm2" dataDxfId="32">
+    <tableColumn id="4" name="Nm2" dataDxfId="23">
       <calculatedColumnFormula>Table36[PS]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Anfahrmoment" dataDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="7" name="Anfahrmoment" dataDxfId="22" dataCellStyle="Percent">
       <calculatedColumnFormula>Table7[Nm1000]/Table7[Nm2Eco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="AnstiegE" dataDxfId="30" dataCellStyle="Percent">
+    <tableColumn id="17" name="AnstiegE" dataDxfId="21" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxTEco]/Table7[Nm2Eco]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Anstieg" dataDxfId="29" dataCellStyle="Percent">
+    <tableColumn id="14" name="Anstieg" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>Table36[maxT]/Table7[Nm2]-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Abfall" dataDxfId="28" dataCellStyle="Percent">
+    <tableColumn id="15" name="Abfall" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>1-Table36[maxTRpm]/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Nm1000" dataDxfId="27" dataCellStyle="Percent">
+    <tableColumn id="20" name="max kW" dataDxfId="2" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table36[maxPS]/1.36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" name="rated kW" dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table36[PS]/1.36</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" name="g/kWh" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>Table36[fuelRatedRate]*1.1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" name="Nm1000" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="NmEco" dataDxfId="26">
+    <tableColumn id="8" name="NmEco" dataDxfId="17">
       <calculatedColumnFormula>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Nm2Eco" dataDxfId="25">
+    <tableColumn id="9" name="Nm2Eco" dataDxfId="16">
       <calculatedColumnFormula>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="f2Eco" dataDxfId="24">
+    <tableColumn id="12" name="f2Eco" dataDxfId="15">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="f3Eco" dataDxfId="23">
+    <tableColumn id="10" name="f3Eco" dataDxfId="14">
       <calculatedColumnFormula>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="f4Eco" dataDxfId="22">
+    <tableColumn id="11" name="f4Eco" dataDxfId="13">
       <calculatedColumnFormula>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="idleT" dataDxfId="21">
+    <tableColumn id="13" name="idleT" dataDxfId="12">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="idleTEco" dataDxfId="20">
+    <tableColumn id="19" name="idleTEco" dataDxfId="11">
       <calculatedColumnFormula>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="xmlComment" dataDxfId="19">
+    <tableColumn id="21" name="xmlComment" dataDxfId="10">
       <calculatedColumnFormula>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6999,17 +7096,17 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$A$22*Table1[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="18">
+    <tableColumn id="6" name="kw_pto" dataDxfId="9">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="17">
+    <tableColumn id="3" name="ps" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor"/>
-    <tableColumn id="5" name="xml" dataDxfId="16">
+    <tableColumn id="5" name="xml" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table1[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table1[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="xml2" dataDxfId="15">
+    <tableColumn id="8" name="xml2" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE("&lt;torque normRpm=""",ROUND(Table1[[#This Row],[rpm]]/Table3[ratedRpm],3),""" torque=""",ROUND(Table1[[#This Row],[motor]]/MAX(Table1[motor]),3),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7043,16 +7140,16 @@
     <tableColumn id="2" name="pto">
       <calculatedColumnFormula>$I$2*Table13[[#This Row],[rawData]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="kw_pto" dataDxfId="14">
+    <tableColumn id="6" name="kw_pto" dataDxfId="5">
       <calculatedColumnFormula>A2*C2/9550</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="ps" dataDxfId="13">
+    <tableColumn id="3" name="ps" dataDxfId="4">
       <calculatedColumnFormula>Table13[[#This Row],[kw_pto]]*1.36/0.94</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="motor">
       <calculatedColumnFormula>C2/0.94</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="xml" dataDxfId="12">
+    <tableColumn id="5" name="xml" dataDxfId="3">
       <calculatedColumnFormula>CONCATENATE("&lt;torque rpm=""",Table13[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table13[[#This Row],[motor]],0),"""/&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7326,7 +7423,7 @@
   <dimension ref="A1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7420,78 +7517,78 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
-        <v>1900</v>
-      </c>
-      <c r="B2" s="14">
-        <v>250</v>
-      </c>
-      <c r="C2" s="18">
+      <c r="A2" s="12">
+        <v>2100</v>
+      </c>
+      <c r="B2" s="13">
+        <v>98</v>
+      </c>
+      <c r="C2" s="17">
         <f>Table36[maxPsEcoRate]*Table36[maxPS]</f>
-        <v>250</v>
+        <v>98</v>
       </c>
       <c r="D2" s="7">
-        <v>2100</v>
+        <v>2300</v>
       </c>
       <c r="E2" s="8">
-        <v>240</v>
-      </c>
-      <c r="F2" s="19">
+        <v>95</v>
+      </c>
+      <c r="F2" s="18">
         <f>Table36[PS]*Table36[PSEcoRate]</f>
-        <v>240</v>
-      </c>
-      <c r="G2" s="13">
-        <v>1500</v>
-      </c>
-      <c r="H2" s="14">
-        <v>1500</v>
-      </c>
-      <c r="I2" s="14">
-        <v>1100</v>
-      </c>
-      <c r="J2" s="18">
+        <v>95</v>
+      </c>
+      <c r="G2" s="12">
+        <v>1600</v>
+      </c>
+      <c r="H2" s="13">
+        <v>1600</v>
+      </c>
+      <c r="I2" s="13">
+        <v>366</v>
+      </c>
+      <c r="J2" s="17">
         <f>Table36[NmEcoRate]*Table36[maxT]</f>
-        <v>1100</v>
-      </c>
-      <c r="K2" s="7">
+        <v>366</v>
+      </c>
+      <c r="K2" s="30">
         <v>900</v>
       </c>
-      <c r="L2" s="11">
-        <v>0.9</v>
-      </c>
-      <c r="M2" s="9">
+      <c r="L2" s="31">
+        <v>0.83</v>
+      </c>
+      <c r="M2" s="32">
         <v>220</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <v>0.5</v>
       </c>
-      <c r="O2" s="14">
-        <v>2</v>
-      </c>
-      <c r="P2" s="14">
+      <c r="O2" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P2" s="13">
         <v>0.94</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="14">
         <v>1</v>
       </c>
-      <c r="R2" s="31">
-        <v>207</v>
-      </c>
-      <c r="S2" s="16">
+      <c r="R2" s="29">
+        <v>215</v>
+      </c>
+      <c r="S2" s="15">
         <f>Table36[fuelMinRate]/0.9</f>
-        <v>230</v>
-      </c>
-      <c r="T2" s="17">
+        <v>238.88888888888889</v>
+      </c>
+      <c r="T2" s="16">
         <f>ROUND(MIN(0.6*Table36[idleRpm]+0.4*Table36[ratedRpm],0.5*Table36[maxTRpm1]+0.5*Table36[maxTRpm]),-1)</f>
-        <v>1380</v>
-      </c>
-      <c r="U2" s="19">
+        <v>1460</v>
+      </c>
+      <c r="U2" s="18">
         <f>0.94*Table36[fuelRatedRate]</f>
-        <v>216.2</v>
-      </c>
-      <c r="V2" s="16">
+        <v>224.55555555555554</v>
+      </c>
+      <c r="V2" s="15">
         <f>ROUND(Table36[ratedRpm]+0.49*Table36[fadeOut],-2)</f>
-        <v>2200</v>
+        <v>2400</v>
       </c>
       <c r="W2" s="7">
         <v>1</v>
@@ -7499,149 +7596,170 @@
       <c r="X2" s="9">
         <v>1</v>
       </c>
-      <c r="Y2" s="29">
+      <c r="Y2" s="27">
         <f>Table36[PSEcoRate]* (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]) + Table36[NmEcoRate]* (1- (Table36[maxPRpm]-Table36[maxTRpm])/(Table36[ratedRpm]-Table36[maxTRpm]))</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="O3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="P3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="Q3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="R3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="S3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="T3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="U3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="V3" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <f>(1-Table36[idleRatio])/((Table36[maxTRpm1]-Table36[idleRpm])^2)</f>
-        <v>2.7777777777777771E-7</v>
-      </c>
-      <c r="B4" s="12">
+        <v>3.4693877551020417E-7</v>
+      </c>
+      <c r="B4" s="11">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>4.0010202645651574E-4</v>
-      </c>
-      <c r="C4" s="12">
+        <v>2.0931104682310087E-4</v>
+      </c>
+      <c r="C4" s="11">
         <f>(Table36[maxT]-Table7[Nm])/Table36[maxT]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.0002550661412894E-6</v>
-      </c>
-      <c r="D4" s="12">
+        <v>4.1862209364620175E-7</v>
+      </c>
+      <c r="D4" s="11">
         <f>(Table36[maxPS]-Table36[PS])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>2.5000000000000001E-4</v>
-      </c>
-      <c r="E4" s="12">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="E4" s="11">
         <f>Table36[maxPS]/1.36*9550/Table36[maxPRpm]</f>
-        <v>923.95510835913308</v>
-      </c>
-      <c r="F4" s="12">
+        <v>327.69607843137254</v>
+      </c>
+      <c r="F4" s="11">
         <f>Table36[PS]/1.36*9550/Table36[ratedRpm]</f>
-        <v>802.52100840336129</v>
-      </c>
-      <c r="G4" s="23">
+        <v>290.04156010230173</v>
+      </c>
+      <c r="G4" s="22">
         <f>Table7[Nm1000]/Table7[Nm2Eco]</f>
-        <v>1.2754944735311229</v>
-      </c>
-      <c r="H4" s="24">
+        <v>1.1042808721129678</v>
+      </c>
+      <c r="H4" s="23">
         <f>Table36[maxTEco]/Table7[Nm2Eco]-1</f>
-        <v>0.37068062827225146</v>
-      </c>
-      <c r="I4" s="24">
+        <v>0.26188812344998658</v>
+      </c>
+      <c r="I4" s="23">
         <f>Table36[maxT]/Table7[Nm2]-1</f>
-        <v>0.37068062827225146</v>
-      </c>
-      <c r="J4" s="25">
+        <v>0.26188812344998658</v>
+      </c>
+      <c r="J4" s="23">
         <f>1-Table36[maxTRpm]/Table36[ratedRpm]</f>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="K4" s="12">
+        <v>0.30434782608695654</v>
+      </c>
+      <c r="K4" s="33">
+        <f>Table36[maxPS]/1.36</f>
+        <v>72.058823529411754</v>
+      </c>
+      <c r="L4" s="34">
+        <f>Table36[PS]/1.36</f>
+        <v>69.85294117647058</v>
+      </c>
+      <c r="M4" s="35">
+        <f>Table36[fuelRatedRate]*1.1</f>
+        <v>262.77777777777777</v>
+      </c>
+      <c r="N4" s="11">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-1000)^2)*Table36[maxTEco]</f>
-        <v>1023.6111111111111</v>
-      </c>
-      <c r="L4" s="12">
+        <v>320.2873469387755</v>
+      </c>
+      <c r="O4" s="11">
         <f>Table36[maxPSEco]/1.36*9550/Table36[maxPRpm]</f>
-        <v>923.95510835913308</v>
-      </c>
-      <c r="M4" s="12">
+        <v>327.69607843137254</v>
+      </c>
+      <c r="P4" s="11">
         <f>Table36[PSEco]/1.36*9550/Table36[ratedRpm]</f>
-        <v>802.52100840336129</v>
-      </c>
-      <c r="N4" s="12">
+        <v>290.04156010230173</v>
+      </c>
+      <c r="Q4" s="11">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])</f>
-        <v>4.0010202645651574E-4</v>
-      </c>
-      <c r="O4" s="12">
+        <v>2.0931104682310087E-4</v>
+      </c>
+      <c r="R4" s="11">
         <f>(Table36[maxTEco]-Table7[NmEco])/Table36[maxTEco]/(Table36[maxPRpm]-Table36[maxTRpm])^2</f>
-        <v>1.0002550661412894E-6</v>
-      </c>
-      <c r="P4" s="12">
+        <v>4.1862209364620175E-7</v>
+      </c>
+      <c r="S4" s="11">
         <f>(Table36[maxPSEco]-Table36[PSEco])/MAX(1,Table36[ratedRpm]-Table36[maxPRpm])^2</f>
-        <v>2.5000000000000001E-4</v>
-      </c>
-      <c r="Q4" s="12">
+        <v>7.4999999999999993E-5</v>
+      </c>
+      <c r="T4" s="11">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxT]</f>
-        <v>990</v>
-      </c>
-      <c r="R4" s="12">
+        <v>303.77999999999997</v>
+      </c>
+      <c r="U4" s="11">
         <f>(1-Table7[f1]*(Table36[maxTRpm1]-Table36[idleRpm])^2)*Table36[maxTEco]</f>
-        <v>990</v>
-      </c>
-      <c r="S4" s="12" t="str">
+        <v>303.77999999999997</v>
+      </c>
+      <c r="V4" s="11" t="str">
         <f>CONCATENATE("        &lt;!-- ",Table36[maxPRpm],": ",Table36[maxPS],"(",ROUND(Table36[maxPSEco],0),") | ",Table36[ratedRpm],": ",Table36[PS],"(",ROUND(Table36[PSEco],0),") | ",Table36[maxTRpm1],"..",Table36[maxTRpm],": ",Table36[maxT],"(",ROUND(Table36[maxTEco],0),") | ",Table36[idleRatio]*100," | ",Table36[linearDown]," | ",Table36[fadeOut]," | ",Table36[fadeOutExp]," | ",Table36[normRpm]," | ",Table36[fuelMinRpm],": ",Table36[fuelMinRate]," --&gt;")</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 2100: 98(98) | 2300: 95(95) | 1600..1600: 366(366) | 83 | 0.5 | 220 | 2.3 | 2400 | 1460: 215 --&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" s="4" customFormat="1" ht="62.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -7717,12 +7835,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -7731,25 +7849,25 @@
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
         <v>0</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
         <v>0</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>283.04374999999993</v>
+        <v>279.95096371882079</v>
       </c>
       <c r="K7" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 2100: 98(98) | 2300: 95(95) | 1600..1600: 366(366) | 83 | 0.5 | 220 | 2.3 | 2400 | 1460: 215 --&gt;</v>
       </c>
       <c r="L7" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;!-- 1900: 250(250) | 2100: 240(240) | 1500..1500: 1100(1100) | 90 | 0.5 | 220 | 2 | 2200 | 1380: 207 --&gt;</v>
+        <v xml:space="preserve">        &lt;!-- 2100: 98(98) | 2300: 95(95) | 1600..1600: 366(366) | 83 | 0.5 | 220 | 2.3 | 2400 | 1460: 215 --&gt;</v>
       </c>
       <c r="M7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -7757,11 +7875,11 @@
       </c>
       <c r="N7" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>412.50000000000011</v>
+        <v>40.932244897959109</v>
       </c>
       <c r="O7" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>192.26852747677987</v>
+        <v>231.17019607843136</v>
       </c>
       <c r="P7" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7769,7 +7887,7 @@
       </c>
       <c r="Q7" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R7" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -7777,11 +7895,11 @@
       </c>
       <c r="S7" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>412.50000000000011</v>
+        <v>40.932244897959109</v>
       </c>
       <c r="T7" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>192.26852747677987</v>
+        <v>231.17019607843136</v>
       </c>
       <c r="U7" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7789,7 +7907,7 @@
       </c>
       <c r="V7" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -7798,53 +7916,53 @@
       </c>
       <c r="B8" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>240.37037037037044</v>
-      </c>
-      <c r="C8" s="21"/>
+        <v>65.594032081968592</v>
+      </c>
+      <c r="C8" s="20"/>
       <c r="D8" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>240.37037037037044</v>
-      </c>
-      <c r="E8" s="21"/>
+        <v>65.594032081968592</v>
+      </c>
+      <c r="E8" s="20"/>
       <c r="F8" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>240.37037037037044</v>
+        <v>65.594032081968592</v>
       </c>
       <c r="G8" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>240.37037037037044</v>
-      </c>
-      <c r="H8" s="30">
+        <v>65.594032081968592</v>
+      </c>
+      <c r="H8" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>3.4230754314523959</v>
-      </c>
-      <c r="I8" s="30">
+        <v>0.93411396472751085</v>
+      </c>
+      <c r="I8" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>3.4230754314523959</v>
-      </c>
-      <c r="J8" s="30">
+        <v>0.93411396472751085</v>
+      </c>
+      <c r="J8" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>272.4222222222221</v>
+        <v>271.35827664399085</v>
       </c>
       <c r="K8" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="240" fuelUsageRatio="272.4"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="100" motorTorque="66" fuelUsageRatio="271.4"/&gt;</v>
       </c>
       <c r="L8" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.045" torque="0.219"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.042" torque="0.179"/&gt;</v>
       </c>
       <c r="M8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>207.77777777777783</v>
+        <v>63.756296296296306</v>
       </c>
       <c r="N8" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>501.11111111111131</v>
+        <v>80.295918367346886</v>
       </c>
       <c r="O8" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>329.80359907120709</v>
+        <v>251.0882352941176</v>
       </c>
       <c r="P8" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7852,19 +7970,19 @@
       </c>
       <c r="Q8" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R8" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>207.77777777777783</v>
+        <v>63.756296296296306</v>
       </c>
       <c r="S8" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>501.11111111111131</v>
+        <v>80.295918367346886</v>
       </c>
       <c r="T8" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>329.80359907120709</v>
+        <v>251.0882352941176</v>
       </c>
       <c r="U8" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7872,7 +7990,7 @@
       </c>
       <c r="V8" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -7881,53 +7999,53 @@
       </c>
       <c r="B9" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>704.81481481481478</v>
-      </c>
-      <c r="C9" s="21"/>
+        <v>198.07791719156796</v>
+      </c>
+      <c r="C9" s="20"/>
       <c r="D9" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>704.81481481481478</v>
-      </c>
-      <c r="E9" s="21"/>
+        <v>198.07791719156796</v>
+      </c>
+      <c r="E9" s="20"/>
       <c r="F9" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>704.81481481481478</v>
+        <v>198.07791719156796</v>
       </c>
       <c r="G9" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>704.81481481481478</v>
-      </c>
-      <c r="H9" s="30">
+        <v>198.07791719156796</v>
+      </c>
+      <c r="H9" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>40.148613535000962</v>
-      </c>
-      <c r="I9" s="30">
+        <v>11.283181879812876</v>
+      </c>
+      <c r="I9" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>40.148613535000962</v>
-      </c>
-      <c r="J9" s="30">
+        <v>11.283181879812876</v>
+      </c>
+      <c r="J9" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>245.3493055555555</v>
+        <v>249.23667800453509</v>
       </c>
       <c r="K9" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="705" fuelUsageRatio="245.3"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="400" motorTorque="198" fuelUsageRatio="249.2"/&gt;</v>
       </c>
       <c r="L9" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.182" torque="0.641"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.167" torque="0.541"/&gt;</v>
       </c>
       <c r="M9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>684.44444444444446</v>
+        <v>210.02074074074071</v>
       </c>
       <c r="N9" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>730.27777777777783</v>
+        <v>183.149387755102</v>
       </c>
       <c r="O9" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>676.39197948916387</v>
+        <v>301.64941176470586</v>
       </c>
       <c r="P9" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7935,19 +8053,19 @@
       </c>
       <c r="Q9" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R9" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>684.44444444444446</v>
+        <v>210.02074074074071</v>
       </c>
       <c r="S9" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>730.27777777777783</v>
+        <v>183.149387755102</v>
       </c>
       <c r="T9" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>676.39197948916387</v>
+        <v>301.64941176470586</v>
       </c>
       <c r="U9" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -7955,7 +8073,7 @@
       </c>
       <c r="V9" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -7964,53 +8082,53 @@
       </c>
       <c r="B10" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>912.59259259259272</v>
-      </c>
-      <c r="C10" s="21"/>
+        <v>268.84252792475007</v>
+      </c>
+      <c r="C10" s="20"/>
       <c r="D10" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>912.59259259259272</v>
-      </c>
-      <c r="E10" s="21"/>
+        <v>268.84252792475007</v>
+      </c>
+      <c r="E10" s="20"/>
       <c r="F10" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>912.59259259259272</v>
+        <v>268.84252792475007</v>
       </c>
       <c r="G10" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>912.59259259259272</v>
-      </c>
-      <c r="H10" s="30">
+        <v>268.84252792475007</v>
+      </c>
+      <c r="H10" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>90.972580957921295</v>
-      </c>
-      <c r="I10" s="30">
+        <v>26.799799642341583</v>
+      </c>
+      <c r="I10" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>90.972580957921295</v>
-      </c>
-      <c r="J10" s="30">
+        <v>26.799799642341583</v>
+      </c>
+      <c r="J10" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>225.46388888888887</v>
+        <v>232.59977324263036</v>
       </c>
       <c r="K10" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="913" fuelUsageRatio="225.5"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="700" motorTorque="269" fuelUsageRatio="232.6"/&gt;</v>
       </c>
       <c r="L10" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.318" torque="0.83"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.292" torque="0.735"/&gt;</v>
       </c>
       <c r="M10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>941.11111111111109</v>
+        <v>288.77851851851847</v>
       </c>
       <c r="N10" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>904.44444444444457</v>
+        <v>263.14653061224482</v>
       </c>
       <c r="O10" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>923.95510835913308</v>
+        <v>338.42117647058819</v>
       </c>
       <c r="P10" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8018,19 +8136,19 @@
       </c>
       <c r="Q10" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R10" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>941.11111111111109</v>
+        <v>288.77851851851847</v>
       </c>
       <c r="S10" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>904.44444444444457</v>
+        <v>263.14653061224482</v>
       </c>
       <c r="T10" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>923.95510835913308</v>
+        <v>338.42117647058819</v>
       </c>
       <c r="U10" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8038,7 +8156,7 @@
       </c>
       <c r="V10" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -8047,53 +8165,53 @@
       </c>
       <c r="B11" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>953.33333333333337</v>
-      </c>
-      <c r="C11" s="21"/>
+        <v>286.43267993617201</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>953.33333333333337</v>
-      </c>
-      <c r="E11" s="21"/>
+        <v>286.43267993617201</v>
+      </c>
+      <c r="E11" s="20"/>
       <c r="F11" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>953.33333333333337</v>
+        <v>286.43267993617201</v>
       </c>
       <c r="G11" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>953.33333333333337</v>
-      </c>
-      <c r="H11" s="30">
+        <v>286.43267993617201</v>
+      </c>
+      <c r="H11" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>108.61012216404887</v>
-      </c>
-      <c r="I11" s="30">
+        <v>32.632330447178546</v>
+      </c>
+      <c r="I11" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>108.61012216404887</v>
-      </c>
-      <c r="J11" s="30">
+        <v>32.632330447178546</v>
+      </c>
+      <c r="J11" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>220.43263888888887</v>
+        <v>228.27295918367346</v>
       </c>
       <c r="K11" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="953" fuelUsageRatio="220.4"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="800" motorTorque="286" fuelUsageRatio="228.3"/&gt;</v>
       </c>
       <c r="L11" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.364" torque="0.867"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.333" torque="0.783"/&gt;</v>
       </c>
       <c r="M11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>977.77777777777771</v>
+        <v>300.0296296296296</v>
       </c>
       <c r="N11" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>950.27777777777783</v>
+        <v>284.7330612244898</v>
       </c>
       <c r="O11" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>984.47053986068101</v>
+        <v>347.61411764705883</v>
       </c>
       <c r="P11" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8101,19 +8219,19 @@
       </c>
       <c r="Q11" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R11" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>977.77777777777771</v>
+        <v>300.0296296296296</v>
       </c>
       <c r="S11" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>950.27777777777783</v>
+        <v>284.7330612244898</v>
       </c>
       <c r="T11" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>984.47053986068101</v>
+        <v>347.61411764705883</v>
       </c>
       <c r="U11" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8121,7 +8239,7 @@
       </c>
       <c r="V11" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -8130,53 +8248,53 @@
       </c>
       <c r="B12" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>990</v>
-      </c>
-      <c r="C12" s="21"/>
+        <v>303.77999999999997</v>
+      </c>
+      <c r="C12" s="20"/>
       <c r="D12" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>990</v>
-      </c>
-      <c r="E12" s="21"/>
+        <v>303.77999999999997</v>
+      </c>
+      <c r="E12" s="20"/>
       <c r="F12" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>990</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="G12" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>990</v>
-      </c>
-      <c r="H12" s="30">
+        <v>303.77999999999997</v>
+      </c>
+      <c r="H12" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>126.88586387434555</v>
-      </c>
-      <c r="I12" s="30">
+        <v>38.934735078534025</v>
+      </c>
+      <c r="I12" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>126.88586387434555</v>
-      </c>
-      <c r="J12" s="30">
+        <v>38.934735078534025</v>
+      </c>
+      <c r="J12" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>216.2</v>
+        <v>224.55555555555554</v>
       </c>
       <c r="K12" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="990" fuelUsageRatio="216.2"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="900" motorTorque="304" fuelUsageRatio="224.6"/&gt;</v>
       </c>
       <c r="L12" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.409" torque="0.9"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.375" torque="0.83"/&gt;</v>
       </c>
       <c r="M12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>990</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="N12" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>990</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="O12" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1033.9831656346751</v>
+        <v>355.27490196078435</v>
       </c>
       <c r="P12" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8184,19 +8302,19 @@
       </c>
       <c r="Q12" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R12" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>990</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="S12" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>990</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="T12" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1033.9831656346751</v>
+        <v>355.27490196078435</v>
       </c>
       <c r="U12" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -8204,7 +8322,7 @@
       </c>
       <c r="V12" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -8213,81 +8331,81 @@
       </c>
       <c r="B13" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1023.6111111111111</v>
-      </c>
-      <c r="C13" s="21"/>
+        <v>320.2873469387755</v>
+      </c>
+      <c r="C13" s="20"/>
       <c r="D13" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1023.6111111111111</v>
-      </c>
-      <c r="E13" s="21"/>
+        <v>320.2873469387755</v>
+      </c>
+      <c r="E13" s="20"/>
       <c r="F13" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1023.6111111111111</v>
+        <v>320.2873469387755</v>
       </c>
       <c r="G13" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1023.6111111111111</v>
-      </c>
-      <c r="H13" s="30">
+        <v>320.2873469387755</v>
+      </c>
+      <c r="H13" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>145.77079697498544</v>
-      </c>
-      <c r="I13" s="30">
+        <v>45.61160123944866</v>
+      </c>
+      <c r="I13" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>145.77079697498544</v>
-      </c>
-      <c r="J13" s="30">
+        <v>45.61160123944866</v>
+      </c>
+      <c r="J13" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>212.76597222222222</v>
+        <v>221.44756235827663</v>
       </c>
       <c r="K13" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="1024" fuelUsageRatio="212.8"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1000" motorTorque="320" fuelUsageRatio="221.4"/&gt;</v>
       </c>
       <c r="L13" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.455" torque="0.931"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.417" torque="0.875"/&gt;</v>
       </c>
       <c r="M13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>977.77777777777771</v>
+        <v>300.0296296296296</v>
       </c>
       <c r="N13" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1023.6111111111111</v>
+        <v>320.2873469387755</v>
       </c>
       <c r="O13" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1072.4929856811145</v>
+        <v>361.40352941176468</v>
       </c>
       <c r="P13" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>333.54779411764702</v>
+        <v>50.909926470588331</v>
       </c>
       <c r="Q13" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R13" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>977.77777777777771</v>
+        <v>300.0296296296296</v>
       </c>
       <c r="S13" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1023.6111111111111</v>
+        <v>320.2873469387755</v>
       </c>
       <c r="T13" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1072.4929856811145</v>
+        <v>361.40352941176468</v>
       </c>
       <c r="U13" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>333.54779411764702</v>
+        <v>50.909926470588331</v>
       </c>
       <c r="V13" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -8296,81 +8414,81 @@
       </c>
       <c r="B14" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1051.1111111111111</v>
-      </c>
-      <c r="C14" s="21"/>
+        <v>334.25510204081633</v>
+      </c>
+      <c r="C14" s="20"/>
       <c r="D14" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1051.1111111111111</v>
-      </c>
-      <c r="E14" s="21"/>
+        <v>334.25510204081633</v>
+      </c>
+      <c r="E14" s="20"/>
       <c r="F14" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1051.1111111111111</v>
+        <v>334.25510204081633</v>
       </c>
       <c r="G14" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1051.1111111111111</v>
-      </c>
-      <c r="H14" s="30">
+        <v>334.25510204081633</v>
+      </c>
+      <c r="H14" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>164.65573007562537</v>
-      </c>
-      <c r="I14" s="30">
+        <v>52.360799230687043</v>
+      </c>
+      <c r="I14" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>164.65573007562537</v>
-      </c>
-      <c r="J14" s="30">
+        <v>52.360799230687043</v>
+      </c>
+      <c r="J14" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>210.13055555555556</v>
+        <v>218.94897959183672</v>
       </c>
       <c r="K14" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="1051" fuelUsageRatio="210.1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1100" motorTorque="334" fuelUsageRatio="218.9"/&gt;</v>
       </c>
       <c r="L14" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="0.956"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.458" torque="0.913"/&gt;</v>
       </c>
       <c r="M14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>941.11111111111109</v>
+        <v>288.77851851851847</v>
       </c>
       <c r="N14" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1051.1111111111111</v>
+        <v>334.25510204081633</v>
       </c>
       <c r="O14" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1100</v>
+        <v>366</v>
       </c>
       <c r="P14" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>574.5320855614973</v>
+        <v>146.82486631016042</v>
       </c>
       <c r="Q14" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R14" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>941.11111111111109</v>
+        <v>288.77851851851847</v>
       </c>
       <c r="S14" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1051.1111111111111</v>
+        <v>334.25510204081633</v>
       </c>
       <c r="T14" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1100</v>
+        <v>366</v>
       </c>
       <c r="U14" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>574.5320855614973</v>
+        <v>146.82486631016042</v>
       </c>
       <c r="V14" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -8379,81 +8497,81 @@
       </c>
       <c r="B15" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1072.5</v>
-      </c>
-      <c r="C15" s="21"/>
+        <v>345.68326530612245</v>
+      </c>
+      <c r="C15" s="20"/>
       <c r="D15" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1072.5</v>
-      </c>
-      <c r="E15" s="21"/>
+        <v>345.68326530612245</v>
+      </c>
+      <c r="E15" s="20"/>
       <c r="F15" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1072.5</v>
+        <v>345.68326530612245</v>
       </c>
       <c r="G15" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1072.5</v>
-      </c>
-      <c r="H15" s="30">
+        <v>345.68326530612245</v>
+      </c>
+      <c r="H15" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>183.27958115183247</v>
-      </c>
-      <c r="I15" s="30">
+        <v>59.073831306763559</v>
+      </c>
+      <c r="I15" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>183.27958115183247</v>
-      </c>
-      <c r="J15" s="30">
+        <v>59.073831306763559</v>
+      </c>
+      <c r="J15" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>208.29374999999999</v>
+        <v>217.05980725623581</v>
       </c>
       <c r="K15" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="1073" fuelUsageRatio="208.3"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1200" motorTorque="346" fuelUsageRatio="217.1"/&gt;</v>
       </c>
       <c r="L15" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.545" torque="0.975"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.5" torque="0.944"/&gt;</v>
       </c>
       <c r="M15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>880.00000000000011</v>
+        <v>270.02666666666664</v>
       </c>
       <c r="N15" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1072.5</v>
+        <v>345.68326530612245</v>
       </c>
       <c r="O15" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1116.5042085913312</v>
+        <v>369.06431372549019</v>
       </c>
       <c r="P15" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>746.09375</v>
+        <v>217.97640931372553</v>
       </c>
       <c r="Q15" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R15" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>880.00000000000011</v>
+        <v>270.02666666666664</v>
       </c>
       <c r="S15" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1072.5</v>
+        <v>345.68326530612245</v>
       </c>
       <c r="T15" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1116.5042085913312</v>
+        <v>369.06431372549019</v>
       </c>
       <c r="U15" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>746.09375</v>
+        <v>217.97640931372553</v>
       </c>
       <c r="V15" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -8462,81 +8580,81 @@
       </c>
       <c r="B16" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1087.7777777777778</v>
-      </c>
-      <c r="C16" s="21"/>
+        <v>354.57183673469387</v>
+      </c>
+      <c r="C16" s="20"/>
       <c r="D16" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1087.7777777777778</v>
-      </c>
-      <c r="E16" s="21"/>
+        <v>354.57183673469387</v>
+      </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1087.7777777777778</v>
+        <v>354.57183673469387</v>
       </c>
       <c r="G16" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1087.7777777777778</v>
-      </c>
-      <c r="H16" s="30">
+        <v>354.57183673469387</v>
+      </c>
+      <c r="H16" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>201.38126817917399</v>
-      </c>
-      <c r="I16" s="30">
+        <v>65.642199722192544</v>
+      </c>
+      <c r="I16" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>201.38126817917399</v>
-      </c>
-      <c r="J16" s="30">
+        <v>65.642199722192544</v>
+      </c>
+      <c r="J16" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.25555555555556</v>
+        <v>215.78004535147392</v>
       </c>
       <c r="K16" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="1088" fuelUsageRatio="207.3"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1300" motorTorque="355" fuelUsageRatio="215.8"/&gt;</v>
       </c>
       <c r="L16" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.591" torque="0.989"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.542" torque="0.969"/&gt;</v>
       </c>
       <c r="M16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>794.44444444444446</v>
+        <v>243.77407407407406</v>
       </c>
       <c r="N16" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1087.7777777777778</v>
+        <v>354.57183673469387</v>
       </c>
       <c r="O16" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1122.0056114551082</v>
+        <v>370.59647058823532</v>
       </c>
       <c r="P16" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>864.25339366515834</v>
+        <v>270.07918552036199</v>
       </c>
       <c r="Q16" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R16" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>794.44444444444446</v>
+        <v>243.77407407407406</v>
       </c>
       <c r="S16" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1087.7777777777778</v>
+        <v>354.57183673469387</v>
       </c>
       <c r="T16" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1122.0056114551082</v>
+        <v>370.59647058823532</v>
       </c>
       <c r="U16" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>864.25339366515834</v>
+        <v>270.07918552036199</v>
       </c>
       <c r="V16" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -8545,81 +8663,81 @@
       </c>
       <c r="B17" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1096.9444444444443</v>
-      </c>
-      <c r="C17" s="21"/>
+        <v>360.9208163265306</v>
+      </c>
+      <c r="C17" s="20"/>
       <c r="D17" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1096.9444444444443</v>
-      </c>
-      <c r="E17" s="21"/>
+        <v>360.9208163265306</v>
+      </c>
+      <c r="E17" s="20"/>
       <c r="F17" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1096.9444444444443</v>
+        <v>360.9208163265306</v>
       </c>
       <c r="G17" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1096.9444444444443</v>
-      </c>
-      <c r="H17" s="30">
+        <v>360.9208163265306</v>
+      </c>
+      <c r="H17" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>218.699709133217</v>
-      </c>
-      <c r="I17" s="30">
+        <v>71.957406731488419</v>
+      </c>
+      <c r="I17" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>218.699709133217</v>
-      </c>
-      <c r="J17" s="30">
+        <v>71.957406731488419</v>
+      </c>
+      <c r="J17" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.01774691358025</v>
+        <v>215.10969387755102</v>
       </c>
       <c r="K17" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="1097" fuelUsageRatio="207"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1400" motorTorque="361" fuelUsageRatio="215.1"/&gt;</v>
       </c>
       <c r="L17" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.636" torque="0.997"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.583" torque="0.986"/&gt;</v>
       </c>
       <c r="M17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>684.44444444444446</v>
+        <v>210.02074074074071</v>
       </c>
       <c r="N17" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1096.9444444444443</v>
+        <v>360.9208163265306</v>
       </c>
       <c r="O17" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1116.5042085913312</v>
+        <v>370.59647058823532</v>
       </c>
       <c r="P17" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>940.45430672268901</v>
+        <v>307.21507352941177</v>
       </c>
       <c r="Q17" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R17" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>684.44444444444446</v>
+        <v>210.02074074074071</v>
       </c>
       <c r="S17" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1096.9444444444443</v>
+        <v>360.9208163265306</v>
       </c>
       <c r="T17" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1116.5042085913312</v>
+        <v>370.59647058823532</v>
       </c>
       <c r="U17" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>940.45430672268901</v>
+        <v>307.21507352941177</v>
       </c>
       <c r="V17" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
@@ -8628,81 +8746,81 @@
       </c>
       <c r="B18" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1100</v>
-      </c>
-      <c r="C18" s="21"/>
+        <v>364.73020408163262</v>
+      </c>
+      <c r="C18" s="20"/>
       <c r="D18" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1100</v>
-      </c>
-      <c r="E18" s="21"/>
+        <v>364.73020408163262</v>
+      </c>
+      <c r="E18" s="20"/>
       <c r="F18" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1100</v>
+        <v>364.73020408163262</v>
       </c>
       <c r="G18" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1100</v>
-      </c>
-      <c r="H18" s="30">
+        <v>364.73020408163262</v>
+      </c>
+      <c r="H18" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>234.97382198952886</v>
-      </c>
-      <c r="I18" s="30">
+        <v>77.910954589165499</v>
+      </c>
+      <c r="I18" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>234.97382198952886</v>
-      </c>
-      <c r="J18" s="30">
+        <v>77.910954589165499</v>
+      </c>
+      <c r="J18" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>207.63888888888889</v>
+        <v>215.05416981607459</v>
       </c>
       <c r="K18" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="1100" fuelUsageRatio="207.6"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1500" motorTorque="365" fuelUsageRatio="215.1"/&gt;</v>
       </c>
       <c r="L18" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.682" torque="1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.625" torque="0.997"/&gt;</v>
       </c>
       <c r="M18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>549.99999999999989</v>
+        <v>168.76666666666662</v>
       </c>
       <c r="N18" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1100</v>
+        <v>364.73020408163262</v>
       </c>
       <c r="O18" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1100</v>
+        <v>369.06431372549019</v>
       </c>
       <c r="P18" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>983.08823529411757</v>
+        <v>332.37745098039215</v>
       </c>
       <c r="Q18" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R18" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>549.99999999999989</v>
+        <v>168.76666666666662</v>
       </c>
       <c r="S18" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1100</v>
+        <v>364.73020408163262</v>
       </c>
       <c r="T18" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1100</v>
+        <v>369.06431372549019</v>
       </c>
       <c r="U18" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>983.08823529411757</v>
+        <v>332.37745098039215</v>
       </c>
       <c r="V18" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
@@ -8711,81 +8829,81 @@
       </c>
       <c r="B19" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1072.4929856811145</v>
-      </c>
-      <c r="C19" s="21"/>
+        <v>366</v>
+      </c>
+      <c r="C19" s="20"/>
       <c r="D19" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1072.4929856811145</v>
-      </c>
-      <c r="E19" s="21"/>
+        <v>366</v>
+      </c>
+      <c r="E19" s="20"/>
       <c r="F19" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1072.4929856811145</v>
+        <v>366</v>
       </c>
       <c r="G19" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1072.4929856811145</v>
-      </c>
-      <c r="H19" s="30">
+        <v>366</v>
+      </c>
+      <c r="H19" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>244.37117663268117</v>
-      </c>
-      <c r="I19" s="30">
+        <v>83.394345549738219</v>
+      </c>
+      <c r="I19" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>244.37117663268117</v>
-      </c>
-      <c r="J19" s="30">
+        <v>83.394345549738219</v>
+      </c>
+      <c r="J19" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>209.14737654320987</v>
+        <v>215.66358024691357</v>
       </c>
       <c r="K19" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="1072" fuelUsageRatio="209.1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1600" motorTorque="366" fuelUsageRatio="215.7"/&gt;</v>
       </c>
       <c r="L19" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.727" torque="0.975"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.667" torque="1"/&gt;</v>
       </c>
       <c r="M19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>391.11111111111131</v>
+        <v>120.0118518518519</v>
       </c>
       <c r="N19" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1096.9444444444443</v>
+        <v>366</v>
       </c>
       <c r="O19" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1072.4929856811145</v>
+        <v>366</v>
       </c>
       <c r="P19" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>998.44898897058829</v>
+        <v>347.8113511029411</v>
       </c>
       <c r="Q19" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R19" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>391.11111111111131</v>
+        <v>120.0118518518519</v>
       </c>
       <c r="S19" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1096.9444444444443</v>
+        <v>366</v>
       </c>
       <c r="T19" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1072.4929856811145</v>
+        <v>366</v>
       </c>
       <c r="U19" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>998.44898897058829</v>
+        <v>347.8113511029411</v>
       </c>
       <c r="V19" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -8794,81 +8912,81 @@
       </c>
       <c r="B20" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>1032.6557093425604</v>
-      </c>
-      <c r="C20" s="21"/>
+        <v>361.40352941176468</v>
+      </c>
+      <c r="C20" s="20"/>
       <c r="D20" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>1032.6557093425604</v>
-      </c>
-      <c r="E20" s="21"/>
+        <v>361.40352941176468</v>
+      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>1032.6557093425604</v>
+        <v>361.40352941176468</v>
       </c>
       <c r="G20" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>1032.6557093425604</v>
-      </c>
-      <c r="H20" s="30">
+        <v>361.40352941176468</v>
+      </c>
+      <c r="H20" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>249.99999999999994</v>
-      </c>
-      <c r="I20" s="30">
+        <v>87.493713089005226</v>
+      </c>
+      <c r="I20" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>249.99999999999994</v>
-      </c>
-      <c r="J20" s="30">
+        <v>87.493713089005226</v>
+      </c>
+      <c r="J20" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>211.54320987654322</v>
+        <v>216.95011337868482</v>
       </c>
       <c r="K20" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="1033" fuelUsageRatio="211.5"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1700" motorTorque="361" fuelUsageRatio="217"/&gt;</v>
       </c>
       <c r="L20" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.773" torque="0.939"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.708" torque="0.987"/&gt;</v>
       </c>
       <c r="M20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>207.77777777777783</v>
+        <v>63.756296296296306</v>
       </c>
       <c r="N20" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1087.7777777777778</v>
+        <v>364.73020408163262</v>
       </c>
       <c r="O20" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>1033.9831656346748</v>
+        <v>361.40352941176468</v>
       </c>
       <c r="P20" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>991.34948096885807</v>
+        <v>355.23356401384075</v>
       </c>
       <c r="Q20" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R20" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>207.77777777777783</v>
+        <v>63.756296296296306</v>
       </c>
       <c r="S20" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1087.7777777777778</v>
+        <v>364.73020408163262</v>
       </c>
       <c r="T20" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>1033.9831656346748</v>
+        <v>361.40352941176468</v>
       </c>
       <c r="U20" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>991.34948096885807</v>
+        <v>355.23356401384075</v>
       </c>
       <c r="V20" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -8877,41 +8995,41 @@
       </c>
       <c r="B21" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>975.28594771241819</v>
-      </c>
-      <c r="C21" s="21"/>
+        <v>355.27490196078435</v>
+      </c>
+      <c r="C21" s="20"/>
       <c r="D21" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>975.28594771241819</v>
-      </c>
-      <c r="E21" s="21"/>
+        <v>355.27490196078435</v>
+      </c>
+      <c r="E21" s="20"/>
       <c r="F21" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>975.28594771241819</v>
+        <v>355.27490196078435</v>
       </c>
       <c r="G21" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>975.28594771241819</v>
-      </c>
-      <c r="H21" s="30">
+        <v>355.27490196078435</v>
+      </c>
+      <c r="H21" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>249.99999999999994</v>
-      </c>
-      <c r="I21" s="30">
+        <v>91.069419895287965</v>
+      </c>
+      <c r="I21" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>249.99999999999994</v>
-      </c>
-      <c r="J21" s="30">
+        <v>91.069419895287965</v>
+      </c>
+      <c r="J21" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>214.82638888888889</v>
+        <v>218.91376921138826</v>
       </c>
       <c r="K21" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="975" fuelUsageRatio="214.8"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1800" motorTorque="355" fuelUsageRatio="218.9"/&gt;</v>
       </c>
       <c r="L21" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.818" torque="0.887"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.75" torque="0.971"/&gt;</v>
       </c>
       <c r="M21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
@@ -8919,19 +9037,19 @@
       </c>
       <c r="N21" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1072.5</v>
+        <v>360.9208163265306</v>
       </c>
       <c r="O21" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>984.47053986068101</v>
+        <v>355.27490196078435</v>
       </c>
       <c r="P21" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>965.53308823529403</v>
+        <v>355.97937091503269</v>
       </c>
       <c r="Q21" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R21" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
@@ -8939,19 +9057,19 @@
       </c>
       <c r="S21" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1072.5</v>
+        <v>360.9208163265306</v>
       </c>
       <c r="T21" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>984.47053986068101</v>
+        <v>355.27490196078435</v>
       </c>
       <c r="U21" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>965.53308823529403</v>
+        <v>355.97937091503269</v>
       </c>
       <c r="V21" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -8960,81 +9078,81 @@
       </c>
       <c r="B22" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>923.95510835913308</v>
-      </c>
-      <c r="C22" s="21"/>
+        <v>347.61411764705883</v>
+      </c>
+      <c r="C22" s="20"/>
       <c r="D22" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>923.95510835913308</v>
-      </c>
-      <c r="E22" s="21"/>
+        <v>347.61411764705883</v>
+      </c>
+      <c r="E22" s="20"/>
       <c r="F22" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>923.95510835913308</v>
+        <v>347.61411764705883</v>
       </c>
       <c r="G22" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>923.95510835913308</v>
-      </c>
-      <c r="H22" s="30">
+        <v>347.61411764705883</v>
+      </c>
+      <c r="H22" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>250</v>
-      </c>
-      <c r="I22" s="30">
+        <v>94.056008376963348</v>
+      </c>
+      <c r="I22" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>250</v>
-      </c>
-      <c r="J22" s="30">
+        <v>94.056008376963348</v>
+      </c>
+      <c r="J22" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>218.99691358024691</v>
+        <v>221.55454774502394</v>
       </c>
       <c r="K22" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="924" fuelUsageRatio="219"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="1900" motorTorque="348" fuelUsageRatio="221.6"/&gt;</v>
       </c>
       <c r="L22" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.864" torque="0.84"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.792" torque="0.95"/&gt;</v>
       </c>
       <c r="M22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-232.22222222222237</v>
+        <v>-71.25703703703708</v>
       </c>
       <c r="N22" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1051.1111111111111</v>
+        <v>354.57183673469387</v>
       </c>
       <c r="O22" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>923.95510835913308</v>
+        <v>347.61411764705883</v>
       </c>
       <c r="P22" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>923.95510835913308</v>
+        <v>351.10294117647049</v>
       </c>
       <c r="Q22" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R22" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-232.22222222222237</v>
+        <v>-71.25703703703708</v>
       </c>
       <c r="S22" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1051.1111111111111</v>
+        <v>354.57183673469387</v>
       </c>
       <c r="T22" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>923.95510835913308</v>
+        <v>347.61411764705883</v>
       </c>
       <c r="U22" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>923.95510835913308</v>
+        <v>351.10294117647049</v>
       </c>
       <c r="V22" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -9043,81 +9161,81 @@
       </c>
       <c r="B23" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>868.97977941176464</v>
-      </c>
-      <c r="C23" s="21"/>
+        <v>338.42117647058825</v>
+      </c>
+      <c r="C23" s="20"/>
       <c r="D23" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>868.97977941176464</v>
-      </c>
-      <c r="E23" s="21"/>
+        <v>338.42117647058825</v>
+      </c>
+      <c r="E23" s="20"/>
       <c r="F23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>868.97977941176464</v>
+        <v>338.42117647058825</v>
       </c>
       <c r="G23" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>868.97977941176464</v>
-      </c>
-      <c r="H23" s="30">
+        <v>338.42117647058825</v>
+      </c>
+      <c r="H23" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>247.5</v>
-      </c>
-      <c r="I23" s="30">
+        <v>96.388020942408389</v>
+      </c>
+      <c r="I23" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>247.5</v>
-      </c>
-      <c r="J23" s="30">
+        <v>96.388020942408389</v>
+      </c>
+      <c r="J23" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>224.05478395061729</v>
+        <v>224.87244897959184</v>
       </c>
       <c r="K23" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="869" fuelUsageRatio="224.1"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2000" motorTorque="338" fuelUsageRatio="224.9"/&gt;</v>
       </c>
       <c r="L23" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.909" torque="0.79"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.833" torque="0.925"/&gt;</v>
       </c>
       <c r="M23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-488.88888888888908</v>
+        <v>-150.01481481481486</v>
       </c>
       <c r="N23" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>1023.6111111111111</v>
+        <v>345.68326530612245</v>
       </c>
       <c r="O23" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>852.4368711300308</v>
+        <v>338.42117647058825</v>
       </c>
       <c r="P23" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>868.97977941176464</v>
+        <v>341.44761029411757</v>
       </c>
       <c r="Q23" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R23" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-488.88888888888908</v>
+        <v>-150.01481481481486</v>
       </c>
       <c r="S23" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>1023.6111111111111</v>
+        <v>345.68326530612245</v>
       </c>
       <c r="T23" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>852.4368711300308</v>
+        <v>338.42117647058825</v>
       </c>
       <c r="U23" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>868.97977941176464</v>
+        <v>341.44761029411757</v>
       </c>
       <c r="V23" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -9126,81 +9244,81 @@
       </c>
       <c r="B24" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>802.52100840336129</v>
-      </c>
-      <c r="C24" s="21"/>
+        <v>327.69607843137254</v>
+      </c>
+      <c r="C24" s="20"/>
       <c r="D24" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>802.52100840336129</v>
-      </c>
-      <c r="E24" s="21"/>
+        <v>327.69607843137254</v>
+      </c>
+      <c r="E24" s="20"/>
       <c r="F24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>802.52100840336129</v>
+        <v>327.69607843137254</v>
       </c>
       <c r="G24" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>802.52100840336129</v>
-      </c>
-      <c r="H24" s="30">
+        <v>327.69607843137254</v>
+      </c>
+      <c r="H24" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>240</v>
-      </c>
-      <c r="I24" s="30">
+        <v>98</v>
+      </c>
+      <c r="I24" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>240</v>
-      </c>
-      <c r="J24" s="30">
+        <v>98</v>
+      </c>
+      <c r="J24" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>230</v>
+        <v>228.86747291509195</v>
       </c>
       <c r="K24" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="803" fuelUsageRatio="230"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2100" motorTorque="328" fuelUsageRatio="228.9"/&gt;</v>
       </c>
       <c r="L24" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="0.955" torque="0.73"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.875" torque="0.895"/&gt;</v>
       </c>
       <c r="M24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-770.00000000000034</v>
+        <v>-236.27333333333343</v>
       </c>
       <c r="N24" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>990</v>
+        <v>334.25510204081633</v>
       </c>
       <c r="O24" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>769.91582817337451</v>
+        <v>327.69607843137254</v>
       </c>
       <c r="P24" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>802.52100840336129</v>
+        <v>327.69607843137254</v>
       </c>
       <c r="Q24" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R24" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-770.00000000000034</v>
+        <v>-236.27333333333343</v>
       </c>
       <c r="S24" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>990</v>
+        <v>334.25510204081633</v>
       </c>
       <c r="T24" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>769.91582817337451</v>
+        <v>327.69607843137254</v>
       </c>
       <c r="U24" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>802.52100840336129</v>
+        <v>327.69607843137254</v>
       </c>
       <c r="V24" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>802.52100840336129</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -9209,81 +9327,81 @@
       </c>
       <c r="B25" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>636.71088270018754</v>
-      </c>
-      <c r="C25" s="21"/>
+        <v>310.4069184491978</v>
+      </c>
+      <c r="C25" s="20"/>
       <c r="D25" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>636.71088270018754</v>
-      </c>
-      <c r="E25" s="21"/>
+        <v>310.4069184491978</v>
+      </c>
+      <c r="E25" s="20"/>
       <c r="F25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>636.71088270018754</v>
+        <v>310.4069184491978</v>
       </c>
       <c r="G25" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>636.71088270018754</v>
-      </c>
-      <c r="H25" s="30">
+        <v>310.4069184491978</v>
+      </c>
+      <c r="H25" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>199.48051948051949</v>
-      </c>
-      <c r="I25" s="30">
+        <v>97.249999999999986</v>
+      </c>
+      <c r="I25" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>199.48051948051949</v>
-      </c>
-      <c r="J25" s="30">
+        <v>97.249999999999986</v>
+      </c>
+      <c r="J25" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>262.03842321622847</v>
+        <v>233.53961955152431</v>
       </c>
       <c r="K25" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="637" fuelUsageRatio="262"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2200" motorTorque="310" fuelUsageRatio="233.5"/&gt;</v>
       </c>
       <c r="L25" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.579"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque normRpm="0.917" torque="0.848"/&gt;</v>
       </c>
       <c r="M25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-1075.5555555555559</v>
+        <v>-330.03259259259266</v>
       </c>
       <c r="N25" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>950.27777777777783</v>
+        <v>320.2873469387755</v>
       </c>
       <c r="O25" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>676.39197948916399</v>
+        <v>315.43882352941176</v>
       </c>
       <c r="P25" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>726.14471925133694</v>
+        <v>310.4069184491978</v>
       </c>
       <c r="Q25" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>636.71088270018754</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R25" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1075.5555555555559</v>
+        <v>-330.03259259259266</v>
       </c>
       <c r="S25" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>950.27777777777783</v>
+        <v>320.2873469387755</v>
       </c>
       <c r="T25" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>676.39197948916399</v>
+        <v>315.43882352941176</v>
       </c>
       <c r="U25" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>726.14471925133694</v>
+        <v>310.4069184491978</v>
       </c>
       <c r="V25" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>636.71088270018754</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
@@ -9292,81 +9410,81 @@
       </c>
       <c r="B26" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>139.28050559066608</v>
-      </c>
-      <c r="C26" s="21"/>
+        <v>290.04156010230173</v>
+      </c>
+      <c r="C26" s="20"/>
       <c r="D26" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>139.28050559066608</v>
-      </c>
-      <c r="E26" s="21"/>
+        <v>290.04156010230173</v>
+      </c>
+      <c r="E26" s="20"/>
       <c r="F26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>139.28050559066608</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="G26" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>139.28050559066608</v>
-      </c>
-      <c r="H26" s="30">
+        <v>290.04156010230173</v>
+      </c>
+      <c r="H26" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>45.619834710743824</v>
-      </c>
-      <c r="I26" s="30">
+        <v>94.999999999999972</v>
+      </c>
+      <c r="I26" s="28">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>45.619834710743824</v>
-      </c>
-      <c r="J26" s="30">
+        <v>94.999999999999972</v>
+      </c>
+      <c r="J26" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>411.23669051775721</v>
+        <v>238.88888888888889</v>
       </c>
       <c r="K26" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="139" fuelUsageRatio="411.2"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2300" motorTorque="290" fuelUsageRatio="238.9"/&gt;</v>
       </c>
       <c r="L26" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v/>
+        <v xml:space="preserve">        &lt;torque normRpm="0.958" torque="0.792"/&gt;</v>
       </c>
       <c r="M26" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-1405.5555555555547</v>
+        <v>-431.29259259259231</v>
       </c>
       <c r="N26" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>904.44444444444457</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="O26" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>571.86532507739912</v>
+        <v>301.64941176470586</v>
       </c>
       <c r="P26" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>641.1445012787724</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="Q26" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>139.28050559066608</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="R26" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1405.5555555555547</v>
+        <v>-431.29259259259231</v>
       </c>
       <c r="S26" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>904.44444444444457</v>
+        <v>303.77999999999997</v>
       </c>
       <c r="T26" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>571.86532507739912</v>
+        <v>301.64941176470586</v>
       </c>
       <c r="U26" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>641.1445012787724</v>
+        <v>290.04156010230173</v>
       </c>
       <c r="V26" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>139.28050559066608</v>
+        <v>290.04156010230173</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -9375,81 +9493,81 @@
       </c>
       <c r="B27" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="21"/>
+        <v>242.73862745517255</v>
+      </c>
+      <c r="C27" s="20"/>
       <c r="D27" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="21"/>
+        <v>242.73862745517255</v>
+      </c>
+      <c r="E27" s="20"/>
       <c r="F27" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>242.73862745517255</v>
       </c>
       <c r="G27" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>0</v>
+        <v>242.73862745517255</v>
       </c>
       <c r="H27" s="3">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>0</v>
+        <v>82.963233509286212</v>
       </c>
       <c r="I27" s="3">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="30">
+        <v>82.963233509286212</v>
+      </c>
+      <c r="J27" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>272.16551203617928</v>
       </c>
       <c r="K27" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="0" fuelUsageRatio="460"/&gt;</v>
+        <v xml:space="preserve">        &lt;torque rpm="2400" motorTorque="243" fuelUsageRatio="272.2"/&gt;</v>
       </c>
       <c r="L27" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
-        <v/>
+        <v xml:space="preserve">        &lt;torque normRpm="1" torque="0.663"/&gt;</v>
       </c>
       <c r="M27" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-1759.9999999999995</v>
+        <v>-540.05333333333317</v>
       </c>
       <c r="N27" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>852.5</v>
+        <v>284.7330612244898</v>
       </c>
       <c r="O27" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>456.33586493808031</v>
+        <v>286.32784313725489</v>
       </c>
       <c r="P27" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>548.59834558823525</v>
+        <v>266.98452818627447</v>
       </c>
       <c r="Q27" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>242.73862745517255</v>
       </c>
       <c r="R27" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-1759.9999999999995</v>
+        <v>-540.05333333333317</v>
       </c>
       <c r="S27" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>852.5</v>
+        <v>284.7330612244898</v>
       </c>
       <c r="T27" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>456.33586493808031</v>
+        <v>286.32784313725489</v>
       </c>
       <c r="U27" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>548.59834558823525</v>
+        <v>266.98452818627447</v>
       </c>
       <c r="V27" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>242.73862745517255</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -9458,37 +9576,37 @@
       </c>
       <c r="B28" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="21"/>
+        <v>57.094595048925981</v>
+      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="21"/>
+        <v>57.094595048925981</v>
+      </c>
+      <c r="E28" s="20"/>
       <c r="F28" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
-        <v>0</v>
+        <v>57.094595048925981</v>
       </c>
       <c r="G28" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manDataEco]]&gt;0,Table15[[#This Row],[manDataEco]],Table15[[#This Row],[rawDataEco]])</f>
-        <v>0</v>
+        <v>57.094595048925981</v>
       </c>
       <c r="H28" s="3">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motor]]/9550</f>
-        <v>0</v>
+        <v>20.326871535743283</v>
       </c>
       <c r="I28" s="3">
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="30">
+        <v>20.326871535743283</v>
+      </c>
+      <c r="J28" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>427.12989594839519</v>
       </c>
       <c r="K28" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
-        <v/>
+        <v xml:space="preserve">        &lt;torque rpm="2500" motorTorque="57" fuelUsageRatio="427.1"/&gt;</v>
       </c>
       <c r="L28" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[normRpm],"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque normRpm=""",ROUND(Table15[[#This Row],[rpm]]/Table36[normRpm],3),""" torque=""",ROUND(Table15[[#This Row],[motor]]/MAX(Table15[motor]),3),"""/&gt;")))</f>
@@ -9496,43 +9614,43 @@
       </c>
       <c r="M28" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-2138.8888888888887</v>
+        <v>-656.31481481481467</v>
       </c>
       <c r="N28" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>794.44444444444457</v>
+        <v>263.14653061224482</v>
       </c>
       <c r="O28" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>329.80359907120709</v>
+        <v>269.47411764705879</v>
       </c>
       <c r="P28" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>449.41176470588232</v>
+        <v>241.55882352941171</v>
       </c>
       <c r="Q28" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>57.094595048925981</v>
       </c>
       <c r="R28" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-2138.8888888888887</v>
+        <v>-656.31481481481467</v>
       </c>
       <c r="S28" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>794.44444444444457</v>
+        <v>263.14653061224482</v>
       </c>
       <c r="T28" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>329.80359907120709</v>
+        <v>269.47411764705879</v>
       </c>
       <c r="U28" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>449.41176470588232</v>
+        <v>241.55882352941171</v>
       </c>
       <c r="V28" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
-        <v>0</v>
+        <v>57.094595048925981</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
@@ -9543,12 +9661,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C29" s="21"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9565,9 +9683,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J29" s="30">
+      <c r="J29" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K29" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9579,19 +9697,19 @@
       </c>
       <c r="M29" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-3193.0555555555547</v>
+        <v>-979.78425925925887</v>
       </c>
       <c r="N29" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>622.56944444444457</v>
+        <v>198.06948979591834</v>
       </c>
       <c r="O29" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>0</v>
+        <v>220.63661764705878</v>
       </c>
       <c r="P29" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>177.14739304812832</v>
+        <v>169.32737299465239</v>
       </c>
       <c r="Q29" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9599,19 +9717,19 @@
       </c>
       <c r="R29" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-3193.0555555555547</v>
+        <v>-979.78425925925887</v>
       </c>
       <c r="S29" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>622.56944444444457</v>
+        <v>198.06948979591834</v>
       </c>
       <c r="T29" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>220.63661764705878</v>
       </c>
       <c r="U29" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>177.14739304812832</v>
+        <v>169.32737299465239</v>
       </c>
       <c r="V29" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9626,12 +9744,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9648,9 +9766,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J30" s="30">
+      <c r="J30" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K30" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9662,19 +9780,19 @@
       </c>
       <c r="M30" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-4400.0000000000009</v>
+        <v>-1350.1333333333334</v>
       </c>
       <c r="N30" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>412.50000000000011</v>
+        <v>117.11999999999995</v>
       </c>
       <c r="O30" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>0</v>
+        <v>162.2231372549019</v>
       </c>
       <c r="P30" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>87.190563725490208</v>
       </c>
       <c r="Q30" s="3">
         <f>MAX(0,Table7[Nm2]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9682,19 +9800,19 @@
       </c>
       <c r="R30" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-4400.0000000000009</v>
+        <v>-1350.1333333333334</v>
       </c>
       <c r="S30" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>412.50000000000011</v>
+        <v>117.11999999999995</v>
       </c>
       <c r="T30" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>162.2231372549019</v>
       </c>
       <c r="U30" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
-        <v>0</v>
+        <v>87.190563725490208</v>
       </c>
       <c r="V30" s="3">
         <f>MAX(0,Table7[Nm2Eco]*MIN(Table36[ratedRpm]/MAX(1,Table15[[#This Row],[rpm]]),1-(MAX(0,Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^Table36[fadeOutExp]))</f>
@@ -9709,12 +9827,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C31" s="21"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E31" s="21"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9731,9 +9849,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J31" s="30">
+      <c r="J31" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K31" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9745,15 +9863,15 @@
       </c>
       <c r="M31" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-5759.7222222222217</v>
+        <v>-1767.3620370370368</v>
       </c>
       <c r="N31" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
-        <v>164.23611111111137</v>
+        <v>20.298061224489704</v>
       </c>
       <c r="O31" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>0</v>
+        <v>94.233676470588179</v>
       </c>
       <c r="P31" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -9765,15 +9883,15 @@
       </c>
       <c r="R31" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-5759.7222222222217</v>
+        <v>-1767.3620370370368</v>
       </c>
       <c r="S31" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
-        <v>164.23611111111137</v>
+        <v>20.298061224489704</v>
       </c>
       <c r="T31" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>94.233676470588179</v>
       </c>
       <c r="U31" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -9792,12 +9910,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9814,9 +9932,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J32" s="30">
+      <c r="J32" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K32" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9828,7 +9946,7 @@
       </c>
       <c r="M32" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-7272.2222222222217</v>
+        <v>-2231.4703703703699</v>
       </c>
       <c r="N32" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -9836,7 +9954,7 @@
       </c>
       <c r="O32" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxT])</f>
-        <v>0</v>
+        <v>16.668235294117558</v>
       </c>
       <c r="P32" s="3">
         <f>MAX(0,(Table36[maxPS]-Table7[f4]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -9848,7 +9966,7 @@
       </c>
       <c r="R32" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-7272.2222222222217</v>
+        <v>-2231.4703703703699</v>
       </c>
       <c r="S32" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -9856,7 +9974,7 @@
       </c>
       <c r="T32" s="3">
         <f>MAX(0,(Table36[linearDown]*(1-Table7[f2Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm]))+(1-Table36[linearDown])*(1-Table7[f3Eco]*(Table15[[#This Row],[rpm]]-Table36[maxTRpm])^2))*Table36[maxTEco])</f>
-        <v>0</v>
+        <v>16.668235294117558</v>
       </c>
       <c r="U32" s="3">
         <f>MAX(0,(Table36[maxPSEco]-Table7[f4Eco]*(Table15[[#This Row],[rpm]]-Table36[maxPRpm])^2)/1.36*9550/MAX(1,Table15[[#This Row],[rpm]]))</f>
@@ -9875,12 +9993,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C33" s="21"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9897,9 +10015,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J33" s="30">
+      <c r="J33" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K33" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9911,7 +10029,7 @@
       </c>
       <c r="M33" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-8937.5000000000018</v>
+        <v>-2742.4583333333339</v>
       </c>
       <c r="N33" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -9931,7 +10049,7 @@
       </c>
       <c r="R33" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-8937.5000000000018</v>
+        <v>-2742.4583333333339</v>
       </c>
       <c r="S33" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -9958,12 +10076,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C34" s="21"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -9980,9 +10098,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J34" s="30">
+      <c r="J34" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K34" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -9994,7 +10112,7 @@
       </c>
       <c r="M34" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-10755.555555555558</v>
+        <v>-3300.3259259259262</v>
       </c>
       <c r="N34" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10014,7 +10132,7 @@
       </c>
       <c r="R34" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-10755.555555555558</v>
+        <v>-3300.3259259259262</v>
       </c>
       <c r="S34" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10041,12 +10159,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10063,9 +10181,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J35" s="30">
+      <c r="J35" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K35" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10077,7 +10195,7 @@
       </c>
       <c r="M35" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-12726.388888888889</v>
+        <v>-3905.073148148148</v>
       </c>
       <c r="N35" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10097,7 +10215,7 @@
       </c>
       <c r="R35" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-12726.388888888889</v>
+        <v>-3905.073148148148</v>
       </c>
       <c r="S35" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10124,12 +10242,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E36" s="21"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10146,9 +10264,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J36" s="30">
+      <c r="J36" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K36" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10160,7 +10278,7 @@
       </c>
       <c r="M36" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-14850</v>
+        <v>-4556.7</v>
       </c>
       <c r="N36" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10180,7 +10298,7 @@
       </c>
       <c r="R36" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-14850</v>
+        <v>-4556.7</v>
       </c>
       <c r="S36" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10207,12 +10325,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10229,9 +10347,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J37" s="30">
+      <c r="J37" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K37" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10243,7 +10361,7 @@
       </c>
       <c r="M37" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-17126.388888888891</v>
+        <v>-5255.2064814814812</v>
       </c>
       <c r="N37" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10263,7 +10381,7 @@
       </c>
       <c r="R37" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-17126.388888888891</v>
+        <v>-5255.2064814814812</v>
       </c>
       <c r="S37" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10290,12 +10408,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C38" s="21"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10312,9 +10430,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J38" s="30">
+      <c r="J38" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K38" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10326,7 +10444,7 @@
       </c>
       <c r="M38" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-19555.555555555555</v>
+        <v>-6000.5925925925922</v>
       </c>
       <c r="N38" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10346,7 +10464,7 @@
       </c>
       <c r="R38" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-19555.555555555555</v>
+        <v>-6000.5925925925922</v>
       </c>
       <c r="S38" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10373,12 +10491,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E39" s="21"/>
+      <c r="E39" s="20"/>
       <c r="F39" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10395,9 +10513,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J39" s="30">
+      <c r="J39" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K39" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10409,7 +10527,7 @@
       </c>
       <c r="M39" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-22137.499999999996</v>
+        <v>-6792.8583333333318</v>
       </c>
       <c r="N39" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10429,7 +10547,7 @@
       </c>
       <c r="R39" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-22137.499999999996</v>
+        <v>-6792.8583333333318</v>
       </c>
       <c r="S39" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10456,12 +10574,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C40" s="21"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E40" s="21"/>
+      <c r="E40" s="20"/>
       <c r="F40" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10478,9 +10596,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J40" s="30">
+      <c r="J40" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K40" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10492,7 +10610,7 @@
       </c>
       <c r="M40" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-24872.222222222219</v>
+        <v>-7632.0037037037018</v>
       </c>
       <c r="N40" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10512,7 +10630,7 @@
       </c>
       <c r="R40" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-24872.222222222219</v>
+        <v>-7632.0037037037018</v>
       </c>
       <c r="S40" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10539,12 +10657,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C41" s="21"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E41" s="21"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10561,9 +10679,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J41" s="30">
+      <c r="J41" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K41" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10575,7 +10693,7 @@
       </c>
       <c r="M41" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-27759.722222222226</v>
+        <v>-8518.0287037037033</v>
       </c>
       <c r="N41" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10595,7 +10713,7 @@
       </c>
       <c r="R41" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-27759.722222222226</v>
+        <v>-8518.0287037037033</v>
       </c>
       <c r="S41" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>
@@ -10622,12 +10740,12 @@
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[Nm]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5]],Table15[[#This Row],[t4]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3]],Table36[maxT]))))))</f>
         <v>0</v>
       </c>
-      <c r="C42" s="22"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="3">
         <f>MIN(IF(Table15[[#This Row],[rpm]]&gt;0,Table7[NmEco]*Table36[maxPRpm]/Table15[[#This Row],[rpm]],0),MAX(0,IF(Table15[[#This Row],[rpm]]&lt;Table36[idleRpm],(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])*Table15[[#This Row],[t1E]]+Table15[[#This Row],[rpm]]/Table36[idleRpm]*Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;=Table36[maxPRpm],IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm],Table15[[#This Row],[t5E]],Table15[[#This Row],[t4E]]),IF(Table15[[#This Row],[rpm]]&lt;Table36[maxTRpm1],Table15[[#This Row],[t2E]],IF(Table15[[#This Row],[rpm]]&gt;Table36[maxTRpm],Table15[[#This Row],[t3E]],Table36[maxTEco]))))))</f>
         <v>0</v>
       </c>
-      <c r="E42" s="22"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="3">
         <f>Table36[Factor]*IF(Table15[[#This Row],[manualData]]&gt;0,Table15[[#This Row],[manualData]],Table15[[#This Row],[rawData]])</f>
         <v>0</v>
@@ -10644,9 +10762,9 @@
         <f>1.36*Table15[[#This Row],[rpm]]*Table15[[#This Row],[motorEco]]/9550</f>
         <v>0</v>
       </c>
-      <c r="J42" s="30">
+      <c r="J42" s="28">
         <f>IF(Table15[[#This Row],[rpm]]&lt;=Table36[fuelMinRpm],Table36[fuelMinRate]+(Table36[fuelIdleRate]-Table36[fuelMinRate])*((Table36[fuelMinRpm]-Table15[[#This Row],[rpm]])/(Table36[fuelMinRpm]-Table36[idleRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm],Table36[fuelMinRate]+(Table36[fuelRatedRate]-Table36[fuelMinRate])*((Table15[[#This Row],[rpm]]-Table36[fuelMinRpm])/(Table36[ratedRpm]-Table36[fuelMinRpm]))^2,IF(Table15[[#This Row],[rpm]]&lt;=Table36[ratedRpm]+Table36[fadeOut],Table36[fuelRatedRate]+Table36[fuelRatedRate]*((Table15[[#This Row],[rpm]]-Table36[ratedRpm])/Table36[fadeOut])^2.5,Table36[fuelRatedRate]*2)))</f>
-        <v>460</v>
+        <v>477.77777777777777</v>
       </c>
       <c r="K42" s="10" t="str">
         <f>IF(Table15[[#This Row],[rpm]]&gt;Table36[ratedRpm]+Table36[fadeOut]+99,"",IF(Table15[[#This Row],[rpm]]&lt;1,Table7[xmlComment],CONCATENATE("        &lt;torque rpm=""",Table15[[#This Row],[rpm]],""" motorTorque=""",ROUND(Table15[[#This Row],[motor]],0),"""",IF( Table15[[#This Row],[motorEco]] &lt; Table15[[#This Row],[motor]],CONCATENATE(" motorTorqueEco=""",ROUND(Table15[[#This Row],[motorEco]],0),""""),"")," fuelUsageRatio=""",ROUND(Table15[[#This Row],[fuelUsageRatio]],1),"""/&gt;",CONCATENATE(IF(Table15[[#This Row],[manualData]]&gt;0,CONCATENATE("&lt;!-- manualData: ",Table15[[#This Row],[manualData]],"--&gt;"),""),IF(Table15[[#This Row],[manDataEco]]&gt;0,CONCATENATE("&lt;!-- manDataEco: ",Table15[[#This Row],[manDataEco]],"--&gt;"),"")))))</f>
@@ -10658,7 +10776,7 @@
       </c>
       <c r="M42" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleT]</f>
-        <v>-30800.000000000004</v>
+        <v>-9450.9333333333343</v>
       </c>
       <c r="N42" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxT])</f>
@@ -10678,7 +10796,7 @@
       </c>
       <c r="R42" s="3">
         <f>(1-(1-Table15[[#This Row],[rpm]]/Table36[idleRpm])^2)*Table7[idleTEco]</f>
-        <v>-30800.000000000004</v>
+        <v>-9450.9333333333343</v>
       </c>
       <c r="S42" s="3">
         <f>MAX(0,(1-Table7[f1]*(Table36[maxTRpm1]-Table15[[#This Row],[rpm]])^2)*Table36[maxTEco])</f>

</xml_diff>